<commit_message>
Auto commit on 2025/06/03 週二 16:53:22.52
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$13</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$20</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="127">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-02  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="180">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-03  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -357,6 +357,52 @@
     <t>2025-06-02 15:30:00</t>
   </si>
   <si>
+    <t>ED649114060201</t>
+  </si>
+  <si>
+    <t>D649</t>
+  </si>
+  <si>
+    <t>北縣中陽店</t>
+  </si>
+  <si>
+    <t>2025-06-02 15:12:15</t>
+  </si>
+  <si>
+    <t>星期一</t>
+  </si>
+  <si>
+    <t>HL23</t>
+  </si>
+  <si>
+    <t>HL-TM主機</t>
+  </si>
+  <si>
+    <t>收銀員顯示器畫面不正常</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應tm2(TCX800)收銀及客顯畫面接觸控不良，需點選很多次才有反應，查看校正程式少一個螢幕無法執行處控校正，重啟tm仍異常..請台芝到店協助(前後屏幕觸恐不良)
+</t>
+  </si>
+  <si>
+    <t>THILF0D649</t>
+  </si>
+  <si>
+    <t>2025-06-02 15:28:17</t>
+  </si>
+  <si>
+    <t>2025-06-03 10:39:00</t>
+  </si>
+  <si>
+    <t>2025-06-03 11:09:00</t>
+  </si>
+  <si>
+    <t>2025-06-03 19:28:00</t>
+  </si>
+  <si>
+    <t>螢幕校正程式檢查正常，重新做一次螢幕對應後客顯可正常觸控</t>
+  </si>
+  <si>
     <t>板橋藝文店</t>
   </si>
   <si>
@@ -415,6 +461,122 @@
   </si>
   <si>
     <t>2025-06-02 16:00:00</t>
+  </si>
+  <si>
+    <t>E4698114060201</t>
+  </si>
+  <si>
+    <t>三重頂崁店</t>
+  </si>
+  <si>
+    <t>2025-06-02 19:13:30</t>
+  </si>
+  <si>
+    <t>夜間</t>
+  </si>
+  <si>
+    <t>HLD3</t>
+  </si>
+  <si>
+    <t>HL-熱感發票機</t>
+  </si>
+  <si>
+    <t>D301</t>
+  </si>
+  <si>
+    <t>發票切刀卡紙，切紙不正常</t>
+  </si>
+  <si>
+    <t>門市反應TM1熱感發票機(BSC10)取出掉落的1塊錢後一直有異音，當下發票、收據列印皆正常，已重啟發票機並重新安裝新紙捲+簡易清潔後仍有出現異常聲音，需請台芝到店協助檢查(怪聲)</t>
+  </si>
+  <si>
+    <t>THILF04698</t>
+  </si>
+  <si>
+    <t>2025-06-02 20:02:59</t>
+  </si>
+  <si>
+    <t>2025-06-03 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-03 15:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-04 00:03:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換下8155000350
+換上8155005421</t>
+  </si>
+  <si>
+    <t>新莊福慧店</t>
+  </si>
+  <si>
+    <t>THILF04552</t>
+  </si>
+  <si>
+    <t>2025-06-03 11:52:48</t>
+  </si>
+  <si>
+    <t>2025-06-03 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-03 12:00:00</t>
+  </si>
+  <si>
+    <t>淡水英才店</t>
+  </si>
+  <si>
+    <t>新北市淡水區</t>
+  </si>
+  <si>
+    <t>THILF04658</t>
+  </si>
+  <si>
+    <t>2025-06-03 13:36:55</t>
+  </si>
+  <si>
+    <t>2025-06-03 13:21:00</t>
+  </si>
+  <si>
+    <t>2025-06-03 13:36:00</t>
+  </si>
+  <si>
+    <t>北縣西雲店</t>
+  </si>
+  <si>
+    <t>新北市五股區</t>
+  </si>
+  <si>
+    <t>THILF03770</t>
+  </si>
+  <si>
+    <t>2025-06-03 14:51:04</t>
+  </si>
+  <si>
+    <t>2025-06-03 14:10:00</t>
+  </si>
+  <si>
+    <t>2025-06-03 14:50:00</t>
+  </si>
+  <si>
+    <t>2025-06-03 15:44:03</t>
+  </si>
+  <si>
+    <t>2025-06-03 15:43:00</t>
+  </si>
+  <si>
+    <t>北縣五泰店</t>
+  </si>
+  <si>
+    <t>THILF02325</t>
+  </si>
+  <si>
+    <t>2025-06-03 15:44:44</t>
+  </si>
+  <si>
+    <t>2025-06-03 15:50:00</t>
   </si>
 </sst>
 </file>
@@ -828,10 +990,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK13"/>
+  <dimension ref="A1:AK20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="AC17" sqref="AC17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1659,38 +1821,58 @@
         <v>8</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C10" s="3">
-        <v>2025060144</v>
-      </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3">
-        <v>4983</v>
+        <v>2025060136</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>108</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K10" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L10" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M10" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="N10" s="3">
+        <v>2303</v>
+      </c>
+      <c r="O10" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="P10" s="10" t="s">
+        <v>115</v>
+      </c>
       <c r="Q10" s="3" t="s">
-        <v>109</v>
+        <v>116</v>
       </c>
       <c r="R10" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S10" s="3" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="T10" s="3">
         <v>1</v>
@@ -1699,36 +1881,34 @@
         <v>53</v>
       </c>
       <c r="V10" s="3" t="s">
-        <v>111</v>
+        <v>117</v>
       </c>
       <c r="W10" s="3" t="s">
-        <v>112</v>
+        <v>118</v>
       </c>
       <c r="X10" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="Y10" s="3"/>
+        <v>119</v>
+      </c>
+      <c r="Y10" s="3" t="s">
+        <v>120</v>
+      </c>
       <c r="Z10" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC10" s="10" t="s">
-        <v>114</v>
-      </c>
-      <c r="AD10" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>121</v>
+      </c>
+      <c r="AD10" s="3"/>
       <c r="AE10" s="3"/>
       <c r="AF10" s="3"/>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
       <c r="AI10" s="3"/>
-      <c r="AJ10" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ10" s="3"/>
       <c r="AK10" s="3" t="s">
         <v>60</v>
       </c>
@@ -1741,18 +1921,18 @@
         <v>94</v>
       </c>
       <c r="C11" s="7">
-        <v>2025060172</v>
+        <v>2025060144</v>
       </c>
       <c r="D11" s="7"/>
       <c r="E11" s="7"/>
       <c r="F11" s="7">
-        <v>2890</v>
+        <v>4983</v>
       </c>
       <c r="G11" s="7" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="I11" s="7"/>
       <c r="J11" s="7"/>
@@ -1763,13 +1943,13 @@
       <c r="O11" s="8"/>
       <c r="P11" s="9"/>
       <c r="Q11" s="7" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="R11" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S11" s="7" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
       <c r="T11" s="7">
         <v>1</v>
@@ -1778,24 +1958,24 @@
         <v>53</v>
       </c>
       <c r="V11" s="7" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="W11" s="7" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="X11" s="7" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="Y11" s="7"/>
       <c r="Z11" s="7">
-        <v>0.9</v>
+        <v>0.3</v>
       </c>
       <c r="AA11" s="7"/>
       <c r="AB11" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC11" s="9" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="AD11" s="7" t="s">
         <v>60</v>
@@ -1820,18 +2000,18 @@
         <v>94</v>
       </c>
       <c r="C12" s="3">
-        <v>2025060176</v>
+        <v>2025060172</v>
       </c>
       <c r="D12" s="3"/>
       <c r="E12" s="3"/>
       <c r="F12" s="3">
-        <v>3183</v>
+        <v>2890</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>120</v>
+        <v>130</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
@@ -1842,13 +2022,13 @@
       <c r="O12" s="4"/>
       <c r="P12" s="10"/>
       <c r="Q12" s="3" t="s">
-        <v>121</v>
+        <v>131</v>
       </c>
       <c r="R12" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S12" s="3" t="s">
-        <v>110</v>
+        <v>52</v>
       </c>
       <c r="T12" s="3">
         <v>1</v>
@@ -1857,17 +2037,17 @@
         <v>53</v>
       </c>
       <c r="V12" s="3" t="s">
-        <v>122</v>
+        <v>132</v>
       </c>
       <c r="W12" s="3" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
       <c r="X12" s="3" t="s">
-        <v>124</v>
+        <v>134</v>
       </c>
       <c r="Y12" s="3"/>
       <c r="Z12" s="3">
-        <v>0.6</v>
+        <v>0.9</v>
       </c>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3" t="s">
@@ -1899,18 +2079,18 @@
         <v>94</v>
       </c>
       <c r="C13" s="7">
-        <v>2025060179</v>
+        <v>2025060176</v>
       </c>
       <c r="D13" s="7"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7">
-        <v>2890</v>
+        <v>3183</v>
       </c>
       <c r="G13" s="7" t="s">
-        <v>115</v>
+        <v>135</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="I13" s="7"/>
       <c r="J13" s="7"/>
@@ -1919,15 +2099,15 @@
       <c r="M13" s="8"/>
       <c r="N13" s="7"/>
       <c r="O13" s="8"/>
-      <c r="P13" s="8"/>
+      <c r="P13" s="9"/>
       <c r="Q13" s="7" t="s">
-        <v>116</v>
+        <v>136</v>
       </c>
       <c r="R13" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S13" s="7" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
       <c r="T13" s="7">
         <v>1</v>
@@ -1936,23 +2116,23 @@
         <v>53</v>
       </c>
       <c r="V13" s="7" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="W13" s="7" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="X13" s="7" t="s">
-        <v>126</v>
+        <v>139</v>
       </c>
       <c r="Y13" s="7"/>
       <c r="Z13" s="7">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="AA13" s="7"/>
       <c r="AB13" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC13" s="8" t="s">
+      <c r="AC13" s="9" t="s">
         <v>98</v>
       </c>
       <c r="AD13" s="7" t="s">
@@ -1967,6 +2147,575 @@
         <v>60</v>
       </c>
       <c r="AK13" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="14" spans="1:37">
+      <c r="A14" s="3">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2025060179</v>
+      </c>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3">
+        <v>2890</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="4"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="4"/>
+      <c r="P14" s="10"/>
+      <c r="Q14" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="R14" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S14" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T14" s="3">
+        <v>1</v>
+      </c>
+      <c r="U14" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V14" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="W14" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="X14" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC14" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK14" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:37">
+      <c r="A15" s="7">
+        <v>13</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C15" s="7">
+        <v>2025060239</v>
+      </c>
+      <c r="D15" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="E15" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F15" s="7">
+        <v>4698</v>
+      </c>
+      <c r="G15" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H15" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I15" s="7" t="s">
+        <v>144</v>
+      </c>
+      <c r="J15" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="K15" s="7" t="s">
+        <v>145</v>
+      </c>
+      <c r="L15" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M15" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="O15" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="P15" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T15" s="7">
+        <v>1</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>152</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y15" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="Z15" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA15" s="7"/>
+      <c r="AB15" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC15" s="9" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+      <c r="AG15" s="7"/>
+      <c r="AH15" s="7"/>
+      <c r="AI15" s="7"/>
+      <c r="AJ15" s="7"/>
+      <c r="AK15" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="16" spans="1:37">
+      <c r="A16" s="3">
+        <v>14</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="3">
+        <v>2025060310</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
+        <v>4552</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+      <c r="M16" s="4"/>
+      <c r="N16" s="3"/>
+      <c r="O16" s="4"/>
+      <c r="P16" s="10"/>
+      <c r="Q16" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="R16" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S16" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T16" s="3">
+        <v>1</v>
+      </c>
+      <c r="U16" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V16" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="W16" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="X16" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y16" s="3"/>
+      <c r="Z16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA16" s="3"/>
+      <c r="AB16" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC16" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE16" s="3"/>
+      <c r="AF16" s="3"/>
+      <c r="AG16" s="3"/>
+      <c r="AH16" s="3"/>
+      <c r="AI16" s="3"/>
+      <c r="AJ16" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK16" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="17" spans="1:37">
+      <c r="A17" s="7">
+        <v>15</v>
+      </c>
+      <c r="B17" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="7">
+        <v>2025060326</v>
+      </c>
+      <c r="D17" s="7"/>
+      <c r="E17" s="7"/>
+      <c r="F17" s="7">
+        <v>4658</v>
+      </c>
+      <c r="G17" s="7" t="s">
+        <v>162</v>
+      </c>
+      <c r="H17" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="8"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="8"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="R17" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S17" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T17" s="7">
+        <v>1</v>
+      </c>
+      <c r="U17" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V17" s="7" t="s">
+        <v>165</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA17" s="7"/>
+      <c r="AB17" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC17" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD17" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE17" s="7"/>
+      <c r="AF17" s="7"/>
+      <c r="AG17" s="7"/>
+      <c r="AH17" s="7"/>
+      <c r="AI17" s="7"/>
+      <c r="AJ17" s="7"/>
+      <c r="AK17" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:37">
+      <c r="A18" s="3">
+        <v>16</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C18" s="3">
+        <v>2025060340</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3">
+        <v>3770</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+      <c r="M18" s="4"/>
+      <c r="N18" s="3"/>
+      <c r="O18" s="4"/>
+      <c r="P18" s="10"/>
+      <c r="Q18" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="R18" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S18" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T18" s="3">
+        <v>1</v>
+      </c>
+      <c r="U18" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V18" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="W18" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="X18" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="Y18" s="3"/>
+      <c r="Z18" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA18" s="3"/>
+      <c r="AB18" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC18" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE18" s="3"/>
+      <c r="AF18" s="3"/>
+      <c r="AG18" s="3"/>
+      <c r="AH18" s="3"/>
+      <c r="AI18" s="3"/>
+      <c r="AJ18" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK18" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="19" spans="1:37">
+      <c r="A19" s="7">
+        <v>17</v>
+      </c>
+      <c r="B19" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C19" s="7">
+        <v>2025060422</v>
+      </c>
+      <c r="D19" s="7"/>
+      <c r="E19" s="7"/>
+      <c r="F19" s="7">
+        <v>4698</v>
+      </c>
+      <c r="G19" s="7" t="s">
+        <v>143</v>
+      </c>
+      <c r="H19" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I19" s="7"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="8"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="7" t="s">
+        <v>151</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T19" s="7">
+        <v>1</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V19" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="W19" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="X19" s="7" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA19" s="7"/>
+      <c r="AB19" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC19" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE19" s="7"/>
+      <c r="AF19" s="7"/>
+      <c r="AG19" s="7"/>
+      <c r="AH19" s="7"/>
+      <c r="AI19" s="7"/>
+      <c r="AJ19" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK19" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="1:37">
+      <c r="A20" s="3">
+        <v>18</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2025060423</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3">
+        <v>2325</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="4"/>
+      <c r="N20" s="3"/>
+      <c r="O20" s="4"/>
+      <c r="P20" s="4"/>
+      <c r="Q20" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="R20" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S20" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T20" s="3">
+        <v>1</v>
+      </c>
+      <c r="U20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V20" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="W20" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="X20" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="Y20" s="3"/>
+      <c r="Z20" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE20" s="3"/>
+      <c r="AF20" s="3"/>
+      <c r="AG20" s="3"/>
+      <c r="AH20" s="3"/>
+      <c r="AI20" s="3"/>
+      <c r="AJ20" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK20" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 2025/06/05 週四 10:17:00.84
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$20</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$26</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="180">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-03  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="235">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-05  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -543,6 +543,53 @@
     <t>2025-06-03 13:36:00</t>
   </si>
   <si>
+    <t>15060114060301</t>
+  </si>
+  <si>
+    <t>淡水魚市店</t>
+  </si>
+  <si>
+    <t>2025-06-03 14:45:47</t>
+  </si>
+  <si>
+    <t>星期二</t>
+  </si>
+  <si>
+    <t>HLF6</t>
+  </si>
+  <si>
+    <t>HL-多卡機QP3000E</t>
+  </si>
+  <si>
+    <t>F603</t>
+  </si>
+  <si>
+    <t>無法連線</t>
+  </si>
+  <si>
+    <t>門市反應TM1多卡機(QP3000E)三種卡片都無法讀卡/加值，協助門市執行版更後協助VNC操作悠遊卡機重開顯示悠遊卡通訊逾時!、操作一卡通開機顯示0801錯誤訊息:...、操作iCash愛金卡手動開機授權顯示代碼:20C...，請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF05060</t>
+  </si>
+  <si>
+    <t>2025-06-03 14:47:41</t>
+  </si>
+  <si>
+    <t>2025-06-04 10:51:00</t>
+  </si>
+  <si>
+    <t>2025-06-04 11:21:00</t>
+  </si>
+  <si>
+    <t>2025-06-04 18:47:00</t>
+  </si>
+  <si>
+    <t>更換多卡機QP3000
+換下8183001602
+換上8183003482</t>
+  </si>
+  <si>
     <t>北縣西雲店</t>
   </si>
   <si>
@@ -577,6 +624,133 @@
   </si>
   <si>
     <t>2025-06-03 15:50:00</t>
+  </si>
+  <si>
+    <t>E5197114060401</t>
+  </si>
+  <si>
+    <t>蘆洲鴻悅店</t>
+  </si>
+  <si>
+    <t>2025-06-04 08:41:31</t>
+  </si>
+  <si>
+    <t>星期三</t>
+  </si>
+  <si>
+    <t>觸控不良(游標偏移)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應TM1(TCX800)螢幕任何地方都需點好幾下才有反應，已協助執行觸控校正仍異常，與門市確認螢幕無貼保護貼、文宣...請台芝到店協助(他不是游標偏移，他是單純的銀幕觸控不良，有時候會要按好幾百次才按地到一個數字，已經嘗試過重開的方式，銀幕也擦過了，就是情況也還是一樣。)
+</t>
+  </si>
+  <si>
+    <t>THILF05197</t>
+  </si>
+  <si>
+    <t>2025-06-04 09:16:53</t>
+  </si>
+  <si>
+    <t>2025-06-04 15:44:00</t>
+  </si>
+  <si>
+    <t>2025-06-04 16:14:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 13:16:00</t>
+  </si>
+  <si>
+    <t>觸控螢幕進行矯正，目前測試正常</t>
+  </si>
+  <si>
+    <t>L519</t>
+  </si>
+  <si>
+    <t>車麗屋林口店</t>
+  </si>
+  <si>
+    <t>新北市林口區</t>
+  </si>
+  <si>
+    <t>THILF0L519</t>
+  </si>
+  <si>
+    <t>2025-06-04 11:03:15</t>
+  </si>
+  <si>
+    <t>2025-06-04 10:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-04 11:00:00</t>
+  </si>
+  <si>
+    <t>PMQ2</t>
+  </si>
+  <si>
+    <t>L551</t>
+  </si>
+  <si>
+    <t>林口顧家店</t>
+  </si>
+  <si>
+    <t>THILF0L551</t>
+  </si>
+  <si>
+    <t>2025-06-04 11:20:31</t>
+  </si>
+  <si>
+    <t>2025-06-04 11:20:00</t>
+  </si>
+  <si>
+    <t>13965114060403</t>
+  </si>
+  <si>
+    <t>急修件</t>
+  </si>
+  <si>
+    <t>板橋民治店</t>
+  </si>
+  <si>
+    <t>2025-06-04 14:55:37</t>
+  </si>
+  <si>
+    <t>HL24</t>
+  </si>
+  <si>
+    <t>HL-SC主機</t>
+  </si>
+  <si>
+    <t>檔案損毀(更換硬碟)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">06/04 15:18 啟動緊急叫修:門市反應sc(SHUTTLE6S)開啟hishop後當機，請門市重啟sc後畫面顯示正在掃瞄並修復磁碟機e槽卡在77%，ping1通無法vnc...請台芝到店協助
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)																																
+與門市確認帳務做到6/4，與通訊健誌副理確認有收到6/4的銷售，缺少tm1.2電子存根聯。並告知為第二顆硬碟有異常
+</t>
+  </si>
+  <si>
+    <t>THILF03965</t>
+  </si>
+  <si>
+    <t>2025-06-04 15:18:52</t>
+  </si>
+  <si>
+    <t>2025-06-04 15:35:00</t>
+  </si>
+  <si>
+    <t>2025-06-04 17:50:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 08:18:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SC更換第二顆硬碟不備份還原
+已提醒核對帳務
+版本：20250408
+</t>
+  </si>
+  <si>
+    <t>2025-06-04 17:57:44</t>
   </si>
 </sst>
 </file>
@@ -990,10 +1164,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK20"/>
+  <dimension ref="A1:AK26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC17" sqref="AC17"/>
+      <selection activeCell="AC23" sqref="AC23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2487,38 +2661,58 @@
         <v>16</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C18" s="3">
-        <v>2025060340</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+        <v>2025060339</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F18" s="3">
-        <v>3770</v>
+        <v>5060</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H18" s="3" t="s">
-        <v>169</v>
-      </c>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
-      <c r="K18" s="3"/>
-      <c r="L18" s="3"/>
-      <c r="M18" s="4"/>
-      <c r="N18" s="3"/>
-      <c r="O18" s="4"/>
-      <c r="P18" s="10"/>
+        <v>163</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K18" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="N18" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="O18" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P18" s="10" t="s">
+        <v>176</v>
+      </c>
       <c r="Q18" s="3" t="s">
-        <v>170</v>
+        <v>177</v>
       </c>
       <c r="R18" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S18" s="3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="T18" s="3">
         <v>1</v>
@@ -2527,36 +2721,34 @@
         <v>53</v>
       </c>
       <c r="V18" s="3" t="s">
-        <v>171</v>
+        <v>178</v>
       </c>
       <c r="W18" s="3" t="s">
-        <v>172</v>
+        <v>179</v>
       </c>
       <c r="X18" s="3" t="s">
-        <v>173</v>
-      </c>
-      <c r="Y18" s="3"/>
+        <v>180</v>
+      </c>
+      <c r="Y18" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="Z18" s="3">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC18" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD18" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>182</v>
+      </c>
+      <c r="AD18" s="3"/>
       <c r="AE18" s="3"/>
       <c r="AF18" s="3"/>
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
       <c r="AI18" s="3"/>
-      <c r="AJ18" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ18" s="3"/>
       <c r="AK18" s="3" t="s">
         <v>60</v>
       </c>
@@ -2569,18 +2761,18 @@
         <v>94</v>
       </c>
       <c r="C19" s="7">
-        <v>2025060422</v>
+        <v>2025060340</v>
       </c>
       <c r="D19" s="7"/>
       <c r="E19" s="7"/>
       <c r="F19" s="7">
-        <v>4698</v>
+        <v>3770</v>
       </c>
       <c r="G19" s="7" t="s">
-        <v>143</v>
+        <v>183</v>
       </c>
       <c r="H19" s="7" t="s">
-        <v>42</v>
+        <v>184</v>
       </c>
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
@@ -2591,13 +2783,13 @@
       <c r="O19" s="8"/>
       <c r="P19" s="9"/>
       <c r="Q19" s="7" t="s">
-        <v>151</v>
+        <v>185</v>
       </c>
       <c r="R19" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S19" s="7" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="T19" s="7">
         <v>1</v>
@@ -2606,13 +2798,13 @@
         <v>53</v>
       </c>
       <c r="V19" s="7" t="s">
-        <v>174</v>
+        <v>186</v>
       </c>
       <c r="W19" s="7" t="s">
-        <v>153</v>
+        <v>187</v>
       </c>
       <c r="X19" s="7" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="Y19" s="7"/>
       <c r="Z19" s="7">
@@ -2648,18 +2840,18 @@
         <v>94</v>
       </c>
       <c r="C20" s="3">
-        <v>2025060423</v>
+        <v>2025060422</v>
       </c>
       <c r="D20" s="3"/>
       <c r="E20" s="3"/>
       <c r="F20" s="3">
-        <v>2325</v>
+        <v>4698</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>169</v>
+        <v>42</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -2668,15 +2860,15 @@
       <c r="M20" s="4"/>
       <c r="N20" s="3"/>
       <c r="O20" s="4"/>
-      <c r="P20" s="4"/>
+      <c r="P20" s="10"/>
       <c r="Q20" s="3" t="s">
-        <v>177</v>
+        <v>151</v>
       </c>
       <c r="R20" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S20" s="3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="T20" s="3">
         <v>1</v>
@@ -2685,23 +2877,23 @@
         <v>53</v>
       </c>
       <c r="V20" s="3" t="s">
-        <v>178</v>
+        <v>189</v>
       </c>
       <c r="W20" s="3" t="s">
         <v>153</v>
       </c>
       <c r="X20" s="3" t="s">
-        <v>179</v>
+        <v>190</v>
       </c>
       <c r="Y20" s="3"/>
       <c r="Z20" s="3">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC20" s="4" t="s">
+      <c r="AC20" s="10" t="s">
         <v>98</v>
       </c>
       <c r="AD20" s="3" t="s">
@@ -2716,6 +2908,516 @@
         <v>60</v>
       </c>
       <c r="AK20" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="21" spans="1:37">
+      <c r="A21" s="7">
+        <v>19</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C21" s="7">
+        <v>2025060423</v>
+      </c>
+      <c r="D21" s="7"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="7">
+        <v>2325</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>191</v>
+      </c>
+      <c r="H21" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="8"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="8"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="7" t="s">
+        <v>192</v>
+      </c>
+      <c r="R21" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S21" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T21" s="7">
+        <v>1</v>
+      </c>
+      <c r="U21" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V21" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="W21" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="X21" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA21" s="7"/>
+      <c r="AB21" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC21" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE21" s="7"/>
+      <c r="AF21" s="7"/>
+      <c r="AG21" s="7"/>
+      <c r="AH21" s="7"/>
+      <c r="AI21" s="7"/>
+      <c r="AJ21" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK21" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="22" spans="1:37">
+      <c r="A22" s="3">
+        <v>20</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2025060521</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F22" s="3">
+        <v>5197</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="K22" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L22" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="N22" s="3">
+        <v>2307</v>
+      </c>
+      <c r="O22" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="P22" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="Q22" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="R22" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S22" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T22" s="3">
+        <v>1</v>
+      </c>
+      <c r="U22" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V22" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="W22" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="X22" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="Y22" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA22" s="3"/>
+      <c r="AB22" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC22" s="10" t="s">
+        <v>206</v>
+      </c>
+      <c r="AD22" s="3"/>
+      <c r="AE22" s="3"/>
+      <c r="AF22" s="3"/>
+      <c r="AG22" s="3"/>
+      <c r="AH22" s="3"/>
+      <c r="AI22" s="3"/>
+      <c r="AJ22" s="3"/>
+      <c r="AK22" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="23" spans="1:37">
+      <c r="A23" s="7">
+        <v>21</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C23" s="7">
+        <v>2025060563</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7" t="s">
+        <v>207</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>208</v>
+      </c>
+      <c r="H23" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="8"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="8"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="7" t="s">
+        <v>210</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T23" s="7">
+        <v>1</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="W23" s="7" t="s">
+        <v>212</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA23" s="7"/>
+      <c r="AB23" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC23" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE23" s="7"/>
+      <c r="AF23" s="7"/>
+      <c r="AG23" s="7"/>
+      <c r="AH23" s="7"/>
+      <c r="AI23" s="7"/>
+      <c r="AJ23" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK23" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="24" spans="1:37">
+      <c r="A24" s="3">
+        <v>22</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2025060568</v>
+      </c>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="G24" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="H24" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="I24" s="3"/>
+      <c r="J24" s="3"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+      <c r="M24" s="4"/>
+      <c r="N24" s="3"/>
+      <c r="O24" s="4"/>
+      <c r="P24" s="10"/>
+      <c r="Q24" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="R24" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T24" s="3">
+        <v>1</v>
+      </c>
+      <c r="U24" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V24" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="W24" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="X24" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y24" s="3"/>
+      <c r="Z24" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA24" s="3"/>
+      <c r="AB24" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC24" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE24" s="3"/>
+      <c r="AF24" s="3"/>
+      <c r="AG24" s="3"/>
+      <c r="AH24" s="3"/>
+      <c r="AI24" s="3"/>
+      <c r="AJ24" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK24" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="25" spans="1:37">
+      <c r="A25" s="7">
+        <v>23</v>
+      </c>
+      <c r="B25" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C25" s="7">
+        <v>2025060626</v>
+      </c>
+      <c r="D25" s="7" t="s">
+        <v>220</v>
+      </c>
+      <c r="E25" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F25" s="7">
+        <v>3965</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>222</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>223</v>
+      </c>
+      <c r="J25" s="7" t="s">
+        <v>198</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="M25" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="N25" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O25" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="P25" s="9" t="s">
+        <v>227</v>
+      </c>
+      <c r="Q25" s="7" t="s">
+        <v>228</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S25" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T25" s="7">
+        <v>1</v>
+      </c>
+      <c r="U25" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V25" s="7" t="s">
+        <v>229</v>
+      </c>
+      <c r="W25" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="X25" s="7" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y25" s="7" t="s">
+        <v>232</v>
+      </c>
+      <c r="Z25" s="7">
+        <v>2.3</v>
+      </c>
+      <c r="AA25" s="7"/>
+      <c r="AB25" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC25" s="9" t="s">
+        <v>233</v>
+      </c>
+      <c r="AD25" s="7"/>
+      <c r="AE25" s="7"/>
+      <c r="AF25" s="7"/>
+      <c r="AG25" s="7"/>
+      <c r="AH25" s="7"/>
+      <c r="AI25" s="7"/>
+      <c r="AJ25" s="7"/>
+      <c r="AK25" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="26" spans="1:37">
+      <c r="A26" s="3">
+        <v>24</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2025060691</v>
+      </c>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3">
+        <v>3965</v>
+      </c>
+      <c r="G26" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="H26" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I26" s="3"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+      <c r="L26" s="3"/>
+      <c r="M26" s="4"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="4"/>
+      <c r="P26" s="4"/>
+      <c r="Q26" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="R26" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S26" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T26" s="3">
+        <v>1</v>
+      </c>
+      <c r="U26" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V26" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="W26" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="X26" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="Y26" s="3"/>
+      <c r="Z26" s="3">
+        <v>2.3</v>
+      </c>
+      <c r="AA26" s="3"/>
+      <c r="AB26" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC26" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE26" s="3"/>
+      <c r="AF26" s="3"/>
+      <c r="AG26" s="3"/>
+      <c r="AH26" s="3"/>
+      <c r="AI26" s="3"/>
+      <c r="AJ26" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK26" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 2025/06/05 週四 16:45:16.42
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$26</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$36</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="284">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-05  )</t>
   </si>
@@ -751,6 +751,153 @@
   </si>
   <si>
     <t>2025-06-04 17:57:44</t>
+  </si>
+  <si>
+    <t>蘆洲中山一</t>
+  </si>
+  <si>
+    <t>THILF03929</t>
+  </si>
+  <si>
+    <t>2025-06-05 11:21:29</t>
+  </si>
+  <si>
+    <t>2025-06-05 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 11:20:00</t>
+  </si>
+  <si>
+    <t>北縣蘆信店</t>
+  </si>
+  <si>
+    <t>THILF03452</t>
+  </si>
+  <si>
+    <t>2025-06-05 12:44:19</t>
+  </si>
+  <si>
+    <t>2025-06-05 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 12:43:00</t>
+  </si>
+  <si>
+    <t>五股工商店</t>
+  </si>
+  <si>
+    <t>THILF04316</t>
+  </si>
+  <si>
+    <t>2025-06-05 13:55:27</t>
+  </si>
+  <si>
+    <t>2025-06-05 13:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 13:50:00</t>
+  </si>
+  <si>
+    <t>蘆洲湧蓮店</t>
+  </si>
+  <si>
+    <t>THILF04218</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:18:15</t>
+  </si>
+  <si>
+    <t>2025-06-05 13:00:00</t>
+  </si>
+  <si>
+    <t>D349</t>
+  </si>
+  <si>
+    <t>板橋成都店</t>
+  </si>
+  <si>
+    <t>THILF0D349</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:20:27</t>
+  </si>
+  <si>
+    <t>2025-06-05 13:58:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:20:00</t>
+  </si>
+  <si>
+    <t>北縣蘆旺店</t>
+  </si>
+  <si>
+    <t>THILF02958</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:25:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:24:00</t>
+  </si>
+  <si>
+    <t>五股成州店</t>
+  </si>
+  <si>
+    <t>THILF04801</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:36:37</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:40:00</t>
+  </si>
+  <si>
+    <t>板橋國慶店</t>
+  </si>
+  <si>
+    <t>THILF03416</t>
+  </si>
+  <si>
+    <t>2025-06-05 15:00:25</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:55:00</t>
+  </si>
+  <si>
+    <t>蘆洲洲正店</t>
+  </si>
+  <si>
+    <t>THILF04609</t>
+  </si>
+  <si>
+    <t>2025-06-05 15:26:43</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:51:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 15:26:00</t>
+  </si>
+  <si>
+    <t>五股凌雲店</t>
+  </si>
+  <si>
+    <t>THILF04819</t>
+  </si>
+  <si>
+    <t>2025-06-05 15:27:15</t>
+  </si>
+  <si>
+    <t>2025-06-05 14:50:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 15:30:00</t>
   </si>
 </sst>
 </file>
@@ -1164,10 +1311,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK26"/>
+  <dimension ref="A1:AK36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC23" sqref="AC23"/>
+      <selection activeCell="AC33" sqref="AC33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3370,7 +3517,7 @@
       <c r="M26" s="4"/>
       <c r="N26" s="3"/>
       <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
+      <c r="P26" s="10"/>
       <c r="Q26" s="3" t="s">
         <v>228</v>
       </c>
@@ -3403,7 +3550,7 @@
       <c r="AB26" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC26" s="4" t="s">
+      <c r="AC26" s="10" t="s">
         <v>98</v>
       </c>
       <c r="AD26" s="3" t="s">
@@ -3418,6 +3565,796 @@
         <v>60</v>
       </c>
       <c r="AK26" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:37">
+      <c r="A27" s="7">
+        <v>25</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C27" s="7">
+        <v>2025060733</v>
+      </c>
+      <c r="D27" s="7"/>
+      <c r="E27" s="7"/>
+      <c r="F27" s="7">
+        <v>3929</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="H27" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="8"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="8"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T27" s="7">
+        <v>1</v>
+      </c>
+      <c r="U27" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="W27" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>239</v>
+      </c>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA27" s="7"/>
+      <c r="AB27" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC27" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE27" s="7"/>
+      <c r="AF27" s="7"/>
+      <c r="AG27" s="7"/>
+      <c r="AH27" s="7"/>
+      <c r="AI27" s="7"/>
+      <c r="AJ27" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK27" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="28" spans="1:37">
+      <c r="A28" s="3">
+        <v>26</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2025060770</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3">
+        <v>3452</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="H28" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="4"/>
+      <c r="N28" s="3"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="10"/>
+      <c r="Q28" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="R28" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S28" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T28" s="3">
+        <v>1</v>
+      </c>
+      <c r="U28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V28" s="3" t="s">
+        <v>242</v>
+      </c>
+      <c r="W28" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="X28" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="Y28" s="3"/>
+      <c r="Z28" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA28" s="3"/>
+      <c r="AB28" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC28" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE28" s="3"/>
+      <c r="AF28" s="3"/>
+      <c r="AG28" s="3"/>
+      <c r="AH28" s="3"/>
+      <c r="AI28" s="3"/>
+      <c r="AJ28" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK28" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="29" spans="1:37">
+      <c r="A29" s="7">
+        <v>27</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C29" s="7">
+        <v>2025060781</v>
+      </c>
+      <c r="D29" s="7"/>
+      <c r="E29" s="7"/>
+      <c r="F29" s="7">
+        <v>4316</v>
+      </c>
+      <c r="G29" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="H29" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I29" s="7"/>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="8"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="8"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="7" t="s">
+        <v>246</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T29" s="7">
+        <v>1</v>
+      </c>
+      <c r="U29" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V29" s="7" t="s">
+        <v>247</v>
+      </c>
+      <c r="W29" s="7" t="s">
+        <v>248</v>
+      </c>
+      <c r="X29" s="7" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA29" s="7"/>
+      <c r="AB29" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC29" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE29" s="7"/>
+      <c r="AF29" s="7"/>
+      <c r="AG29" s="7"/>
+      <c r="AH29" s="7"/>
+      <c r="AI29" s="7"/>
+      <c r="AJ29" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK29" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="30" spans="1:37">
+      <c r="A30" s="3">
+        <v>28</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2025060792</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3">
+        <v>4218</v>
+      </c>
+      <c r="G30" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I30" s="3"/>
+      <c r="J30" s="3"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+      <c r="M30" s="4"/>
+      <c r="N30" s="3"/>
+      <c r="O30" s="4"/>
+      <c r="P30" s="10"/>
+      <c r="Q30" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="R30" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T30" s="3">
+        <v>1</v>
+      </c>
+      <c r="U30" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V30" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="W30" s="3" t="s">
+        <v>253</v>
+      </c>
+      <c r="X30" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y30" s="3"/>
+      <c r="Z30" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA30" s="3"/>
+      <c r="AB30" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC30" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE30" s="3"/>
+      <c r="AF30" s="3"/>
+      <c r="AG30" s="3"/>
+      <c r="AH30" s="3"/>
+      <c r="AI30" s="3"/>
+      <c r="AJ30" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK30" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="31" spans="1:37">
+      <c r="A31" s="7">
+        <v>29</v>
+      </c>
+      <c r="B31" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C31" s="7">
+        <v>2025060795</v>
+      </c>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7" t="s">
+        <v>254</v>
+      </c>
+      <c r="G31" s="7" t="s">
+        <v>255</v>
+      </c>
+      <c r="H31" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="8"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="8"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="R31" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S31" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T31" s="7">
+        <v>1</v>
+      </c>
+      <c r="U31" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V31" s="7" t="s">
+        <v>257</v>
+      </c>
+      <c r="W31" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="X31" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA31" s="7"/>
+      <c r="AB31" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC31" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD31" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE31" s="7"/>
+      <c r="AF31" s="7"/>
+      <c r="AG31" s="7"/>
+      <c r="AH31" s="7"/>
+      <c r="AI31" s="7"/>
+      <c r="AJ31" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK31" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="32" spans="1:37">
+      <c r="A32" s="3">
+        <v>30</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C32" s="3">
+        <v>2025060796</v>
+      </c>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3">
+        <v>2958</v>
+      </c>
+      <c r="G32" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="H32" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I32" s="3"/>
+      <c r="J32" s="3"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+      <c r="M32" s="4"/>
+      <c r="N32" s="3"/>
+      <c r="O32" s="4"/>
+      <c r="P32" s="10"/>
+      <c r="Q32" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S32" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T32" s="3">
+        <v>1</v>
+      </c>
+      <c r="U32" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V32" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="W32" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="X32" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="Y32" s="3"/>
+      <c r="Z32" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA32" s="3"/>
+      <c r="AB32" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC32" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE32" s="3"/>
+      <c r="AF32" s="3"/>
+      <c r="AG32" s="3"/>
+      <c r="AH32" s="3"/>
+      <c r="AI32" s="3"/>
+      <c r="AJ32" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK32" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="33" spans="1:37">
+      <c r="A33" s="7">
+        <v>31</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C33" s="7">
+        <v>2025060799</v>
+      </c>
+      <c r="D33" s="7"/>
+      <c r="E33" s="7"/>
+      <c r="F33" s="7">
+        <v>4801</v>
+      </c>
+      <c r="G33" s="7" t="s">
+        <v>264</v>
+      </c>
+      <c r="H33" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I33" s="7"/>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="8"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="8"/>
+      <c r="P33" s="9"/>
+      <c r="Q33" s="7" t="s">
+        <v>265</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S33" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T33" s="7">
+        <v>1</v>
+      </c>
+      <c r="U33" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V33" s="7" t="s">
+        <v>266</v>
+      </c>
+      <c r="W33" s="7" t="s">
+        <v>267</v>
+      </c>
+      <c r="X33" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA33" s="7"/>
+      <c r="AB33" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC33" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE33" s="7"/>
+      <c r="AF33" s="7"/>
+      <c r="AG33" s="7"/>
+      <c r="AH33" s="7"/>
+      <c r="AI33" s="7"/>
+      <c r="AJ33" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK33" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="34" spans="1:37">
+      <c r="A34" s="3">
+        <v>32</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="3">
+        <v>2025060808</v>
+      </c>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3">
+        <v>3416</v>
+      </c>
+      <c r="G34" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="H34" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I34" s="3"/>
+      <c r="J34" s="3"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+      <c r="M34" s="4"/>
+      <c r="N34" s="3"/>
+      <c r="O34" s="4"/>
+      <c r="P34" s="10"/>
+      <c r="Q34" s="3" t="s">
+        <v>270</v>
+      </c>
+      <c r="R34" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S34" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T34" s="3">
+        <v>1</v>
+      </c>
+      <c r="U34" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V34" s="3" t="s">
+        <v>271</v>
+      </c>
+      <c r="W34" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="X34" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="Y34" s="3"/>
+      <c r="Z34" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA34" s="3"/>
+      <c r="AB34" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC34" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE34" s="3"/>
+      <c r="AF34" s="3"/>
+      <c r="AG34" s="3"/>
+      <c r="AH34" s="3"/>
+      <c r="AI34" s="3"/>
+      <c r="AJ34" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK34" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="35" spans="1:37">
+      <c r="A35" s="7">
+        <v>33</v>
+      </c>
+      <c r="B35" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C35" s="7">
+        <v>2025060816</v>
+      </c>
+      <c r="D35" s="7"/>
+      <c r="E35" s="7"/>
+      <c r="F35" s="7">
+        <v>4609</v>
+      </c>
+      <c r="G35" s="7" t="s">
+        <v>274</v>
+      </c>
+      <c r="H35" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="8"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="8"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="7" t="s">
+        <v>275</v>
+      </c>
+      <c r="R35" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S35" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T35" s="7">
+        <v>1</v>
+      </c>
+      <c r="U35" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V35" s="7" t="s">
+        <v>276</v>
+      </c>
+      <c r="W35" s="7" t="s">
+        <v>277</v>
+      </c>
+      <c r="X35" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA35" s="7"/>
+      <c r="AB35" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC35" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE35" s="7"/>
+      <c r="AF35" s="7"/>
+      <c r="AG35" s="7"/>
+      <c r="AH35" s="7"/>
+      <c r="AI35" s="7"/>
+      <c r="AJ35" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK35" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="36" spans="1:37">
+      <c r="A36" s="3">
+        <v>34</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2025060817</v>
+      </c>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3">
+        <v>4819</v>
+      </c>
+      <c r="G36" s="3" t="s">
+        <v>279</v>
+      </c>
+      <c r="H36" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I36" s="3"/>
+      <c r="J36" s="3"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="3"/>
+      <c r="O36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="3" t="s">
+        <v>280</v>
+      </c>
+      <c r="R36" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S36" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T36" s="3">
+        <v>1</v>
+      </c>
+      <c r="U36" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V36" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="W36" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="X36" s="3" t="s">
+        <v>283</v>
+      </c>
+      <c r="Y36" s="3"/>
+      <c r="Z36" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA36" s="3"/>
+      <c r="AB36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC36" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE36" s="3"/>
+      <c r="AF36" s="3"/>
+      <c r="AG36" s="3"/>
+      <c r="AH36" s="3"/>
+      <c r="AI36" s="3"/>
+      <c r="AJ36" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK36" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 2025/06/05 週四 17:23:26.07
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$36</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$37</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="289">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-05  )</t>
   </si>
@@ -898,6 +898,21 @@
   </si>
   <si>
     <t>2025-06-05 15:30:00</t>
+  </si>
+  <si>
+    <t>蘆洲長樂店</t>
+  </si>
+  <si>
+    <t>THILF04125</t>
+  </si>
+  <si>
+    <t>2025-06-05 17:00:54</t>
+  </si>
+  <si>
+    <t>2025-06-05 16:10:00</t>
+  </si>
+  <si>
+    <t>2025-06-05 17:00:00</t>
   </si>
 </sst>
 </file>
@@ -1311,10 +1326,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK36"/>
+  <dimension ref="A1:AK37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC33" sqref="AC33"/>
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4307,7 +4322,7 @@
       <c r="M36" s="4"/>
       <c r="N36" s="3"/>
       <c r="O36" s="4"/>
-      <c r="P36" s="4"/>
+      <c r="P36" s="10"/>
       <c r="Q36" s="3" t="s">
         <v>280</v>
       </c>
@@ -4340,7 +4355,7 @@
       <c r="AB36" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC36" s="4" t="s">
+      <c r="AC36" s="10" t="s">
         <v>98</v>
       </c>
       <c r="AD36" s="3" t="s">
@@ -4355,6 +4370,85 @@
         <v>60</v>
       </c>
       <c r="AK36" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="37" spans="1:37">
+      <c r="A37" s="7">
+        <v>35</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C37" s="7">
+        <v>2025060867</v>
+      </c>
+      <c r="D37" s="7"/>
+      <c r="E37" s="7"/>
+      <c r="F37" s="7">
+        <v>4125</v>
+      </c>
+      <c r="G37" s="7" t="s">
+        <v>284</v>
+      </c>
+      <c r="H37" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I37" s="7"/>
+      <c r="J37" s="7"/>
+      <c r="K37" s="7"/>
+      <c r="L37" s="7"/>
+      <c r="M37" s="8"/>
+      <c r="N37" s="7"/>
+      <c r="O37" s="8"/>
+      <c r="P37" s="8"/>
+      <c r="Q37" s="7" t="s">
+        <v>285</v>
+      </c>
+      <c r="R37" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S37" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T37" s="7">
+        <v>1</v>
+      </c>
+      <c r="U37" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V37" s="7" t="s">
+        <v>286</v>
+      </c>
+      <c r="W37" s="7" t="s">
+        <v>287</v>
+      </c>
+      <c r="X37" s="7" t="s">
+        <v>288</v>
+      </c>
+      <c r="Y37" s="7"/>
+      <c r="Z37" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA37" s="7"/>
+      <c r="AB37" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC37" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD37" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE37" s="7"/>
+      <c r="AF37" s="7"/>
+      <c r="AG37" s="7"/>
+      <c r="AH37" s="7"/>
+      <c r="AI37" s="7"/>
+      <c r="AJ37" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK37" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 2025/06/06 週五 17:41:16.64
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$37</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$38</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="289">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-05  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="300">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-06  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -751,6 +751,41 @@
   </si>
   <si>
     <t>2025-06-04 17:57:44</t>
+  </si>
+  <si>
+    <t>14259114060501</t>
+  </si>
+  <si>
+    <t>八里水灣店</t>
+  </si>
+  <si>
+    <t>新北市八里區</t>
+  </si>
+  <si>
+    <t>2025-06-05 10:32:08</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2025/6/5 (週四) 上午 10:30總公司日正mail:請協助派工4259 八里水灣店，到店更換SC(SHUTTLE5S)第二顆硬碟不備份還原。請啟動一般叫修，謝謝。
+PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)
+</t>
+  </si>
+  <si>
+    <t>THILF04259</t>
+  </si>
+  <si>
+    <t>2025-06-05 10:38:10</t>
+  </si>
+  <si>
+    <t>2025-06-06 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-06 13:05:00</t>
+  </si>
+  <si>
+    <t>2025-06-06 14:38:00</t>
+  </si>
+  <si>
+    <t>更換第二顆硬碟不備份還原完成</t>
   </si>
   <si>
     <t>蘆洲中山一</t>
@@ -1326,10 +1361,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK37"/>
+  <dimension ref="A1:AK38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A37" sqref="A37"/>
+      <selection activeCell="AC35" sqref="AC35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3588,32 +3623,52 @@
         <v>25</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C27" s="7">
-        <v>2025060733</v>
-      </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="7"/>
+        <v>2025060710</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>235</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F27" s="7">
-        <v>3929</v>
+        <v>4259</v>
       </c>
       <c r="G27" s="7" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="H27" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="I27" s="7"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="7"/>
-      <c r="L27" s="7"/>
-      <c r="M27" s="8"/>
-      <c r="N27" s="7"/>
-      <c r="O27" s="8"/>
-      <c r="P27" s="9"/>
+        <v>237</v>
+      </c>
+      <c r="I27" s="7" t="s">
+        <v>238</v>
+      </c>
+      <c r="J27" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="M27" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="N27" s="7">
+        <v>2405</v>
+      </c>
+      <c r="O27" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="P27" s="9" t="s">
+        <v>239</v>
+      </c>
       <c r="Q27" s="7" t="s">
-        <v>236</v>
+        <v>240</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>51</v>
@@ -3628,36 +3683,34 @@
         <v>53</v>
       </c>
       <c r="V27" s="7" t="s">
-        <v>237</v>
+        <v>241</v>
       </c>
       <c r="W27" s="7" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="X27" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="Y27" s="7"/>
+        <v>243</v>
+      </c>
+      <c r="Y27" s="7" t="s">
+        <v>244</v>
+      </c>
       <c r="Z27" s="7">
-        <v>0.3</v>
+        <v>2.1</v>
       </c>
       <c r="AA27" s="7"/>
       <c r="AB27" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC27" s="9" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD27" s="7" t="s">
-        <v>60</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="AD27" s="7"/>
       <c r="AE27" s="7"/>
       <c r="AF27" s="7"/>
       <c r="AG27" s="7"/>
       <c r="AH27" s="7"/>
       <c r="AI27" s="7"/>
-      <c r="AJ27" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ27" s="7"/>
       <c r="AK27" s="7" t="s">
         <v>60</v>
       </c>
@@ -3670,15 +3723,15 @@
         <v>94</v>
       </c>
       <c r="C28" s="3">
-        <v>2025060770</v>
+        <v>2025060733</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3">
-        <v>3452</v>
+        <v>3929</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>240</v>
+        <v>246</v>
       </c>
       <c r="H28" s="3" t="s">
         <v>101</v>
@@ -3692,7 +3745,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="10"/>
       <c r="Q28" s="3" t="s">
-        <v>241</v>
+        <v>247</v>
       </c>
       <c r="R28" s="3" t="s">
         <v>51</v>
@@ -3707,17 +3760,17 @@
         <v>53</v>
       </c>
       <c r="V28" s="3" t="s">
-        <v>242</v>
+        <v>248</v>
       </c>
       <c r="W28" s="3" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="X28" s="3" t="s">
-        <v>244</v>
+        <v>250</v>
       </c>
       <c r="Y28" s="3"/>
       <c r="Z28" s="3">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="AA28" s="3"/>
       <c r="AB28" s="3" t="s">
@@ -3749,18 +3802,18 @@
         <v>94</v>
       </c>
       <c r="C29" s="7">
-        <v>2025060781</v>
+        <v>2025060770</v>
       </c>
       <c r="D29" s="7"/>
       <c r="E29" s="7"/>
       <c r="F29" s="7">
-        <v>4316</v>
+        <v>3452</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>245</v>
+        <v>251</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>184</v>
+        <v>101</v>
       </c>
       <c r="I29" s="7"/>
       <c r="J29" s="7"/>
@@ -3771,13 +3824,13 @@
       <c r="O29" s="8"/>
       <c r="P29" s="9"/>
       <c r="Q29" s="7" t="s">
-        <v>246</v>
+        <v>252</v>
       </c>
       <c r="R29" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S29" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="T29" s="7">
         <v>1</v>
@@ -3786,24 +3839,24 @@
         <v>53</v>
       </c>
       <c r="V29" s="7" t="s">
-        <v>247</v>
+        <v>253</v>
       </c>
       <c r="W29" s="7" t="s">
-        <v>248</v>
+        <v>254</v>
       </c>
       <c r="X29" s="7" t="s">
-        <v>249</v>
+        <v>255</v>
       </c>
       <c r="Y29" s="7"/>
       <c r="Z29" s="7">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="AA29" s="7"/>
       <c r="AB29" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC29" s="9" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="AD29" s="7" t="s">
         <v>60</v>
@@ -3828,18 +3881,18 @@
         <v>94</v>
       </c>
       <c r="C30" s="3">
-        <v>2025060792</v>
+        <v>2025060781</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3">
-        <v>4218</v>
+        <v>4316</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>250</v>
+        <v>256</v>
       </c>
       <c r="H30" s="3" t="s">
-        <v>101</v>
+        <v>184</v>
       </c>
       <c r="I30" s="3"/>
       <c r="J30" s="3"/>
@@ -3850,13 +3903,13 @@
       <c r="O30" s="4"/>
       <c r="P30" s="10"/>
       <c r="Q30" s="3" t="s">
-        <v>251</v>
+        <v>257</v>
       </c>
       <c r="R30" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S30" s="3" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="T30" s="3">
         <v>1</v>
@@ -3865,24 +3918,24 @@
         <v>53</v>
       </c>
       <c r="V30" s="3" t="s">
-        <v>252</v>
+        <v>258</v>
       </c>
       <c r="W30" s="3" t="s">
-        <v>253</v>
+        <v>259</v>
       </c>
       <c r="X30" s="3" t="s">
-        <v>248</v>
+        <v>260</v>
       </c>
       <c r="Y30" s="3"/>
       <c r="Z30" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA30" s="3"/>
       <c r="AB30" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC30" s="10" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="AD30" s="3" t="s">
         <v>60</v>
@@ -3907,18 +3960,18 @@
         <v>94</v>
       </c>
       <c r="C31" s="7">
-        <v>2025060795</v>
+        <v>2025060792</v>
       </c>
       <c r="D31" s="7"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="7" t="s">
-        <v>254</v>
+      <c r="F31" s="7">
+        <v>4218</v>
       </c>
       <c r="G31" s="7" t="s">
-        <v>255</v>
+        <v>261</v>
       </c>
       <c r="H31" s="7" t="s">
-        <v>123</v>
+        <v>101</v>
       </c>
       <c r="I31" s="7"/>
       <c r="J31" s="7"/>
@@ -3929,13 +3982,13 @@
       <c r="O31" s="8"/>
       <c r="P31" s="9"/>
       <c r="Q31" s="7" t="s">
-        <v>256</v>
+        <v>262</v>
       </c>
       <c r="R31" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S31" s="7" t="s">
-        <v>125</v>
+        <v>52</v>
       </c>
       <c r="T31" s="7">
         <v>1</v>
@@ -3944,24 +3997,24 @@
         <v>53</v>
       </c>
       <c r="V31" s="7" t="s">
-        <v>257</v>
+        <v>263</v>
       </c>
       <c r="W31" s="7" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="X31" s="7" t="s">
         <v>259</v>
       </c>
       <c r="Y31" s="7"/>
       <c r="Z31" s="7">
-        <v>0.4</v>
+        <v>0.5</v>
       </c>
       <c r="AA31" s="7"/>
       <c r="AB31" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC31" s="9" t="s">
-        <v>129</v>
+        <v>98</v>
       </c>
       <c r="AD31" s="7" t="s">
         <v>60</v>
@@ -3986,18 +4039,18 @@
         <v>94</v>
       </c>
       <c r="C32" s="3">
-        <v>2025060796</v>
+        <v>2025060795</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
-      <c r="F32" s="3">
-        <v>2958</v>
+      <c r="F32" s="3" t="s">
+        <v>265</v>
       </c>
       <c r="G32" s="3" t="s">
-        <v>260</v>
+        <v>266</v>
       </c>
       <c r="H32" s="3" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="I32" s="3"/>
       <c r="J32" s="3"/>
@@ -4008,13 +4061,13 @@
       <c r="O32" s="4"/>
       <c r="P32" s="10"/>
       <c r="Q32" s="3" t="s">
-        <v>261</v>
+        <v>267</v>
       </c>
       <c r="R32" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S32" s="3" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
       <c r="T32" s="3">
         <v>1</v>
@@ -4023,24 +4076,24 @@
         <v>53</v>
       </c>
       <c r="V32" s="3" t="s">
-        <v>262</v>
+        <v>268</v>
       </c>
       <c r="W32" s="3" t="s">
-        <v>249</v>
+        <v>269</v>
       </c>
       <c r="X32" s="3" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="Y32" s="3"/>
       <c r="Z32" s="3">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="AA32" s="3"/>
       <c r="AB32" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC32" s="10" t="s">
-        <v>98</v>
+        <v>129</v>
       </c>
       <c r="AD32" s="3" t="s">
         <v>60</v>
@@ -4065,18 +4118,18 @@
         <v>94</v>
       </c>
       <c r="C33" s="7">
-        <v>2025060799</v>
+        <v>2025060796</v>
       </c>
       <c r="D33" s="7"/>
       <c r="E33" s="7"/>
       <c r="F33" s="7">
-        <v>4801</v>
+        <v>2958</v>
       </c>
       <c r="G33" s="7" t="s">
-        <v>264</v>
+        <v>271</v>
       </c>
       <c r="H33" s="7" t="s">
-        <v>184</v>
+        <v>101</v>
       </c>
       <c r="I33" s="7"/>
       <c r="J33" s="7"/>
@@ -4087,13 +4140,13 @@
       <c r="O33" s="8"/>
       <c r="P33" s="9"/>
       <c r="Q33" s="7" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S33" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="T33" s="7">
         <v>1</v>
@@ -4102,17 +4155,17 @@
         <v>53</v>
       </c>
       <c r="V33" s="7" t="s">
-        <v>266</v>
+        <v>273</v>
       </c>
       <c r="W33" s="7" t="s">
-        <v>267</v>
+        <v>260</v>
       </c>
       <c r="X33" s="7" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="Y33" s="7"/>
       <c r="Z33" s="7">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="AA33" s="7"/>
       <c r="AB33" s="7" t="s">
@@ -4144,18 +4197,18 @@
         <v>94</v>
       </c>
       <c r="C34" s="3">
-        <v>2025060808</v>
+        <v>2025060799</v>
       </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3">
-        <v>3416</v>
+        <v>4801</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>269</v>
+        <v>275</v>
       </c>
       <c r="H34" s="3" t="s">
-        <v>123</v>
+        <v>184</v>
       </c>
       <c r="I34" s="3"/>
       <c r="J34" s="3"/>
@@ -4166,13 +4219,13 @@
       <c r="O34" s="4"/>
       <c r="P34" s="10"/>
       <c r="Q34" s="3" t="s">
-        <v>270</v>
+        <v>276</v>
       </c>
       <c r="R34" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S34" s="3" t="s">
-        <v>125</v>
+        <v>73</v>
       </c>
       <c r="T34" s="3">
         <v>1</v>
@@ -4181,17 +4234,17 @@
         <v>53</v>
       </c>
       <c r="V34" s="3" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="W34" s="3" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="X34" s="3" t="s">
-        <v>273</v>
+        <v>279</v>
       </c>
       <c r="Y34" s="3"/>
       <c r="Z34" s="3">
-        <v>0.4</v>
+        <v>0.7</v>
       </c>
       <c r="AA34" s="3"/>
       <c r="AB34" s="3" t="s">
@@ -4223,18 +4276,18 @@
         <v>94</v>
       </c>
       <c r="C35" s="7">
-        <v>2025060816</v>
+        <v>2025060808</v>
       </c>
       <c r="D35" s="7"/>
       <c r="E35" s="7"/>
       <c r="F35" s="7">
-        <v>4609</v>
+        <v>3416</v>
       </c>
       <c r="G35" s="7" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="H35" s="7" t="s">
-        <v>101</v>
+        <v>123</v>
       </c>
       <c r="I35" s="7"/>
       <c r="J35" s="7"/>
@@ -4245,13 +4298,13 @@
       <c r="O35" s="8"/>
       <c r="P35" s="9"/>
       <c r="Q35" s="7" t="s">
-        <v>275</v>
+        <v>281</v>
       </c>
       <c r="R35" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S35" s="7" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
       <c r="T35" s="7">
         <v>1</v>
@@ -4260,17 +4313,17 @@
         <v>53</v>
       </c>
       <c r="V35" s="7" t="s">
-        <v>276</v>
+        <v>282</v>
       </c>
       <c r="W35" s="7" t="s">
-        <v>277</v>
+        <v>283</v>
       </c>
       <c r="X35" s="7" t="s">
-        <v>278</v>
+        <v>284</v>
       </c>
       <c r="Y35" s="7"/>
       <c r="Z35" s="7">
-        <v>0.6</v>
+        <v>0.4</v>
       </c>
       <c r="AA35" s="7"/>
       <c r="AB35" s="7" t="s">
@@ -4302,18 +4355,18 @@
         <v>94</v>
       </c>
       <c r="C36" s="3">
-        <v>2025060817</v>
+        <v>2025060816</v>
       </c>
       <c r="D36" s="3"/>
       <c r="E36" s="3"/>
       <c r="F36" s="3">
-        <v>4819</v>
+        <v>4609</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>279</v>
+        <v>285</v>
       </c>
       <c r="H36" s="3" t="s">
-        <v>184</v>
+        <v>101</v>
       </c>
       <c r="I36" s="3"/>
       <c r="J36" s="3"/>
@@ -4324,13 +4377,13 @@
       <c r="O36" s="4"/>
       <c r="P36" s="10"/>
       <c r="Q36" s="3" t="s">
-        <v>280</v>
+        <v>286</v>
       </c>
       <c r="R36" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S36" s="3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="T36" s="3">
         <v>1</v>
@@ -4339,17 +4392,17 @@
         <v>53</v>
       </c>
       <c r="V36" s="3" t="s">
-        <v>281</v>
+        <v>287</v>
       </c>
       <c r="W36" s="3" t="s">
-        <v>282</v>
+        <v>288</v>
       </c>
       <c r="X36" s="3" t="s">
-        <v>283</v>
+        <v>289</v>
       </c>
       <c r="Y36" s="3"/>
       <c r="Z36" s="3">
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="AA36" s="3"/>
       <c r="AB36" s="3" t="s">
@@ -4381,18 +4434,18 @@
         <v>94</v>
       </c>
       <c r="C37" s="7">
-        <v>2025060867</v>
+        <v>2025060817</v>
       </c>
       <c r="D37" s="7"/>
       <c r="E37" s="7"/>
       <c r="F37" s="7">
-        <v>4125</v>
+        <v>4819</v>
       </c>
       <c r="G37" s="7" t="s">
-        <v>284</v>
+        <v>290</v>
       </c>
       <c r="H37" s="7" t="s">
-        <v>101</v>
+        <v>184</v>
       </c>
       <c r="I37" s="7"/>
       <c r="J37" s="7"/>
@@ -4401,15 +4454,15 @@
       <c r="M37" s="8"/>
       <c r="N37" s="7"/>
       <c r="O37" s="8"/>
-      <c r="P37" s="8"/>
+      <c r="P37" s="9"/>
       <c r="Q37" s="7" t="s">
-        <v>285</v>
+        <v>291</v>
       </c>
       <c r="R37" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S37" s="7" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="T37" s="7">
         <v>1</v>
@@ -4418,23 +4471,23 @@
         <v>53</v>
       </c>
       <c r="V37" s="7" t="s">
-        <v>286</v>
+        <v>292</v>
       </c>
       <c r="W37" s="7" t="s">
-        <v>287</v>
+        <v>293</v>
       </c>
       <c r="X37" s="7" t="s">
-        <v>288</v>
+        <v>294</v>
       </c>
       <c r="Y37" s="7"/>
       <c r="Z37" s="7">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="AA37" s="7"/>
       <c r="AB37" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC37" s="8" t="s">
+      <c r="AC37" s="9" t="s">
         <v>98</v>
       </c>
       <c r="AD37" s="7" t="s">
@@ -4449,6 +4502,85 @@
         <v>60</v>
       </c>
       <c r="AK37" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="38" spans="1:37">
+      <c r="A38" s="3">
+        <v>36</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2025060867</v>
+      </c>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3">
+        <v>4125</v>
+      </c>
+      <c r="G38" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I38" s="3"/>
+      <c r="J38" s="3"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="3"/>
+      <c r="O38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="R38" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S38" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T38" s="3">
+        <v>1</v>
+      </c>
+      <c r="U38" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V38" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="W38" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="X38" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="Y38" s="3"/>
+      <c r="Z38" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA38" s="3"/>
+      <c r="AB38" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC38" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE38" s="3"/>
+      <c r="AF38" s="3"/>
+      <c r="AG38" s="3"/>
+      <c r="AH38" s="3"/>
+      <c r="AI38" s="3"/>
+      <c r="AJ38" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK38" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 2025/06/09 週一 13:49:14.01
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$38</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$47</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="300">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-06  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="364">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-09  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -948,6 +948,201 @@
   </si>
   <si>
     <t>2025-06-05 17:00:00</t>
+  </si>
+  <si>
+    <t>13840114060601</t>
+  </si>
+  <si>
+    <t>北縣天龍店</t>
+  </si>
+  <si>
+    <t>2025-06-06 12:14:43</t>
+  </si>
+  <si>
+    <t>門市反應tm2多卡機(QP3000E)無法使用版本更新後悠遊卡機重開顯示悠遊卡通訊逾時!、操作一卡通開機顯示0801錯誤訊息....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03840</t>
+  </si>
+  <si>
+    <t>2025-06-06 12:18:18</t>
+  </si>
+  <si>
+    <t>2025-06-09 11:07:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 11:37:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 16:18:00</t>
+  </si>
+  <si>
+    <t>重新插拔電源及COM線接測試，現場測試多卡機為正常狀態無異狀，請店員進行觀察</t>
+  </si>
+  <si>
+    <t>E3785114060601</t>
+  </si>
+  <si>
+    <t>北縣莊榮店</t>
+  </si>
+  <si>
+    <t>2025-06-06 14:32:13</t>
+  </si>
+  <si>
+    <t>HL58</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET主機</t>
+  </si>
+  <si>
+    <t>門市反應MMK四代機無法連線，PING60不通，門市嘗試重啟MMK後無跳出網路偵測介面.....請台芝到店協助(無法?線)</t>
+  </si>
+  <si>
+    <t>THILF03785</t>
+  </si>
+  <si>
+    <t>2025-06-06 15:01:39</t>
+  </si>
+  <si>
+    <t>2025-06-09 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 19:01:00</t>
+  </si>
+  <si>
+    <t>重設hub 重插網路線 網路偵測介面設定正常</t>
+  </si>
+  <si>
+    <t>E2222114060701</t>
+  </si>
+  <si>
+    <t>三重義天店</t>
+  </si>
+  <si>
+    <t>2025-06-07 00:45:53</t>
+  </si>
+  <si>
+    <t>星期六</t>
+  </si>
+  <si>
+    <t>凌晨</t>
+  </si>
+  <si>
+    <t>門市反應TM2熱感發票機(BSC10)裁切異常，已嘗試重啟設備+安裝新紙捲及簡易清潔仍無改善...請台芝到店協助(熱感應機無法連線)
+06/07 09:00 門市未接聽多通...廖</t>
+  </si>
+  <si>
+    <t>THILF02222</t>
+  </si>
+  <si>
+    <t>2025-06-07 09:06:13</t>
+  </si>
+  <si>
+    <t>2025-06-09 12:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 12:57:00</t>
+  </si>
+  <si>
+    <t>2025-06-10 13:00:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換下8155001634
+換上8155005449</t>
+  </si>
+  <si>
+    <t>13627114060701</t>
+  </si>
+  <si>
+    <t>三重重新橋</t>
+  </si>
+  <si>
+    <t>2025-06-07 11:56:21</t>
+  </si>
+  <si>
+    <t>門市反應MMK4代機畫面顯示乙太網路無法連線，未跳出網路設定介面視窗，請門市關機休息重啟仍異常，PING60不通...須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF03627</t>
+  </si>
+  <si>
+    <t>2025-06-07 11:58:13</t>
+  </si>
+  <si>
+    <t>2025-06-09 09:50:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 10:20:00</t>
+  </si>
+  <si>
+    <t>重新啟動檢查網路連線測試正常</t>
+  </si>
+  <si>
+    <t>14762114060901</t>
+  </si>
+  <si>
+    <t>新莊巷口店</t>
+  </si>
+  <si>
+    <t>2025-06-09 09:49:49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應MMK 四代機顯示尚未偵測到網路，無跳出偵測網路小視窗，已有關機休息重啟仍異常，PING60不通...請台芝到店協助	</t>
+  </si>
+  <si>
+    <t>THILF04762</t>
+  </si>
+  <si>
+    <t>2025-06-09 09:53:39</t>
+  </si>
+  <si>
+    <t>2025-06-09 11:25:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 11:55:00</t>
+  </si>
+  <si>
+    <t>2025-06-10 13:53:00</t>
+  </si>
+  <si>
+    <t>重設hub 重插網路線 偵測網路介面 設定正常</t>
+  </si>
+  <si>
+    <t>2025-06-09 11:17:02</t>
+  </si>
+  <si>
+    <t>2025-06-09 11:20:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 11:44:25</t>
+  </si>
+  <si>
+    <t>2025-06-09 11:42:00</t>
+  </si>
+  <si>
+    <t>Star</t>
+  </si>
+  <si>
+    <t>2025-06-09 13:00:58</t>
+  </si>
+  <si>
+    <t>2025-06-09 13:00:00</t>
+  </si>
+  <si>
+    <t>新莊鼎苑店</t>
+  </si>
+  <si>
+    <t>THILF04194</t>
+  </si>
+  <si>
+    <t>2025-06-09 13:43:19</t>
+  </si>
+  <si>
+    <t>2025-06-09 13:45:00</t>
   </si>
 </sst>
 </file>
@@ -1361,10 +1556,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK38"/>
+  <dimension ref="A1:AK47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC35" sqref="AC35"/>
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4533,7 +4728,7 @@
       <c r="M38" s="4"/>
       <c r="N38" s="3"/>
       <c r="O38" s="4"/>
-      <c r="P38" s="4"/>
+      <c r="P38" s="10"/>
       <c r="Q38" s="3" t="s">
         <v>296</v>
       </c>
@@ -4566,7 +4761,7 @@
       <c r="AB38" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC38" s="4" t="s">
+      <c r="AC38" s="10" t="s">
         <v>98</v>
       </c>
       <c r="AD38" s="3" t="s">
@@ -4581,6 +4776,805 @@
         <v>60</v>
       </c>
       <c r="AK38" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:37">
+      <c r="A39" s="7">
+        <v>37</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C39" s="7">
+        <v>2025061078</v>
+      </c>
+      <c r="D39" s="7" t="s">
+        <v>300</v>
+      </c>
+      <c r="E39" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F39" s="7">
+        <v>3840</v>
+      </c>
+      <c r="G39" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="H39" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I39" s="7" t="s">
+        <v>302</v>
+      </c>
+      <c r="J39" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K39" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L39" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="M39" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="N39" s="7" t="s">
+        <v>174</v>
+      </c>
+      <c r="O39" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="P39" s="9" t="s">
+        <v>303</v>
+      </c>
+      <c r="Q39" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="R39" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S39" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T39" s="7">
+        <v>1</v>
+      </c>
+      <c r="U39" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V39" s="7" t="s">
+        <v>305</v>
+      </c>
+      <c r="W39" s="7" t="s">
+        <v>306</v>
+      </c>
+      <c r="X39" s="7" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y39" s="7" t="s">
+        <v>308</v>
+      </c>
+      <c r="Z39" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA39" s="7"/>
+      <c r="AB39" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC39" s="9" t="s">
+        <v>309</v>
+      </c>
+      <c r="AD39" s="7"/>
+      <c r="AE39" s="7"/>
+      <c r="AF39" s="7"/>
+      <c r="AG39" s="7"/>
+      <c r="AH39" s="7"/>
+      <c r="AI39" s="7"/>
+      <c r="AJ39" s="7"/>
+      <c r="AK39" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:37">
+      <c r="A40" s="3">
+        <v>38</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C40" s="3">
+        <v>2025061140</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F40" s="3">
+        <v>3785</v>
+      </c>
+      <c r="G40" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="H40" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I40" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K40" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L40" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="M40" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="N40" s="3">
+        <v>5804</v>
+      </c>
+      <c r="O40" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P40" s="10" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q40" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="R40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S40" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T40" s="3">
+        <v>1</v>
+      </c>
+      <c r="U40" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V40" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="W40" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="X40" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="Y40" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="Z40" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA40" s="3"/>
+      <c r="AB40" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC40" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="AD40" s="3"/>
+      <c r="AE40" s="3"/>
+      <c r="AF40" s="3"/>
+      <c r="AG40" s="3"/>
+      <c r="AH40" s="3"/>
+      <c r="AI40" s="3"/>
+      <c r="AJ40" s="3"/>
+      <c r="AK40" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="41" spans="1:37">
+      <c r="A41" s="7">
+        <v>39</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C41" s="7">
+        <v>2025061180</v>
+      </c>
+      <c r="D41" s="7" t="s">
+        <v>322</v>
+      </c>
+      <c r="E41" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F41" s="7">
+        <v>2222</v>
+      </c>
+      <c r="G41" s="7" t="s">
+        <v>323</v>
+      </c>
+      <c r="H41" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I41" s="7" t="s">
+        <v>324</v>
+      </c>
+      <c r="J41" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M41" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="O41" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="P41" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>328</v>
+      </c>
+      <c r="R41" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S41" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T41" s="7">
+        <v>1</v>
+      </c>
+      <c r="U41" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V41" s="7" t="s">
+        <v>329</v>
+      </c>
+      <c r="W41" s="7" t="s">
+        <v>330</v>
+      </c>
+      <c r="X41" s="7" t="s">
+        <v>331</v>
+      </c>
+      <c r="Y41" s="7" t="s">
+        <v>332</v>
+      </c>
+      <c r="Z41" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA41" s="7"/>
+      <c r="AB41" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC41" s="9" t="s">
+        <v>333</v>
+      </c>
+      <c r="AD41" s="7"/>
+      <c r="AE41" s="7"/>
+      <c r="AF41" s="7"/>
+      <c r="AG41" s="7"/>
+      <c r="AH41" s="7"/>
+      <c r="AI41" s="7"/>
+      <c r="AJ41" s="7"/>
+      <c r="AK41" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="1:37">
+      <c r="A42" s="3">
+        <v>40</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C42" s="3">
+        <v>2025061184</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F42" s="3">
+        <v>3627</v>
+      </c>
+      <c r="G42" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="H42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I42" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="J42" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K42" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L42" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="M42" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="N42" s="3">
+        <v>5804</v>
+      </c>
+      <c r="O42" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P42" s="10" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q42" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="R42" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S42" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T42" s="3">
+        <v>1</v>
+      </c>
+      <c r="U42" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V42" s="3" t="s">
+        <v>339</v>
+      </c>
+      <c r="W42" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="X42" s="3" t="s">
+        <v>341</v>
+      </c>
+      <c r="Y42" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="Z42" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA42" s="3"/>
+      <c r="AB42" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC42" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="AD42" s="3"/>
+      <c r="AE42" s="3"/>
+      <c r="AF42" s="3"/>
+      <c r="AG42" s="3"/>
+      <c r="AH42" s="3"/>
+      <c r="AI42" s="3"/>
+      <c r="AJ42" s="3"/>
+      <c r="AK42" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="43" spans="1:37">
+      <c r="A43" s="7">
+        <v>41</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C43" s="7">
+        <v>2025061207</v>
+      </c>
+      <c r="D43" s="7" t="s">
+        <v>343</v>
+      </c>
+      <c r="E43" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F43" s="7">
+        <v>4762</v>
+      </c>
+      <c r="G43" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="H43" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I43" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="J43" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="K43" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L43" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="M43" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="N43" s="7">
+        <v>5804</v>
+      </c>
+      <c r="O43" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="P43" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="Q43" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="R43" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S43" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T43" s="7">
+        <v>1</v>
+      </c>
+      <c r="U43" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V43" s="7" t="s">
+        <v>348</v>
+      </c>
+      <c r="W43" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="X43" s="7" t="s">
+        <v>350</v>
+      </c>
+      <c r="Y43" s="7" t="s">
+        <v>351</v>
+      </c>
+      <c r="Z43" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA43" s="7"/>
+      <c r="AB43" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC43" s="9" t="s">
+        <v>352</v>
+      </c>
+      <c r="AD43" s="7"/>
+      <c r="AE43" s="7"/>
+      <c r="AF43" s="7"/>
+      <c r="AG43" s="7"/>
+      <c r="AH43" s="7"/>
+      <c r="AI43" s="7"/>
+      <c r="AJ43" s="7"/>
+      <c r="AK43" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="44" spans="1:37">
+      <c r="A44" s="3">
+        <v>42</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2025061246</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3">
+        <v>3785</v>
+      </c>
+      <c r="G44" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="H44" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="K44" s="3"/>
+      <c r="L44" s="3"/>
+      <c r="M44" s="4"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="4"/>
+      <c r="P44" s="10"/>
+      <c r="Q44" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="R44" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S44" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T44" s="3">
+        <v>1</v>
+      </c>
+      <c r="U44" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V44" s="3" t="s">
+        <v>353</v>
+      </c>
+      <c r="W44" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="X44" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="Y44" s="3"/>
+      <c r="Z44" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA44" s="3"/>
+      <c r="AB44" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC44" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE44" s="3"/>
+      <c r="AF44" s="3"/>
+      <c r="AG44" s="3"/>
+      <c r="AH44" s="3"/>
+      <c r="AI44" s="3"/>
+      <c r="AJ44" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK44" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="45" spans="1:37">
+      <c r="A45" s="7">
+        <v>43</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="7">
+        <v>2025061255</v>
+      </c>
+      <c r="D45" s="7"/>
+      <c r="E45" s="7"/>
+      <c r="F45" s="7">
+        <v>3840</v>
+      </c>
+      <c r="G45" s="7" t="s">
+        <v>301</v>
+      </c>
+      <c r="H45" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I45" s="7"/>
+      <c r="J45" s="7"/>
+      <c r="K45" s="7"/>
+      <c r="L45" s="7"/>
+      <c r="M45" s="8"/>
+      <c r="N45" s="7"/>
+      <c r="O45" s="8"/>
+      <c r="P45" s="9"/>
+      <c r="Q45" s="7" t="s">
+        <v>304</v>
+      </c>
+      <c r="R45" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S45" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T45" s="7">
+        <v>1</v>
+      </c>
+      <c r="U45" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V45" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="W45" s="7" t="s">
+        <v>319</v>
+      </c>
+      <c r="X45" s="7" t="s">
+        <v>356</v>
+      </c>
+      <c r="Y45" s="7"/>
+      <c r="Z45" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA45" s="7"/>
+      <c r="AB45" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC45" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="AD45" s="7"/>
+      <c r="AE45" s="7"/>
+      <c r="AF45" s="7"/>
+      <c r="AG45" s="7"/>
+      <c r="AH45" s="7"/>
+      <c r="AI45" s="7"/>
+      <c r="AJ45" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK45" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="1:37">
+      <c r="A46" s="3">
+        <v>44</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2025061263</v>
+      </c>
+      <c r="D46" s="3"/>
+      <c r="E46" s="3"/>
+      <c r="F46" s="3">
+        <v>2222</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I46" s="3"/>
+      <c r="J46" s="3"/>
+      <c r="K46" s="3"/>
+      <c r="L46" s="3"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="3"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="10"/>
+      <c r="Q46" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="R46" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S46" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T46" s="3">
+        <v>1</v>
+      </c>
+      <c r="U46" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V46" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="W46" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="X46" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="Y46" s="3"/>
+      <c r="Z46" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA46" s="3"/>
+      <c r="AB46" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC46" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE46" s="3"/>
+      <c r="AF46" s="3"/>
+      <c r="AG46" s="3"/>
+      <c r="AH46" s="3"/>
+      <c r="AI46" s="3"/>
+      <c r="AJ46" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK46" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="47" spans="1:37">
+      <c r="A47" s="7">
+        <v>45</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C47" s="7">
+        <v>2025061274</v>
+      </c>
+      <c r="D47" s="7"/>
+      <c r="E47" s="7"/>
+      <c r="F47" s="7">
+        <v>4194</v>
+      </c>
+      <c r="G47" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="H47" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I47" s="7"/>
+      <c r="J47" s="7"/>
+      <c r="K47" s="7"/>
+      <c r="L47" s="7"/>
+      <c r="M47" s="8"/>
+      <c r="N47" s="7"/>
+      <c r="O47" s="8"/>
+      <c r="P47" s="8"/>
+      <c r="Q47" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="R47" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S47" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T47" s="7">
+        <v>1</v>
+      </c>
+      <c r="U47" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V47" s="7" t="s">
+        <v>362</v>
+      </c>
+      <c r="W47" s="7" t="s">
+        <v>359</v>
+      </c>
+      <c r="X47" s="7" t="s">
+        <v>363</v>
+      </c>
+      <c r="Y47" s="7"/>
+      <c r="Z47" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA47" s="7"/>
+      <c r="AB47" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC47" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD47" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE47" s="7"/>
+      <c r="AF47" s="7"/>
+      <c r="AG47" s="7"/>
+      <c r="AH47" s="7"/>
+      <c r="AI47" s="7"/>
+      <c r="AJ47" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK47" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 09-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$47</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$49</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="364">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="373">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-09  )</t>
   </si>
@@ -1143,6 +1143,33 @@
   </si>
   <si>
     <t>2025-06-09 13:45:00</t>
+  </si>
+  <si>
+    <t>新莊頭前店</t>
+  </si>
+  <si>
+    <t>THILF04144</t>
+  </si>
+  <si>
+    <t>2025-06-09 14:40:10</t>
+  </si>
+  <si>
+    <t>2025-06-09 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 14:45:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 14:53:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 14:36:00</t>
+  </si>
+  <si>
+    <t>2025-06-09 14:51:00</t>
+  </si>
+  <si>
+    <t>測試交易發票照片（補）</t>
   </si>
 </sst>
 </file>
@@ -1556,10 +1583,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK47"/>
+  <dimension ref="A1:AK49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A47" sqref="A47"/>
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5527,7 +5554,7 @@
       <c r="M47" s="8"/>
       <c r="N47" s="7"/>
       <c r="O47" s="8"/>
-      <c r="P47" s="8"/>
+      <c r="P47" s="9"/>
       <c r="Q47" s="7" t="s">
         <v>361</v>
       </c>
@@ -5560,7 +5587,7 @@
       <c r="AB47" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC47" s="8" t="s">
+      <c r="AC47" s="9" t="s">
         <v>98</v>
       </c>
       <c r="AD47" s="7" t="s">
@@ -5575,6 +5602,164 @@
         <v>60</v>
       </c>
       <c r="AK47" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="48" spans="1:37">
+      <c r="A48" s="3">
+        <v>46</v>
+      </c>
+      <c r="B48" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C48" s="3">
+        <v>2025061283</v>
+      </c>
+      <c r="D48" s="3"/>
+      <c r="E48" s="3"/>
+      <c r="F48" s="3">
+        <v>4144</v>
+      </c>
+      <c r="G48" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="H48" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I48" s="3"/>
+      <c r="J48" s="3"/>
+      <c r="K48" s="3"/>
+      <c r="L48" s="3"/>
+      <c r="M48" s="4"/>
+      <c r="N48" s="3"/>
+      <c r="O48" s="4"/>
+      <c r="P48" s="10"/>
+      <c r="Q48" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="R48" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S48" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T48" s="3">
+        <v>1</v>
+      </c>
+      <c r="U48" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V48" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="W48" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="X48" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="Y48" s="3"/>
+      <c r="Z48" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA48" s="3"/>
+      <c r="AB48" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC48" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD48" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE48" s="3"/>
+      <c r="AF48" s="3"/>
+      <c r="AG48" s="3"/>
+      <c r="AH48" s="3"/>
+      <c r="AI48" s="3"/>
+      <c r="AJ48" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK48" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="49" spans="1:37">
+      <c r="A49" s="7">
+        <v>47</v>
+      </c>
+      <c r="B49" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C49" s="7">
+        <v>2025061289</v>
+      </c>
+      <c r="D49" s="7"/>
+      <c r="E49" s="7"/>
+      <c r="F49" s="7">
+        <v>4194</v>
+      </c>
+      <c r="G49" s="7" t="s">
+        <v>360</v>
+      </c>
+      <c r="H49" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I49" s="7"/>
+      <c r="J49" s="7"/>
+      <c r="K49" s="7"/>
+      <c r="L49" s="7"/>
+      <c r="M49" s="8"/>
+      <c r="N49" s="7"/>
+      <c r="O49" s="8"/>
+      <c r="P49" s="8"/>
+      <c r="Q49" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="R49" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S49" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T49" s="7">
+        <v>1</v>
+      </c>
+      <c r="U49" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V49" s="7" t="s">
+        <v>369</v>
+      </c>
+      <c r="W49" s="7" t="s">
+        <v>370</v>
+      </c>
+      <c r="X49" s="7" t="s">
+        <v>371</v>
+      </c>
+      <c r="Y49" s="7"/>
+      <c r="Z49" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA49" s="7"/>
+      <c r="AB49" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC49" s="8" t="s">
+        <v>372</v>
+      </c>
+      <c r="AD49" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE49" s="7"/>
+      <c r="AF49" s="7"/>
+      <c r="AG49" s="7"/>
+      <c r="AH49" s="7"/>
+      <c r="AI49" s="7"/>
+      <c r="AJ49" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK49" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 10-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,14 +11,14 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$49</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$54</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="373">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="411">
   <si>
     <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-10  )</t>
   </si>
@@ -1082,6 +1082,33 @@
     <t>重新啟動檢查網路連線測試正常</t>
   </si>
   <si>
+    <t>13890114060702</t>
+  </si>
+  <si>
+    <t>三重美堤店</t>
+  </si>
+  <si>
+    <t>2025-06-07 12:26:39</t>
+  </si>
+  <si>
+    <t>門市反應近期TM2(TCX800)螢幕鼠標會不定期發生飄移異狀，已確認當下TM未張貼文宣、透明塑膠墊，當下重啟後會正常，但不久後又會再度發生，尤其今日需重啟高達10次才正常，5/30客服已協助執行觸控校正仍無改善，需請台芝到店協助檢查 ※非24H營業門市，周一公休，營業時間:周二至周日0600~1500</t>
+  </si>
+  <si>
+    <t>THILF03890</t>
+  </si>
+  <si>
+    <t>2025-06-07 12:31:37</t>
+  </si>
+  <si>
+    <t>2025-06-10 10:25:00</t>
+  </si>
+  <si>
+    <t>2025-06-10 10:55:00</t>
+  </si>
+  <si>
+    <t>重新矯正螢幕，目前測試正常，請店員觀察狀況</t>
+  </si>
+  <si>
     <t>14762114060901</t>
   </si>
   <si>
@@ -1133,6 +1160,32 @@
     <t>2025-06-09 13:00:00</t>
   </si>
   <si>
+    <t>13840114060901</t>
+  </si>
+  <si>
+    <t>2025-06-09 13:24:15</t>
+  </si>
+  <si>
+    <t>門市反應TM2多卡機(QP3000E)悠遊卡、一卡通、愛金卡皆無法使用,已有協助版更後點選悠遊卡重開TM顯示通訊逾時、一卡通重開顯示0801 錯誤訊息、愛金卡點選手動開機授權顯示卡片回應資料長度錯誤.......請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-06-09 13:28:42</t>
+  </si>
+  <si>
+    <t>2025-06-10 11:24:00</t>
+  </si>
+  <si>
+    <t>2025-06-10 11:54:00</t>
+  </si>
+  <si>
+    <t>2025-06-10 17:28:00</t>
+  </si>
+  <si>
+    <t>更換多卡機QP3000
+換下8183000512
+換上8183003484</t>
+  </si>
+  <si>
     <t>新莊鼎苑店</t>
   </si>
   <si>
@@ -1145,6 +1198,39 @@
     <t>2025-06-09 13:45:00</t>
   </si>
   <si>
+    <t>12209114060901</t>
+  </si>
+  <si>
+    <t>北縣重強店</t>
+  </si>
+  <si>
+    <t>2025-06-09 14:14:26</t>
+  </si>
+  <si>
+    <t>鍵盤按鍵不良或無反應</t>
+  </si>
+  <si>
+    <t>門市反應sc鍵盤右邊的數字鍵0很難按以及英文C鍵按無反應，已嘗試重新拔插後方線路+簡易清潔仍異常..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF02209</t>
+  </si>
+  <si>
+    <t>2025-06-09 14:15:53</t>
+  </si>
+  <si>
+    <t>2025-06-10 12:20:00</t>
+  </si>
+  <si>
+    <t>2025-06-10 12:50:00</t>
+  </si>
+  <si>
+    <t>2025-06-10 18:15:00</t>
+  </si>
+  <si>
+    <t>更換鍵盤</t>
+  </si>
+  <si>
     <t>新莊頭前店</t>
   </si>
   <si>
@@ -1170,6 +1256,36 @@
   </si>
   <si>
     <t>測試交易發票照片（補）</t>
+  </si>
+  <si>
+    <t>三重圖書館</t>
+  </si>
+  <si>
+    <t>2025-06-10 12:59:14</t>
+  </si>
+  <si>
+    <t>2025-06-10 12:10:00</t>
+  </si>
+  <si>
+    <t>2025-06-10 12:58:00</t>
+  </si>
+  <si>
+    <t>林口舊街店</t>
+  </si>
+  <si>
+    <t>THILF05364</t>
+  </si>
+  <si>
+    <t>2025-06-10 13:53:51</t>
+  </si>
+  <si>
+    <t>2025-06-10 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-10 13:30:00</t>
+  </si>
+  <si>
+    <t>新開門市</t>
   </si>
 </sst>
 </file>
@@ -1583,10 +1699,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK49"/>
+  <dimension ref="A1:AK54"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A49" sqref="A49"/>
+      <selection activeCell="AC51" sqref="AC51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5202,7 +5318,7 @@
         <v>38</v>
       </c>
       <c r="C43" s="7">
-        <v>2025061207</v>
+        <v>2025061187</v>
       </c>
       <c r="D43" s="7" t="s">
         <v>343</v>
@@ -5211,34 +5327,34 @@
         <v>40</v>
       </c>
       <c r="F43" s="7">
-        <v>4762</v>
+        <v>3890</v>
       </c>
       <c r="G43" s="7" t="s">
         <v>344</v>
       </c>
       <c r="H43" s="7" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="I43" s="7" t="s">
         <v>345</v>
       </c>
       <c r="J43" s="7" t="s">
-        <v>111</v>
+        <v>325</v>
       </c>
       <c r="K43" s="7" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="L43" s="7" t="s">
-        <v>313</v>
+        <v>112</v>
       </c>
       <c r="M43" s="8" t="s">
-        <v>314</v>
+        <v>113</v>
       </c>
       <c r="N43" s="7">
-        <v>5804</v>
+        <v>2307</v>
       </c>
       <c r="O43" s="8" t="s">
-        <v>175</v>
+        <v>199</v>
       </c>
       <c r="P43" s="9" t="s">
         <v>346</v>
@@ -5250,7 +5366,7 @@
         <v>51</v>
       </c>
       <c r="S43" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="T43" s="7">
         <v>1</v>
@@ -5268,7 +5384,7 @@
         <v>350</v>
       </c>
       <c r="Y43" s="7" t="s">
-        <v>351</v>
+        <v>332</v>
       </c>
       <c r="Z43" s="7">
         <v>0.5</v>
@@ -5278,7 +5394,7 @@
         <v>58</v>
       </c>
       <c r="AC43" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AD43" s="7"/>
       <c r="AE43" s="7"/>
@@ -5296,32 +5412,52 @@
         <v>42</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C44" s="3">
-        <v>2025061246</v>
-      </c>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
+        <v>2025061207</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F44" s="3">
-        <v>3785</v>
+        <v>4762</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>311</v>
+        <v>353</v>
       </c>
       <c r="H44" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="4"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="4"/>
-      <c r="P44" s="10"/>
+      <c r="I44" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K44" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L44" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="M44" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="N44" s="3">
+        <v>5804</v>
+      </c>
+      <c r="O44" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P44" s="10" t="s">
+        <v>355</v>
+      </c>
       <c r="Q44" s="3" t="s">
-        <v>316</v>
+        <v>356</v>
       </c>
       <c r="R44" s="3" t="s">
         <v>51</v>
@@ -5336,36 +5472,34 @@
         <v>53</v>
       </c>
       <c r="V44" s="3" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="W44" s="3" t="s">
-        <v>319</v>
+        <v>358</v>
       </c>
       <c r="X44" s="3" t="s">
-        <v>354</v>
-      </c>
-      <c r="Y44" s="3"/>
+        <v>359</v>
+      </c>
+      <c r="Y44" s="3" t="s">
+        <v>360</v>
+      </c>
       <c r="Z44" s="3">
-        <v>0.3</v>
+        <v>0.5</v>
       </c>
       <c r="AA44" s="3"/>
       <c r="AB44" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC44" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="AD44" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>361</v>
+      </c>
+      <c r="AD44" s="3"/>
       <c r="AE44" s="3"/>
       <c r="AF44" s="3"/>
       <c r="AG44" s="3"/>
       <c r="AH44" s="3"/>
       <c r="AI44" s="3"/>
-      <c r="AJ44" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ44" s="3"/>
       <c r="AK44" s="3" t="s">
         <v>60</v>
       </c>
@@ -5378,18 +5512,18 @@
         <v>94</v>
       </c>
       <c r="C45" s="7">
-        <v>2025061255</v>
+        <v>2025061246</v>
       </c>
       <c r="D45" s="7"/>
       <c r="E45" s="7"/>
       <c r="F45" s="7">
-        <v>3840</v>
+        <v>3785</v>
       </c>
       <c r="G45" s="7" t="s">
-        <v>301</v>
+        <v>311</v>
       </c>
       <c r="H45" s="7" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="I45" s="7"/>
       <c r="J45" s="7"/>
@@ -5400,13 +5534,13 @@
       <c r="O45" s="8"/>
       <c r="P45" s="9"/>
       <c r="Q45" s="7" t="s">
-        <v>304</v>
+        <v>316</v>
       </c>
       <c r="R45" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S45" s="7" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="T45" s="7">
         <v>1</v>
@@ -5415,26 +5549,28 @@
         <v>53</v>
       </c>
       <c r="V45" s="7" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="W45" s="7" t="s">
         <v>319</v>
       </c>
       <c r="X45" s="7" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="Y45" s="7"/>
       <c r="Z45" s="7">
-        <v>0.7</v>
+        <v>0.3</v>
       </c>
       <c r="AA45" s="7"/>
       <c r="AB45" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC45" s="9" t="s">
-        <v>357</v>
-      </c>
-      <c r="AD45" s="7"/>
+        <v>129</v>
+      </c>
+      <c r="AD45" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AE45" s="7"/>
       <c r="AF45" s="7"/>
       <c r="AG45" s="7"/>
@@ -5455,15 +5591,15 @@
         <v>94</v>
       </c>
       <c r="C46" s="3">
-        <v>2025061263</v>
+        <v>2025061255</v>
       </c>
       <c r="D46" s="3"/>
       <c r="E46" s="3"/>
       <c r="F46" s="3">
-        <v>2222</v>
+        <v>3840</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>323</v>
+        <v>301</v>
       </c>
       <c r="H46" s="3" t="s">
         <v>42</v>
@@ -5477,7 +5613,7 @@
       <c r="O46" s="4"/>
       <c r="P46" s="10"/>
       <c r="Q46" s="3" t="s">
-        <v>328</v>
+        <v>304</v>
       </c>
       <c r="R46" s="3" t="s">
         <v>51</v>
@@ -5492,28 +5628,26 @@
         <v>53</v>
       </c>
       <c r="V46" s="3" t="s">
-        <v>358</v>
+        <v>364</v>
       </c>
       <c r="W46" s="3" t="s">
-        <v>330</v>
+        <v>319</v>
       </c>
       <c r="X46" s="3" t="s">
-        <v>359</v>
+        <v>365</v>
       </c>
       <c r="Y46" s="3"/>
       <c r="Z46" s="3">
-        <v>1</v>
+        <v>0.7</v>
       </c>
       <c r="AA46" s="3"/>
       <c r="AB46" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC46" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD46" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>366</v>
+      </c>
+      <c r="AD46" s="3"/>
       <c r="AE46" s="3"/>
       <c r="AF46" s="3"/>
       <c r="AG46" s="3"/>
@@ -5534,18 +5668,18 @@
         <v>94</v>
       </c>
       <c r="C47" s="7">
-        <v>2025061274</v>
+        <v>2025061263</v>
       </c>
       <c r="D47" s="7"/>
       <c r="E47" s="7"/>
       <c r="F47" s="7">
-        <v>4194</v>
+        <v>2222</v>
       </c>
       <c r="G47" s="7" t="s">
-        <v>360</v>
+        <v>323</v>
       </c>
       <c r="H47" s="7" t="s">
-        <v>63</v>
+        <v>42</v>
       </c>
       <c r="I47" s="7"/>
       <c r="J47" s="7"/>
@@ -5556,13 +5690,13 @@
       <c r="O47" s="8"/>
       <c r="P47" s="9"/>
       <c r="Q47" s="7" t="s">
-        <v>361</v>
+        <v>328</v>
       </c>
       <c r="R47" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S47" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="T47" s="7">
         <v>1</v>
@@ -5571,17 +5705,17 @@
         <v>53</v>
       </c>
       <c r="V47" s="7" t="s">
-        <v>362</v>
+        <v>367</v>
       </c>
       <c r="W47" s="7" t="s">
-        <v>359</v>
+        <v>330</v>
       </c>
       <c r="X47" s="7" t="s">
-        <v>363</v>
+        <v>368</v>
       </c>
       <c r="Y47" s="7"/>
       <c r="Z47" s="7">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="AA47" s="7"/>
       <c r="AB47" s="7" t="s">
@@ -5610,38 +5744,58 @@
         <v>46</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C48" s="3">
-        <v>2025061283</v>
-      </c>
-      <c r="D48" s="3"/>
-      <c r="E48" s="3"/>
+        <v>2025061272</v>
+      </c>
+      <c r="D48" s="3" t="s">
+        <v>369</v>
+      </c>
+      <c r="E48" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F48" s="3">
-        <v>4144</v>
+        <v>3840</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>364</v>
+        <v>301</v>
       </c>
       <c r="H48" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I48" s="3"/>
-      <c r="J48" s="3"/>
-      <c r="K48" s="3"/>
-      <c r="L48" s="3"/>
-      <c r="M48" s="4"/>
-      <c r="N48" s="3"/>
-      <c r="O48" s="4"/>
-      <c r="P48" s="10"/>
+        <v>42</v>
+      </c>
+      <c r="I48" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K48" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L48" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M48" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="N48" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="O48" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P48" s="10" t="s">
+        <v>371</v>
+      </c>
       <c r="Q48" s="3" t="s">
-        <v>365</v>
+        <v>304</v>
       </c>
       <c r="R48" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S48" s="3" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="T48" s="3">
         <v>1</v>
@@ -5650,36 +5804,34 @@
         <v>53</v>
       </c>
       <c r="V48" s="3" t="s">
-        <v>366</v>
+        <v>372</v>
       </c>
       <c r="W48" s="3" t="s">
-        <v>367</v>
+        <v>373</v>
       </c>
       <c r="X48" s="3" t="s">
-        <v>368</v>
-      </c>
-      <c r="Y48" s="3"/>
+        <v>374</v>
+      </c>
+      <c r="Y48" s="3" t="s">
+        <v>375</v>
+      </c>
       <c r="Z48" s="3">
-        <v>0.8</v>
+        <v>0.5</v>
       </c>
       <c r="AA48" s="3"/>
       <c r="AB48" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC48" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD48" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>376</v>
+      </c>
+      <c r="AD48" s="3"/>
       <c r="AE48" s="3"/>
       <c r="AF48" s="3"/>
       <c r="AG48" s="3"/>
       <c r="AH48" s="3"/>
       <c r="AI48" s="3"/>
-      <c r="AJ48" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ48" s="3"/>
       <c r="AK48" s="3" t="s">
         <v>60</v>
       </c>
@@ -5692,7 +5844,7 @@
         <v>94</v>
       </c>
       <c r="C49" s="7">
-        <v>2025061289</v>
+        <v>2025061274</v>
       </c>
       <c r="D49" s="7"/>
       <c r="E49" s="7"/>
@@ -5700,7 +5852,7 @@
         <v>4194</v>
       </c>
       <c r="G49" s="7" t="s">
-        <v>360</v>
+        <v>377</v>
       </c>
       <c r="H49" s="7" t="s">
         <v>63</v>
@@ -5712,9 +5864,9 @@
       <c r="M49" s="8"/>
       <c r="N49" s="7"/>
       <c r="O49" s="8"/>
-      <c r="P49" s="8"/>
+      <c r="P49" s="9"/>
       <c r="Q49" s="7" t="s">
-        <v>361</v>
+        <v>378</v>
       </c>
       <c r="R49" s="7" t="s">
         <v>51</v>
@@ -5729,24 +5881,24 @@
         <v>53</v>
       </c>
       <c r="V49" s="7" t="s">
-        <v>369</v>
+        <v>379</v>
       </c>
       <c r="W49" s="7" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="X49" s="7" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
       <c r="Y49" s="7"/>
       <c r="Z49" s="7">
-        <v>0.3</v>
+        <v>0.8</v>
       </c>
       <c r="AA49" s="7"/>
       <c r="AB49" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC49" s="8" t="s">
-        <v>372</v>
+      <c r="AC49" s="9" t="s">
+        <v>98</v>
       </c>
       <c r="AD49" s="7" t="s">
         <v>60</v>
@@ -5760,6 +5912,415 @@
         <v>60</v>
       </c>
       <c r="AK49" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="50" spans="1:37">
+      <c r="A50" s="3">
+        <v>48</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="3">
+        <v>2025061276</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>381</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50" s="3">
+        <v>2209</v>
+      </c>
+      <c r="G50" s="3" t="s">
+        <v>382</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I50" s="3" t="s">
+        <v>383</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K50" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L50" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="M50" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="N50" s="3">
+        <v>2402</v>
+      </c>
+      <c r="O50" s="4" t="s">
+        <v>384</v>
+      </c>
+      <c r="P50" s="10" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q50" s="3" t="s">
+        <v>386</v>
+      </c>
+      <c r="R50" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S50" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T50" s="3">
+        <v>1</v>
+      </c>
+      <c r="U50" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V50" s="3" t="s">
+        <v>387</v>
+      </c>
+      <c r="W50" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="X50" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="Y50" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="Z50" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA50" s="3"/>
+      <c r="AB50" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC50" s="10" t="s">
+        <v>391</v>
+      </c>
+      <c r="AD50" s="3"/>
+      <c r="AE50" s="3"/>
+      <c r="AF50" s="3"/>
+      <c r="AG50" s="3"/>
+      <c r="AH50" s="3"/>
+      <c r="AI50" s="3"/>
+      <c r="AJ50" s="3"/>
+      <c r="AK50" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="51" spans="1:37">
+      <c r="A51" s="7">
+        <v>49</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C51" s="7">
+        <v>2025061283</v>
+      </c>
+      <c r="D51" s="7"/>
+      <c r="E51" s="7"/>
+      <c r="F51" s="7">
+        <v>4144</v>
+      </c>
+      <c r="G51" s="7" t="s">
+        <v>392</v>
+      </c>
+      <c r="H51" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I51" s="7"/>
+      <c r="J51" s="7"/>
+      <c r="K51" s="7"/>
+      <c r="L51" s="7"/>
+      <c r="M51" s="8"/>
+      <c r="N51" s="7"/>
+      <c r="O51" s="8"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="7" t="s">
+        <v>393</v>
+      </c>
+      <c r="R51" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S51" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T51" s="7">
+        <v>1</v>
+      </c>
+      <c r="U51" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V51" s="7" t="s">
+        <v>394</v>
+      </c>
+      <c r="W51" s="7" t="s">
+        <v>395</v>
+      </c>
+      <c r="X51" s="7" t="s">
+        <v>396</v>
+      </c>
+      <c r="Y51" s="7"/>
+      <c r="Z51" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA51" s="7"/>
+      <c r="AB51" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC51" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD51" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE51" s="7"/>
+      <c r="AF51" s="7"/>
+      <c r="AG51" s="7"/>
+      <c r="AH51" s="7"/>
+      <c r="AI51" s="7"/>
+      <c r="AJ51" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK51" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="52" spans="1:37">
+      <c r="A52" s="3">
+        <v>50</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C52" s="3">
+        <v>2025061289</v>
+      </c>
+      <c r="D52" s="3"/>
+      <c r="E52" s="3"/>
+      <c r="F52" s="3">
+        <v>4194</v>
+      </c>
+      <c r="G52" s="3" t="s">
+        <v>377</v>
+      </c>
+      <c r="H52" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I52" s="3"/>
+      <c r="J52" s="3"/>
+      <c r="K52" s="3"/>
+      <c r="L52" s="3"/>
+      <c r="M52" s="4"/>
+      <c r="N52" s="3"/>
+      <c r="O52" s="4"/>
+      <c r="P52" s="10"/>
+      <c r="Q52" s="3" t="s">
+        <v>378</v>
+      </c>
+      <c r="R52" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S52" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T52" s="3">
+        <v>1</v>
+      </c>
+      <c r="U52" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V52" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="W52" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="X52" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="Y52" s="3"/>
+      <c r="Z52" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA52" s="3"/>
+      <c r="AB52" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC52" s="10" t="s">
+        <v>400</v>
+      </c>
+      <c r="AD52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE52" s="3"/>
+      <c r="AF52" s="3"/>
+      <c r="AG52" s="3"/>
+      <c r="AH52" s="3"/>
+      <c r="AI52" s="3"/>
+      <c r="AJ52" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK52" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="53" spans="1:37">
+      <c r="A53" s="7">
+        <v>51</v>
+      </c>
+      <c r="B53" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C53" s="7">
+        <v>2025061477</v>
+      </c>
+      <c r="D53" s="7"/>
+      <c r="E53" s="7"/>
+      <c r="F53" s="7">
+        <v>2209</v>
+      </c>
+      <c r="G53" s="7" t="s">
+        <v>401</v>
+      </c>
+      <c r="H53" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I53" s="7"/>
+      <c r="J53" s="7"/>
+      <c r="K53" s="7"/>
+      <c r="L53" s="7"/>
+      <c r="M53" s="8"/>
+      <c r="N53" s="7"/>
+      <c r="O53" s="8"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="7" t="s">
+        <v>386</v>
+      </c>
+      <c r="R53" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S53" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T53" s="7">
+        <v>1</v>
+      </c>
+      <c r="U53" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V53" s="7" t="s">
+        <v>402</v>
+      </c>
+      <c r="W53" s="7" t="s">
+        <v>403</v>
+      </c>
+      <c r="X53" s="7" t="s">
+        <v>404</v>
+      </c>
+      <c r="Y53" s="7"/>
+      <c r="Z53" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA53" s="7"/>
+      <c r="AB53" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC53" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="AD53" s="7"/>
+      <c r="AE53" s="7"/>
+      <c r="AF53" s="7"/>
+      <c r="AG53" s="7"/>
+      <c r="AH53" s="7"/>
+      <c r="AI53" s="7"/>
+      <c r="AJ53" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK53" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="54" spans="1:37">
+      <c r="A54" s="3">
+        <v>52</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C54" s="3">
+        <v>2025061496</v>
+      </c>
+      <c r="D54" s="3"/>
+      <c r="E54" s="3"/>
+      <c r="F54" s="3">
+        <v>5364</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="I54" s="3"/>
+      <c r="J54" s="3"/>
+      <c r="K54" s="3"/>
+      <c r="L54" s="3"/>
+      <c r="M54" s="4"/>
+      <c r="N54" s="3"/>
+      <c r="O54" s="4"/>
+      <c r="P54" s="4"/>
+      <c r="Q54" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="R54" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S54" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T54" s="3">
+        <v>1</v>
+      </c>
+      <c r="U54" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V54" s="3" t="s">
+        <v>407</v>
+      </c>
+      <c r="W54" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="X54" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="Y54" s="3"/>
+      <c r="Z54" s="3">
+        <v>3.5</v>
+      </c>
+      <c r="AA54" s="3"/>
+      <c r="AB54" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC54" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD54" s="3"/>
+      <c r="AE54" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF54" s="3"/>
+      <c r="AG54" s="3"/>
+      <c r="AH54" s="3"/>
+      <c r="AI54" s="3"/>
+      <c r="AJ54" s="3"/>
+      <c r="AK54" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 11-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$54</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$60</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="411">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-10  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="442">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-11  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1286,6 +1286,99 @@
   </si>
   <si>
     <t>新開門市</t>
+  </si>
+  <si>
+    <t>林口麗園店</t>
+  </si>
+  <si>
+    <t>THILF04154</t>
+  </si>
+  <si>
+    <t>2025-06-11 10:37:11</t>
+  </si>
+  <si>
+    <t>2025-06-11 10:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-11 10:40:00</t>
+  </si>
+  <si>
+    <t>北縣醒吾店</t>
+  </si>
+  <si>
+    <t>THILF03243</t>
+  </si>
+  <si>
+    <t>2025-06-11 11:28:56</t>
+  </si>
+  <si>
+    <t>2025-06-11 10:50:00</t>
+  </si>
+  <si>
+    <t>2025-06-11 11:30:00</t>
+  </si>
+  <si>
+    <t>STAR</t>
+  </si>
+  <si>
+    <t>三重進安店</t>
+  </si>
+  <si>
+    <t>THILF03796</t>
+  </si>
+  <si>
+    <t>2025-06-11 12:01:06</t>
+  </si>
+  <si>
+    <t>2025-06-11 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-11 12:00:00</t>
+  </si>
+  <si>
+    <t>D609</t>
+  </si>
+  <si>
+    <t>板橋大興店</t>
+  </si>
+  <si>
+    <t>THILF0D609</t>
+  </si>
+  <si>
+    <t>2025-06-11 12:41:00</t>
+  </si>
+  <si>
+    <t>2025-06-11 12:38:00</t>
+  </si>
+  <si>
+    <t>三重碧華公園</t>
+  </si>
+  <si>
+    <t>THILF03811</t>
+  </si>
+  <si>
+    <t>2025-06-11 13:09:44</t>
+  </si>
+  <si>
+    <t>2025-06-11 12:10:00</t>
+  </si>
+  <si>
+    <t>2025-06-11 13:09:00</t>
+  </si>
+  <si>
+    <t>板橋合安店</t>
+  </si>
+  <si>
+    <t>THILF04422</t>
+  </si>
+  <si>
+    <t>2025-06-11 13:16:35</t>
+  </si>
+  <si>
+    <t>2025-06-11 12:55:00</t>
+  </si>
+  <si>
+    <t>2025-06-11 13:15:00</t>
   </si>
 </sst>
 </file>
@@ -1699,10 +1792,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK54"/>
+  <dimension ref="A1:AK60"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC51" sqref="AC51"/>
+      <selection activeCell="AC57" sqref="AC57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6275,7 +6368,7 @@
       <c r="M54" s="4"/>
       <c r="N54" s="3"/>
       <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
+      <c r="P54" s="10"/>
       <c r="Q54" s="3" t="s">
         <v>406</v>
       </c>
@@ -6308,7 +6401,7 @@
       <c r="AB54" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC54" s="4" t="s">
+      <c r="AC54" s="10" t="s">
         <v>410</v>
       </c>
       <c r="AD54" s="3"/>
@@ -6321,6 +6414,478 @@
       <c r="AI54" s="3"/>
       <c r="AJ54" s="3"/>
       <c r="AK54" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="55" spans="1:37">
+      <c r="A55" s="7">
+        <v>53</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C55" s="7">
+        <v>2025061656</v>
+      </c>
+      <c r="D55" s="7"/>
+      <c r="E55" s="7"/>
+      <c r="F55" s="7">
+        <v>4154</v>
+      </c>
+      <c r="G55" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="H55" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="I55" s="7"/>
+      <c r="J55" s="7"/>
+      <c r="K55" s="7"/>
+      <c r="L55" s="7"/>
+      <c r="M55" s="8"/>
+      <c r="N55" s="7"/>
+      <c r="O55" s="8"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="7" t="s">
+        <v>412</v>
+      </c>
+      <c r="R55" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S55" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T55" s="7">
+        <v>1</v>
+      </c>
+      <c r="U55" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V55" s="7" t="s">
+        <v>413</v>
+      </c>
+      <c r="W55" s="7" t="s">
+        <v>414</v>
+      </c>
+      <c r="X55" s="7" t="s">
+        <v>415</v>
+      </c>
+      <c r="Y55" s="7"/>
+      <c r="Z55" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA55" s="7"/>
+      <c r="AB55" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC55" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD55" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE55" s="7"/>
+      <c r="AF55" s="7"/>
+      <c r="AG55" s="7"/>
+      <c r="AH55" s="7"/>
+      <c r="AI55" s="7"/>
+      <c r="AJ55" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK55" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="56" spans="1:37">
+      <c r="A56" s="3">
+        <v>54</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C56" s="3">
+        <v>2025061668</v>
+      </c>
+      <c r="D56" s="3"/>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3">
+        <v>3243</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>416</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="3"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="10"/>
+      <c r="Q56" s="3" t="s">
+        <v>417</v>
+      </c>
+      <c r="R56" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S56" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T56" s="3">
+        <v>1</v>
+      </c>
+      <c r="U56" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V56" s="3" t="s">
+        <v>418</v>
+      </c>
+      <c r="W56" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="X56" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="Y56" s="3"/>
+      <c r="Z56" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA56" s="3"/>
+      <c r="AB56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC56" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="AD56" s="3"/>
+      <c r="AE56" s="3"/>
+      <c r="AF56" s="3"/>
+      <c r="AG56" s="3"/>
+      <c r="AH56" s="3"/>
+      <c r="AI56" s="3"/>
+      <c r="AJ56" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK56" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="57" spans="1:37">
+      <c r="A57" s="7">
+        <v>55</v>
+      </c>
+      <c r="B57" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C57" s="7">
+        <v>2025061676</v>
+      </c>
+      <c r="D57" s="7"/>
+      <c r="E57" s="7"/>
+      <c r="F57" s="7">
+        <v>3796</v>
+      </c>
+      <c r="G57" s="7" t="s">
+        <v>422</v>
+      </c>
+      <c r="H57" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I57" s="7"/>
+      <c r="J57" s="7"/>
+      <c r="K57" s="7"/>
+      <c r="L57" s="7"/>
+      <c r="M57" s="8"/>
+      <c r="N57" s="7"/>
+      <c r="O57" s="8"/>
+      <c r="P57" s="9"/>
+      <c r="Q57" s="7" t="s">
+        <v>423</v>
+      </c>
+      <c r="R57" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S57" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T57" s="7">
+        <v>1</v>
+      </c>
+      <c r="U57" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V57" s="7" t="s">
+        <v>424</v>
+      </c>
+      <c r="W57" s="7" t="s">
+        <v>425</v>
+      </c>
+      <c r="X57" s="7" t="s">
+        <v>426</v>
+      </c>
+      <c r="Y57" s="7"/>
+      <c r="Z57" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA57" s="7"/>
+      <c r="AB57" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC57" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD57" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE57" s="7"/>
+      <c r="AF57" s="7"/>
+      <c r="AG57" s="7"/>
+      <c r="AH57" s="7"/>
+      <c r="AI57" s="7"/>
+      <c r="AJ57" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK57" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="58" spans="1:37">
+      <c r="A58" s="3">
+        <v>56</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C58" s="3">
+        <v>2025061682</v>
+      </c>
+      <c r="D58" s="3"/>
+      <c r="E58" s="3"/>
+      <c r="F58" s="3" t="s">
+        <v>427</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>428</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I58" s="3"/>
+      <c r="J58" s="3"/>
+      <c r="K58" s="3"/>
+      <c r="L58" s="3"/>
+      <c r="M58" s="4"/>
+      <c r="N58" s="3"/>
+      <c r="O58" s="4"/>
+      <c r="P58" s="10"/>
+      <c r="Q58" s="3" t="s">
+        <v>429</v>
+      </c>
+      <c r="R58" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S58" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T58" s="3">
+        <v>1</v>
+      </c>
+      <c r="U58" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V58" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="W58" s="3" t="s">
+        <v>426</v>
+      </c>
+      <c r="X58" s="3" t="s">
+        <v>431</v>
+      </c>
+      <c r="Y58" s="3"/>
+      <c r="Z58" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA58" s="3"/>
+      <c r="AB58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC58" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD58" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE58" s="3"/>
+      <c r="AF58" s="3"/>
+      <c r="AG58" s="3"/>
+      <c r="AH58" s="3"/>
+      <c r="AI58" s="3"/>
+      <c r="AJ58" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK58" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="59" spans="1:37">
+      <c r="A59" s="7">
+        <v>57</v>
+      </c>
+      <c r="B59" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C59" s="7">
+        <v>2025061684</v>
+      </c>
+      <c r="D59" s="7"/>
+      <c r="E59" s="7"/>
+      <c r="F59" s="7">
+        <v>3811</v>
+      </c>
+      <c r="G59" s="7" t="s">
+        <v>432</v>
+      </c>
+      <c r="H59" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I59" s="7"/>
+      <c r="J59" s="7"/>
+      <c r="K59" s="7"/>
+      <c r="L59" s="7"/>
+      <c r="M59" s="8"/>
+      <c r="N59" s="7"/>
+      <c r="O59" s="8"/>
+      <c r="P59" s="9"/>
+      <c r="Q59" s="7" t="s">
+        <v>433</v>
+      </c>
+      <c r="R59" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S59" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T59" s="7">
+        <v>1</v>
+      </c>
+      <c r="U59" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V59" s="7" t="s">
+        <v>434</v>
+      </c>
+      <c r="W59" s="7" t="s">
+        <v>435</v>
+      </c>
+      <c r="X59" s="7" t="s">
+        <v>436</v>
+      </c>
+      <c r="Y59" s="7"/>
+      <c r="Z59" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA59" s="7"/>
+      <c r="AB59" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC59" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD59" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE59" s="7"/>
+      <c r="AF59" s="7"/>
+      <c r="AG59" s="7"/>
+      <c r="AH59" s="7"/>
+      <c r="AI59" s="7"/>
+      <c r="AJ59" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK59" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="60" spans="1:37">
+      <c r="A60" s="3">
+        <v>58</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C60" s="3">
+        <v>2025061685</v>
+      </c>
+      <c r="D60" s="3"/>
+      <c r="E60" s="3"/>
+      <c r="F60" s="3">
+        <v>4422</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I60" s="3"/>
+      <c r="J60" s="3"/>
+      <c r="K60" s="3"/>
+      <c r="L60" s="3"/>
+      <c r="M60" s="4"/>
+      <c r="N60" s="3"/>
+      <c r="O60" s="4"/>
+      <c r="P60" s="4"/>
+      <c r="Q60" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="R60" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S60" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T60" s="3">
+        <v>1</v>
+      </c>
+      <c r="U60" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V60" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="W60" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="X60" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="Y60" s="3"/>
+      <c r="Z60" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA60" s="3"/>
+      <c r="AB60" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC60" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD60" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE60" s="3"/>
+      <c r="AF60" s="3"/>
+      <c r="AG60" s="3"/>
+      <c r="AH60" s="3"/>
+      <c r="AI60" s="3"/>
+      <c r="AJ60" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK60" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 12-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$60</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$63</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="442">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-11  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="457">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-12  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1379,6 +1379,52 @@
   </si>
   <si>
     <t>2025-06-11 13:15:00</t>
+  </si>
+  <si>
+    <t>北縣重富店</t>
+  </si>
+  <si>
+    <t>THILF03601</t>
+  </si>
+  <si>
+    <t>2025-06-11 16:29:05</t>
+  </si>
+  <si>
+    <t>2025-06-11 15:20:00</t>
+  </si>
+  <si>
+    <t>2025-06-11 16:10:00</t>
+  </si>
+  <si>
+    <t>D057</t>
+  </si>
+  <si>
+    <t>北縣溪尾二店</t>
+  </si>
+  <si>
+    <t>THILF0D057</t>
+  </si>
+  <si>
+    <t>2025-06-12 11:49:00</t>
+  </si>
+  <si>
+    <t>2025-06-12 10:50:00</t>
+  </si>
+  <si>
+    <t>2025-06-12 11:48:00</t>
+  </si>
+  <si>
+    <t>2025-06-12 11:53:05</t>
+  </si>
+  <si>
+    <t>2025-06-12 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-12 11:50:00</t>
+  </si>
+  <si>
+    <t>貼資產貼紙 電路編號2901299425 
+序號2PVQCJA000068 測速15m</t>
   </si>
 </sst>
 </file>
@@ -1792,10 +1838,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK60"/>
+  <dimension ref="A1:AK63"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC57" sqref="AC57"/>
+      <selection activeCell="A63" sqref="A63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -6838,7 +6884,7 @@
       <c r="M60" s="4"/>
       <c r="N60" s="3"/>
       <c r="O60" s="4"/>
-      <c r="P60" s="4"/>
+      <c r="P60" s="10"/>
       <c r="Q60" s="3" t="s">
         <v>438</v>
       </c>
@@ -6871,7 +6917,7 @@
       <c r="AB60" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC60" s="4" t="s">
+      <c r="AC60" s="10" t="s">
         <v>129</v>
       </c>
       <c r="AD60" s="3" t="s">
@@ -6886,6 +6932,241 @@
         <v>60</v>
       </c>
       <c r="AK60" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="1:37">
+      <c r="A61" s="7">
+        <v>59</v>
+      </c>
+      <c r="B61" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C61" s="7">
+        <v>2025061822</v>
+      </c>
+      <c r="D61" s="7"/>
+      <c r="E61" s="7"/>
+      <c r="F61" s="7">
+        <v>3601</v>
+      </c>
+      <c r="G61" s="7" t="s">
+        <v>442</v>
+      </c>
+      <c r="H61" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I61" s="7"/>
+      <c r="J61" s="7"/>
+      <c r="K61" s="7"/>
+      <c r="L61" s="7"/>
+      <c r="M61" s="8"/>
+      <c r="N61" s="7"/>
+      <c r="O61" s="8"/>
+      <c r="P61" s="9"/>
+      <c r="Q61" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="R61" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S61" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T61" s="7">
+        <v>1</v>
+      </c>
+      <c r="U61" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V61" s="7" t="s">
+        <v>444</v>
+      </c>
+      <c r="W61" s="7" t="s">
+        <v>445</v>
+      </c>
+      <c r="X61" s="7" t="s">
+        <v>446</v>
+      </c>
+      <c r="Y61" s="7"/>
+      <c r="Z61" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA61" s="7"/>
+      <c r="AB61" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC61" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD61" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE61" s="7"/>
+      <c r="AF61" s="7"/>
+      <c r="AG61" s="7"/>
+      <c r="AH61" s="7"/>
+      <c r="AI61" s="7"/>
+      <c r="AJ61" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK61" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" spans="1:37">
+      <c r="A62" s="3">
+        <v>60</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C62" s="3">
+        <v>2025061888</v>
+      </c>
+      <c r="D62" s="3"/>
+      <c r="E62" s="3"/>
+      <c r="F62" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>448</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I62" s="3"/>
+      <c r="J62" s="3"/>
+      <c r="K62" s="3"/>
+      <c r="L62" s="3"/>
+      <c r="M62" s="4"/>
+      <c r="N62" s="3"/>
+      <c r="O62" s="4"/>
+      <c r="P62" s="10"/>
+      <c r="Q62" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="R62" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S62" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T62" s="3">
+        <v>1</v>
+      </c>
+      <c r="U62" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V62" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="W62" s="3" t="s">
+        <v>451</v>
+      </c>
+      <c r="X62" s="3" t="s">
+        <v>452</v>
+      </c>
+      <c r="Y62" s="3"/>
+      <c r="Z62" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA62" s="3"/>
+      <c r="AB62" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC62" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD62" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE62" s="3"/>
+      <c r="AF62" s="3"/>
+      <c r="AG62" s="3"/>
+      <c r="AH62" s="3"/>
+      <c r="AI62" s="3"/>
+      <c r="AJ62" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK62" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="63" spans="1:37">
+      <c r="A63" s="7">
+        <v>61</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C63" s="7">
+        <v>2025061891</v>
+      </c>
+      <c r="D63" s="7"/>
+      <c r="E63" s="7"/>
+      <c r="F63" s="7">
+        <v>5364</v>
+      </c>
+      <c r="G63" s="7" t="s">
+        <v>405</v>
+      </c>
+      <c r="H63" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="I63" s="7"/>
+      <c r="J63" s="7"/>
+      <c r="K63" s="7"/>
+      <c r="L63" s="7"/>
+      <c r="M63" s="8"/>
+      <c r="N63" s="7"/>
+      <c r="O63" s="8"/>
+      <c r="P63" s="8"/>
+      <c r="Q63" s="7" t="s">
+        <v>406</v>
+      </c>
+      <c r="R63" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S63" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T63" s="7">
+        <v>1</v>
+      </c>
+      <c r="U63" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V63" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="W63" s="7" t="s">
+        <v>454</v>
+      </c>
+      <c r="X63" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="Y63" s="7"/>
+      <c r="Z63" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA63" s="7"/>
+      <c r="AB63" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC63" s="8" t="s">
+        <v>456</v>
+      </c>
+      <c r="AD63" s="7"/>
+      <c r="AE63" s="7"/>
+      <c r="AF63" s="7"/>
+      <c r="AG63" s="7"/>
+      <c r="AH63" s="7"/>
+      <c r="AI63" s="7"/>
+      <c r="AJ63" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK63" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 13-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$64</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$69</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="462">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-12  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="497">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-13  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1396,6 +1396,44 @@
     <t>2025-06-11 16:10:00</t>
   </si>
   <si>
+    <t>14923114061201</t>
+  </si>
+  <si>
+    <t>蘆洲永平店</t>
+  </si>
+  <si>
+    <t>2025-06-12 11:07:38</t>
+  </si>
+  <si>
+    <t>D307</t>
+  </si>
+  <si>
+    <t>異物掉進發票機</t>
+  </si>
+  <si>
+    <t>TM2發票機(BSC-10	)列印時會發出異音，已有關機、重裝紙捲後仍異常，但列印皆正常OK，請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04923</t>
+  </si>
+  <si>
+    <t>2025-06-12 11:10:04</t>
+  </si>
+  <si>
+    <t>2025-06-13 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-13 11:26:00</t>
+  </si>
+  <si>
+    <t>2025-06-13 15:10:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換下8155002473
+換上8155006243</t>
+  </si>
+  <si>
     <t>D057</t>
   </si>
   <si>
@@ -1440,6 +1478,75 @@
   </si>
   <si>
     <t>2025-06-12 15:10:00</t>
+  </si>
+  <si>
+    <t>五股興珍店</t>
+  </si>
+  <si>
+    <t>THILF02691</t>
+  </si>
+  <si>
+    <t>2025-06-12 15:51:08</t>
+  </si>
+  <si>
+    <t>2025-06-12 15:20:00</t>
+  </si>
+  <si>
+    <t>2025-06-12 15:55:00</t>
+  </si>
+  <si>
+    <t>E3623114061201</t>
+  </si>
+  <si>
+    <t>三重自強店</t>
+  </si>
+  <si>
+    <t>2025-06-12 15:47:00</t>
+  </si>
+  <si>
+    <t>螢幕畫面異常/觸控不良(游標偏移)</t>
+  </si>
+  <si>
+    <t>門市反應MMK四代機觸控無反應，PING60有通，已嘗試重啟MMK仍異常..請台芝到店協助(螢幕當機無法使用)</t>
+  </si>
+  <si>
+    <t>THILF03623</t>
+  </si>
+  <si>
+    <t>2025-06-12 16:00:24</t>
+  </si>
+  <si>
+    <t>2025-06-12 16:23:00</t>
+  </si>
+  <si>
+    <t>2025-06-12 16:53:00</t>
+  </si>
+  <si>
+    <t>2025-06-13 20:00:00</t>
+  </si>
+  <si>
+    <t>現場將Touch線重新插拔，目前可正常使用，需請店員在進行觀察狀況</t>
+  </si>
+  <si>
+    <t>五股五工店</t>
+  </si>
+  <si>
+    <t>THILF02535</t>
+  </si>
+  <si>
+    <t>2025-06-12 16:25:53</t>
+  </si>
+  <si>
+    <t>2025-06-12 16:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-12 16:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-13 11:30:06</t>
+  </si>
+  <si>
+    <t>2025-06-13 11:29:00</t>
   </si>
 </sst>
 </file>
@@ -1853,10 +1960,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK64"/>
+  <dimension ref="A1:AK69"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC61" sqref="AC61"/>
+      <selection activeCell="A69" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -7034,32 +7141,52 @@
         <v>60</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C62" s="3">
-        <v>2025061888</v>
-      </c>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3" t="s">
+        <v>2025061882</v>
+      </c>
+      <c r="D62" s="3" t="s">
         <v>447</v>
+      </c>
+      <c r="E62" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F62" s="3">
+        <v>4923</v>
       </c>
       <c r="G62" s="3" t="s">
         <v>448</v>
       </c>
       <c r="H62" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="4"/>
-      <c r="N62" s="3"/>
-      <c r="O62" s="4"/>
-      <c r="P62" s="10"/>
+        <v>101</v>
+      </c>
+      <c r="I62" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K62" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L62" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M62" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N62" s="3" t="s">
+        <v>450</v>
+      </c>
+      <c r="O62" s="4" t="s">
+        <v>451</v>
+      </c>
+      <c r="P62" s="10" t="s">
+        <v>452</v>
+      </c>
       <c r="Q62" s="3" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="R62" s="3" t="s">
         <v>51</v>
@@ -7074,36 +7201,34 @@
         <v>53</v>
       </c>
       <c r="V62" s="3" t="s">
-        <v>450</v>
+        <v>454</v>
       </c>
       <c r="W62" s="3" t="s">
-        <v>451</v>
+        <v>455</v>
       </c>
       <c r="X62" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="Y62" s="3"/>
+        <v>456</v>
+      </c>
+      <c r="Y62" s="3" t="s">
+        <v>457</v>
+      </c>
       <c r="Z62" s="3">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="AA62" s="3"/>
       <c r="AB62" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC62" s="10" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD62" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>458</v>
+      </c>
+      <c r="AD62" s="3"/>
       <c r="AE62" s="3"/>
       <c r="AF62" s="3"/>
       <c r="AG62" s="3"/>
       <c r="AH62" s="3"/>
       <c r="AI62" s="3"/>
-      <c r="AJ62" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ62" s="3"/>
       <c r="AK62" s="3" t="s">
         <v>60</v>
       </c>
@@ -7116,18 +7241,18 @@
         <v>94</v>
       </c>
       <c r="C63" s="7">
-        <v>2025061891</v>
+        <v>2025061888</v>
       </c>
       <c r="D63" s="7"/>
       <c r="E63" s="7"/>
-      <c r="F63" s="7">
-        <v>5364</v>
+      <c r="F63" s="7" t="s">
+        <v>459</v>
       </c>
       <c r="G63" s="7" t="s">
-        <v>405</v>
+        <v>460</v>
       </c>
       <c r="H63" s="7" t="s">
-        <v>209</v>
+        <v>42</v>
       </c>
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
@@ -7138,13 +7263,13 @@
       <c r="O63" s="8"/>
       <c r="P63" s="9"/>
       <c r="Q63" s="7" t="s">
-        <v>406</v>
+        <v>461</v>
       </c>
       <c r="R63" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S63" s="7" t="s">
-        <v>73</v>
+        <v>52</v>
       </c>
       <c r="T63" s="7">
         <v>1</v>
@@ -7153,26 +7278,28 @@
         <v>53</v>
       </c>
       <c r="V63" s="7" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
       <c r="W63" s="7" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="X63" s="7" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
       <c r="Y63" s="7"/>
       <c r="Z63" s="7">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="AA63" s="7"/>
       <c r="AB63" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC63" s="9" t="s">
-        <v>456</v>
-      </c>
-      <c r="AD63" s="7"/>
+        <v>98</v>
+      </c>
+      <c r="AD63" s="7" t="s">
+        <v>60</v>
+      </c>
       <c r="AE63" s="7"/>
       <c r="AF63" s="7"/>
       <c r="AG63" s="7"/>
@@ -7193,18 +7320,18 @@
         <v>94</v>
       </c>
       <c r="C64" s="3">
-        <v>2025061929</v>
+        <v>2025061891</v>
       </c>
       <c r="D64" s="3"/>
       <c r="E64" s="3"/>
       <c r="F64" s="3">
-        <v>2390</v>
+        <v>5364</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>457</v>
+        <v>405</v>
       </c>
       <c r="H64" s="3" t="s">
-        <v>184</v>
+        <v>209</v>
       </c>
       <c r="I64" s="3"/>
       <c r="J64" s="3"/>
@@ -7213,9 +7340,9 @@
       <c r="M64" s="4"/>
       <c r="N64" s="3"/>
       <c r="O64" s="4"/>
-      <c r="P64" s="4"/>
+      <c r="P64" s="10"/>
       <c r="Q64" s="3" t="s">
-        <v>458</v>
+        <v>406</v>
       </c>
       <c r="R64" s="3" t="s">
         <v>51</v>
@@ -7230,24 +7357,24 @@
         <v>53</v>
       </c>
       <c r="V64" s="3" t="s">
-        <v>459</v>
+        <v>465</v>
       </c>
       <c r="W64" s="3" t="s">
-        <v>460</v>
+        <v>466</v>
       </c>
       <c r="X64" s="3" t="s">
-        <v>461</v>
+        <v>467</v>
       </c>
       <c r="Y64" s="3"/>
       <c r="Z64" s="3">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="AA64" s="3"/>
       <c r="AB64" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC64" s="4" t="s">
-        <v>421</v>
+      <c r="AC64" s="10" t="s">
+        <v>468</v>
       </c>
       <c r="AD64" s="3"/>
       <c r="AE64" s="3"/>
@@ -7259,6 +7386,413 @@
         <v>60</v>
       </c>
       <c r="AK64" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="65" spans="1:37">
+      <c r="A65" s="7">
+        <v>63</v>
+      </c>
+      <c r="B65" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C65" s="7">
+        <v>2025061929</v>
+      </c>
+      <c r="D65" s="7"/>
+      <c r="E65" s="7"/>
+      <c r="F65" s="7">
+        <v>2390</v>
+      </c>
+      <c r="G65" s="7" t="s">
+        <v>469</v>
+      </c>
+      <c r="H65" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I65" s="7"/>
+      <c r="J65" s="7"/>
+      <c r="K65" s="7"/>
+      <c r="L65" s="7"/>
+      <c r="M65" s="8"/>
+      <c r="N65" s="7"/>
+      <c r="O65" s="8"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="7" t="s">
+        <v>470</v>
+      </c>
+      <c r="R65" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S65" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T65" s="7">
+        <v>1</v>
+      </c>
+      <c r="U65" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V65" s="7" t="s">
+        <v>471</v>
+      </c>
+      <c r="W65" s="7" t="s">
+        <v>472</v>
+      </c>
+      <c r="X65" s="7" t="s">
+        <v>473</v>
+      </c>
+      <c r="Y65" s="7"/>
+      <c r="Z65" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA65" s="7"/>
+      <c r="AB65" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC65" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="AD65" s="7"/>
+      <c r="AE65" s="7"/>
+      <c r="AF65" s="7"/>
+      <c r="AG65" s="7"/>
+      <c r="AH65" s="7"/>
+      <c r="AI65" s="7"/>
+      <c r="AJ65" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK65" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="66" spans="1:37">
+      <c r="A66" s="3">
+        <v>64</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C66" s="3">
+        <v>2025061933</v>
+      </c>
+      <c r="D66" s="3"/>
+      <c r="E66" s="3"/>
+      <c r="F66" s="3">
+        <v>2691</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I66" s="3"/>
+      <c r="J66" s="3"/>
+      <c r="K66" s="3"/>
+      <c r="L66" s="3"/>
+      <c r="M66" s="4"/>
+      <c r="N66" s="3"/>
+      <c r="O66" s="4"/>
+      <c r="P66" s="10"/>
+      <c r="Q66" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="R66" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S66" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T66" s="3">
+        <v>1</v>
+      </c>
+      <c r="U66" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V66" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="W66" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="X66" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="Y66" s="3"/>
+      <c r="Z66" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA66" s="3"/>
+      <c r="AB66" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC66" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="AD66" s="3"/>
+      <c r="AE66" s="3"/>
+      <c r="AF66" s="3"/>
+      <c r="AG66" s="3"/>
+      <c r="AH66" s="3"/>
+      <c r="AI66" s="3"/>
+      <c r="AJ66" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK66" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="67" spans="1:37">
+      <c r="A67" s="7">
+        <v>65</v>
+      </c>
+      <c r="B67" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C67" s="7">
+        <v>2025061936</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>479</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F67" s="7">
+        <v>3623</v>
+      </c>
+      <c r="G67" s="7" t="s">
+        <v>480</v>
+      </c>
+      <c r="H67" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I67" s="7" t="s">
+        <v>481</v>
+      </c>
+      <c r="J67" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K67" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L67" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="M67" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="N67" s="7">
+        <v>5802</v>
+      </c>
+      <c r="O67" s="8" t="s">
+        <v>482</v>
+      </c>
+      <c r="P67" s="9" t="s">
+        <v>483</v>
+      </c>
+      <c r="Q67" s="7" t="s">
+        <v>484</v>
+      </c>
+      <c r="R67" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S67" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T67" s="7">
+        <v>1</v>
+      </c>
+      <c r="U67" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V67" s="7" t="s">
+        <v>485</v>
+      </c>
+      <c r="W67" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="X67" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="Y67" s="7" t="s">
+        <v>488</v>
+      </c>
+      <c r="Z67" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA67" s="7"/>
+      <c r="AB67" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC67" s="9" t="s">
+        <v>489</v>
+      </c>
+      <c r="AD67" s="7"/>
+      <c r="AE67" s="7"/>
+      <c r="AF67" s="7"/>
+      <c r="AG67" s="7"/>
+      <c r="AH67" s="7"/>
+      <c r="AI67" s="7"/>
+      <c r="AJ67" s="7"/>
+      <c r="AK67" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="68" spans="1:37">
+      <c r="A68" s="3">
+        <v>66</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C68" s="3">
+        <v>2025061942</v>
+      </c>
+      <c r="D68" s="3"/>
+      <c r="E68" s="3"/>
+      <c r="F68" s="3">
+        <v>2535</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>490</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I68" s="3"/>
+      <c r="J68" s="3"/>
+      <c r="K68" s="3"/>
+      <c r="L68" s="3"/>
+      <c r="M68" s="4"/>
+      <c r="N68" s="3"/>
+      <c r="O68" s="4"/>
+      <c r="P68" s="10"/>
+      <c r="Q68" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="R68" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S68" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T68" s="3">
+        <v>1</v>
+      </c>
+      <c r="U68" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V68" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="W68" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="X68" s="3" t="s">
+        <v>494</v>
+      </c>
+      <c r="Y68" s="3"/>
+      <c r="Z68" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA68" s="3"/>
+      <c r="AB68" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC68" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD68" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE68" s="3"/>
+      <c r="AF68" s="3"/>
+      <c r="AG68" s="3"/>
+      <c r="AH68" s="3"/>
+      <c r="AI68" s="3"/>
+      <c r="AJ68" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK68" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="69" spans="1:37">
+      <c r="A69" s="7">
+        <v>67</v>
+      </c>
+      <c r="B69" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C69" s="7">
+        <v>2025061995</v>
+      </c>
+      <c r="D69" s="7"/>
+      <c r="E69" s="7"/>
+      <c r="F69" s="7">
+        <v>4923</v>
+      </c>
+      <c r="G69" s="7" t="s">
+        <v>448</v>
+      </c>
+      <c r="H69" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I69" s="7"/>
+      <c r="J69" s="7"/>
+      <c r="K69" s="7"/>
+      <c r="L69" s="7"/>
+      <c r="M69" s="8"/>
+      <c r="N69" s="7"/>
+      <c r="O69" s="8"/>
+      <c r="P69" s="8"/>
+      <c r="Q69" s="7" t="s">
+        <v>453</v>
+      </c>
+      <c r="R69" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S69" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T69" s="7">
+        <v>1</v>
+      </c>
+      <c r="U69" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V69" s="7" t="s">
+        <v>495</v>
+      </c>
+      <c r="W69" s="7" t="s">
+        <v>455</v>
+      </c>
+      <c r="X69" s="7" t="s">
+        <v>496</v>
+      </c>
+      <c r="Y69" s="7"/>
+      <c r="Z69" s="7">
+        <v>1</v>
+      </c>
+      <c r="AA69" s="7"/>
+      <c r="AB69" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC69" s="8" t="s">
+        <v>366</v>
+      </c>
+      <c r="AD69" s="7"/>
+      <c r="AE69" s="7"/>
+      <c r="AF69" s="7"/>
+      <c r="AG69" s="7"/>
+      <c r="AH69" s="7"/>
+      <c r="AI69" s="7"/>
+      <c r="AJ69" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK69" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 16-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$74</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$75</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="530">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-13  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="541">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-16  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1648,6 +1648,39 @@
   </si>
   <si>
     <t>2025-06-13 15:45:00</t>
+  </si>
+  <si>
+    <t>15074114061501</t>
+  </si>
+  <si>
+    <t>八里福德新村</t>
+  </si>
+  <si>
+    <t>2025-06-15 13:33:16</t>
+  </si>
+  <si>
+    <t>星期日</t>
+  </si>
+  <si>
+    <t>門市反應TM1-CCD掃描器(HC56II-TR、HC76-TR)無電源反應，確認後方線路無鬆脫，已嘗試重啟TM仍異常..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF05074</t>
+  </si>
+  <si>
+    <t>2025-06-15 13:34:53</t>
+  </si>
+  <si>
+    <t>2025-06-16 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-16 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-17 13:00:00</t>
+  </si>
+  <si>
+    <t>重新插上IO卡，掃描槍可正常反應，請店員再觀察看看</t>
   </si>
 </sst>
 </file>
@@ -2061,10 +2094,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK74"/>
+  <dimension ref="A1:AK75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC71" sqref="AC71"/>
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8255,7 +8288,7 @@
       <c r="M74" s="4"/>
       <c r="N74" s="3"/>
       <c r="O74" s="4"/>
-      <c r="P74" s="4"/>
+      <c r="P74" s="10"/>
       <c r="Q74" s="3" t="s">
         <v>526</v>
       </c>
@@ -8288,7 +8321,7 @@
       <c r="AB74" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC74" s="4" t="s">
+      <c r="AC74" s="10" t="s">
         <v>129</v>
       </c>
       <c r="AD74" s="3" t="s">
@@ -8303,6 +8336,103 @@
         <v>60</v>
       </c>
       <c r="AK74" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="75" spans="1:37">
+      <c r="A75" s="7">
+        <v>73</v>
+      </c>
+      <c r="B75" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C75" s="7">
+        <v>2025062091</v>
+      </c>
+      <c r="D75" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="E75" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F75" s="7">
+        <v>5074</v>
+      </c>
+      <c r="G75" s="7" t="s">
+        <v>531</v>
+      </c>
+      <c r="H75" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="I75" s="7" t="s">
+        <v>532</v>
+      </c>
+      <c r="J75" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="K75" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L75" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M75" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N75" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O75" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P75" s="8" t="s">
+        <v>534</v>
+      </c>
+      <c r="Q75" s="7" t="s">
+        <v>535</v>
+      </c>
+      <c r="R75" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S75" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T75" s="7">
+        <v>1</v>
+      </c>
+      <c r="U75" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V75" s="7" t="s">
+        <v>536</v>
+      </c>
+      <c r="W75" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="X75" s="7" t="s">
+        <v>538</v>
+      </c>
+      <c r="Y75" s="7" t="s">
+        <v>539</v>
+      </c>
+      <c r="Z75" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA75" s="7"/>
+      <c r="AB75" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC75" s="8" t="s">
+        <v>540</v>
+      </c>
+      <c r="AD75" s="7"/>
+      <c r="AE75" s="7"/>
+      <c r="AF75" s="7"/>
+      <c r="AG75" s="7"/>
+      <c r="AH75" s="7"/>
+      <c r="AI75" s="7"/>
+      <c r="AJ75" s="7"/>
+      <c r="AK75" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 17-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$75</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$85</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="541">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-16  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="599">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-17  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1650,6 +1650,47 @@
     <t>2025-06-13 15:45:00</t>
   </si>
   <si>
+    <t>E4093114061501</t>
+  </si>
+  <si>
+    <t>淡水新市一</t>
+  </si>
+  <si>
+    <t>2025-06-15 09:59:56</t>
+  </si>
+  <si>
+    <t>星期日</t>
+  </si>
+  <si>
+    <t>D303</t>
+  </si>
+  <si>
+    <t>無反應，不會轉動</t>
+  </si>
+  <si>
+    <t>門市反應TM1熱感發票機(BSC-10、BSC10II)TM顯示[熱感機正在列印中或熱感機無法連線!請稍後或檢查發票機電源、上蓋是否蓋妥!請按清除!]，門市已嘗試重新拔插線路及重啟發票機仍持續跳出此訊息...請台芝到店協助(線接觸不良 無法使用 SOS)</t>
+  </si>
+  <si>
+    <t>THILF04093</t>
+  </si>
+  <si>
+    <t>2025-06-15 10:15:31</t>
+  </si>
+  <si>
+    <t>2025-06-16 12:10:00</t>
+  </si>
+  <si>
+    <t>2025-06-16 12:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-17 13:00:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換下8155003404
+換上8155006255</t>
+  </si>
+  <si>
     <t>15074114061501</t>
   </si>
   <si>
@@ -1659,9 +1700,6 @@
     <t>2025-06-15 13:33:16</t>
   </si>
   <si>
-    <t>星期日</t>
-  </si>
-  <si>
     <t>門市反應TM1-CCD掃描器(HC56II-TR、HC76-TR)無電源反應，確認後方線路無鬆脫，已嘗試重啟TM仍異常..請台芝到店協助</t>
   </si>
   <si>
@@ -1677,10 +1715,152 @@
     <t>2025-06-16 11:00:00</t>
   </si>
   <si>
-    <t>2025-06-17 13:00:00</t>
-  </si>
-  <si>
     <t>重新插上IO卡，掃描槍可正常反應，請店員再觀察看看</t>
+  </si>
+  <si>
+    <t>14680114061601</t>
+  </si>
+  <si>
+    <t>板橋江寧店</t>
+  </si>
+  <si>
+    <t>2025-06-16 09:20:31</t>
+  </si>
+  <si>
+    <t>TM1收銀抽屜(外觀顏色白色，鎖頭置中，編號5001)使用鑰匙無法鎖起來，門市確認有卡住聲音，但點選開抽屜仍會被開啟，請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04680</t>
+  </si>
+  <si>
+    <t>2025-06-16 09:23:30</t>
+  </si>
+  <si>
+    <t>2025-06-16 15:20:00</t>
+  </si>
+  <si>
+    <t>2025-06-16 15:50:00</t>
+  </si>
+  <si>
+    <t>2025-06-17 13:23:00</t>
+  </si>
+  <si>
+    <t>更換錢箱
+換上：81Z1004280
+換下：81Z1000991</t>
+  </si>
+  <si>
+    <t>14680114061602</t>
+  </si>
+  <si>
+    <t>2025-06-16 09:23:41</t>
+  </si>
+  <si>
+    <t>TM2收銀抽屜(外觀顏色白色，鎖頭置中，編號5001)使用鑰匙無法鎖起來，門市確認有卡住聲音，但點選開抽屜仍會被開啟，請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-06-16 09:24:11</t>
+  </si>
+  <si>
+    <t>2025-06-17 13:24:00</t>
+  </si>
+  <si>
+    <t>更換錢箱
+換上：81Z1004275
+換下：81Z1000992</t>
+  </si>
+  <si>
+    <t>新莊中港店</t>
+  </si>
+  <si>
+    <t>THILF05057</t>
+  </si>
+  <si>
+    <t>2025-06-16 13:36:56</t>
+  </si>
+  <si>
+    <t>2025-06-16 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-16 13:45:00</t>
+  </si>
+  <si>
+    <t>北縣莊玲店</t>
+  </si>
+  <si>
+    <t>THILF03052</t>
+  </si>
+  <si>
+    <t>2025-06-16 14:20:21</t>
+  </si>
+  <si>
+    <t>2025-06-16 13:55:00</t>
+  </si>
+  <si>
+    <t>2025-06-16 14:25:00</t>
+  </si>
+  <si>
+    <t>D350</t>
+  </si>
+  <si>
+    <t>北縣仁和店</t>
+  </si>
+  <si>
+    <t>THILF0D350</t>
+  </si>
+  <si>
+    <t>2025-06-16 14:28:07</t>
+  </si>
+  <si>
+    <t>2025-06-16 13:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-16 14:27:00</t>
+  </si>
+  <si>
+    <t>三重美溪店</t>
+  </si>
+  <si>
+    <t>THILF03772</t>
+  </si>
+  <si>
+    <t>2025-06-16 15:47:19</t>
+  </si>
+  <si>
+    <t>2025-06-16 15:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-16 15:45:00</t>
+  </si>
+  <si>
+    <t>2025-06-16 15:59:48</t>
+  </si>
+  <si>
+    <t>北縣板嘉店</t>
+  </si>
+  <si>
+    <t>THILF02746</t>
+  </si>
+  <si>
+    <t>2025-06-16 16:37:11</t>
+  </si>
+  <si>
+    <t>2025-06-16 16:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-16 16:35:00</t>
+  </si>
+  <si>
+    <t>三重福仁店</t>
+  </si>
+  <si>
+    <t>THILF03957</t>
+  </si>
+  <si>
+    <t>2025-06-16 16:38:41</t>
+  </si>
+  <si>
+    <t>2025-06-16 16:38:00</t>
   </si>
 </sst>
 </file>
@@ -2094,10 +2274,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK75"/>
+  <dimension ref="A1:AK85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A75" sqref="A75"/>
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -8347,7 +8527,7 @@
         <v>38</v>
       </c>
       <c r="C75" s="7">
-        <v>2025062091</v>
+        <v>2025062090</v>
       </c>
       <c r="D75" s="7" t="s">
         <v>530</v>
@@ -8356,13 +8536,13 @@
         <v>40</v>
       </c>
       <c r="F75" s="7">
-        <v>5074</v>
+        <v>4093</v>
       </c>
       <c r="G75" s="7" t="s">
         <v>531</v>
       </c>
       <c r="H75" s="7" t="s">
-        <v>237</v>
+        <v>163</v>
       </c>
       <c r="I75" s="7" t="s">
         <v>532</v>
@@ -8371,25 +8551,25 @@
         <v>533</v>
       </c>
       <c r="K75" s="7" t="s">
-        <v>45</v>
+        <v>66</v>
       </c>
       <c r="L75" s="7" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="M75" s="8" t="s">
-        <v>68</v>
+        <v>147</v>
       </c>
       <c r="N75" s="7" t="s">
-        <v>69</v>
+        <v>534</v>
       </c>
       <c r="O75" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="P75" s="8" t="s">
-        <v>534</v>
+        <v>535</v>
+      </c>
+      <c r="P75" s="9" t="s">
+        <v>536</v>
       </c>
       <c r="Q75" s="7" t="s">
-        <v>535</v>
+        <v>537</v>
       </c>
       <c r="R75" s="7" t="s">
         <v>51</v>
@@ -8404,16 +8584,16 @@
         <v>53</v>
       </c>
       <c r="V75" s="7" t="s">
-        <v>536</v>
+        <v>538</v>
       </c>
       <c r="W75" s="7" t="s">
-        <v>537</v>
+        <v>539</v>
       </c>
       <c r="X75" s="7" t="s">
-        <v>538</v>
+        <v>540</v>
       </c>
       <c r="Y75" s="7" t="s">
-        <v>539</v>
+        <v>541</v>
       </c>
       <c r="Z75" s="7">
         <v>0.5</v>
@@ -8422,8 +8602,8 @@
       <c r="AB75" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC75" s="8" t="s">
-        <v>540</v>
+      <c r="AC75" s="9" t="s">
+        <v>542</v>
       </c>
       <c r="AD75" s="7"/>
       <c r="AE75" s="7"/>
@@ -8433,6 +8613,844 @@
       <c r="AI75" s="7"/>
       <c r="AJ75" s="7"/>
       <c r="AK75" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="76" spans="1:37">
+      <c r="A76" s="3">
+        <v>74</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C76" s="3">
+        <v>2025062091</v>
+      </c>
+      <c r="D76" s="3" t="s">
+        <v>543</v>
+      </c>
+      <c r="E76" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F76" s="3">
+        <v>5074</v>
+      </c>
+      <c r="G76" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="H76" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="I76" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="J76" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="K76" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L76" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M76" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N76" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O76" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P76" s="10" t="s">
+        <v>546</v>
+      </c>
+      <c r="Q76" s="3" t="s">
+        <v>547</v>
+      </c>
+      <c r="R76" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S76" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T76" s="3">
+        <v>1</v>
+      </c>
+      <c r="U76" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V76" s="3" t="s">
+        <v>548</v>
+      </c>
+      <c r="W76" s="3" t="s">
+        <v>549</v>
+      </c>
+      <c r="X76" s="3" t="s">
+        <v>550</v>
+      </c>
+      <c r="Y76" s="3" t="s">
+        <v>541</v>
+      </c>
+      <c r="Z76" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA76" s="3"/>
+      <c r="AB76" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC76" s="10" t="s">
+        <v>551</v>
+      </c>
+      <c r="AD76" s="3"/>
+      <c r="AE76" s="3"/>
+      <c r="AF76" s="3"/>
+      <c r="AG76" s="3"/>
+      <c r="AH76" s="3"/>
+      <c r="AI76" s="3"/>
+      <c r="AJ76" s="3"/>
+      <c r="AK76" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="77" spans="1:37">
+      <c r="A77" s="7">
+        <v>75</v>
+      </c>
+      <c r="B77" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C77" s="7">
+        <v>2025062097</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>552</v>
+      </c>
+      <c r="E77" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F77" s="7">
+        <v>4680</v>
+      </c>
+      <c r="G77" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="H77" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I77" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="J77" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="K77" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L77" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="M77" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N77" s="7">
+        <v>2305</v>
+      </c>
+      <c r="O77" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="P77" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="Q77" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="R77" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S77" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T77" s="7">
+        <v>1</v>
+      </c>
+      <c r="U77" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V77" s="7" t="s">
+        <v>557</v>
+      </c>
+      <c r="W77" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="X77" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="Y77" s="7" t="s">
+        <v>560</v>
+      </c>
+      <c r="Z77" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA77" s="7"/>
+      <c r="AB77" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC77" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="AD77" s="7"/>
+      <c r="AE77" s="7"/>
+      <c r="AF77" s="7"/>
+      <c r="AG77" s="7"/>
+      <c r="AH77" s="7"/>
+      <c r="AI77" s="7"/>
+      <c r="AJ77" s="7"/>
+      <c r="AK77" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="78" spans="1:37">
+      <c r="A78" s="3">
+        <v>76</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C78" s="3">
+        <v>2025062098</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>562</v>
+      </c>
+      <c r="E78" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F78" s="3">
+        <v>4680</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I78" s="3" t="s">
+        <v>563</v>
+      </c>
+      <c r="J78" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K78" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L78" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M78" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="N78" s="3">
+        <v>2305</v>
+      </c>
+      <c r="O78" s="4" t="s">
+        <v>478</v>
+      </c>
+      <c r="P78" s="10" t="s">
+        <v>564</v>
+      </c>
+      <c r="Q78" s="3" t="s">
+        <v>556</v>
+      </c>
+      <c r="R78" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S78" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T78" s="3">
+        <v>1</v>
+      </c>
+      <c r="U78" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V78" s="3" t="s">
+        <v>565</v>
+      </c>
+      <c r="W78" s="3" t="s">
+        <v>558</v>
+      </c>
+      <c r="X78" s="3" t="s">
+        <v>559</v>
+      </c>
+      <c r="Y78" s="3" t="s">
+        <v>566</v>
+      </c>
+      <c r="Z78" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA78" s="3"/>
+      <c r="AB78" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC78" s="10" t="s">
+        <v>567</v>
+      </c>
+      <c r="AD78" s="3"/>
+      <c r="AE78" s="3"/>
+      <c r="AF78" s="3"/>
+      <c r="AG78" s="3"/>
+      <c r="AH78" s="3"/>
+      <c r="AI78" s="3"/>
+      <c r="AJ78" s="3"/>
+      <c r="AK78" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="79" spans="1:37">
+      <c r="A79" s="7">
+        <v>77</v>
+      </c>
+      <c r="B79" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C79" s="7">
+        <v>2025062144</v>
+      </c>
+      <c r="D79" s="7"/>
+      <c r="E79" s="7"/>
+      <c r="F79" s="7">
+        <v>5057</v>
+      </c>
+      <c r="G79" s="7" t="s">
+        <v>568</v>
+      </c>
+      <c r="H79" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I79" s="7"/>
+      <c r="J79" s="7"/>
+      <c r="K79" s="7"/>
+      <c r="L79" s="7"/>
+      <c r="M79" s="8"/>
+      <c r="N79" s="7"/>
+      <c r="O79" s="8"/>
+      <c r="P79" s="9"/>
+      <c r="Q79" s="7" t="s">
+        <v>569</v>
+      </c>
+      <c r="R79" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S79" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T79" s="7">
+        <v>1</v>
+      </c>
+      <c r="U79" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V79" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="W79" s="7" t="s">
+        <v>571</v>
+      </c>
+      <c r="X79" s="7" t="s">
+        <v>572</v>
+      </c>
+      <c r="Y79" s="7"/>
+      <c r="Z79" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA79" s="7"/>
+      <c r="AB79" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC79" s="9" t="s">
+        <v>421</v>
+      </c>
+      <c r="AD79" s="7"/>
+      <c r="AE79" s="7"/>
+      <c r="AF79" s="7"/>
+      <c r="AG79" s="7"/>
+      <c r="AH79" s="7"/>
+      <c r="AI79" s="7"/>
+      <c r="AJ79" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK79" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="1:37">
+      <c r="A80" s="3">
+        <v>78</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C80" s="3">
+        <v>2025062155</v>
+      </c>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3">
+        <v>3052</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>573</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="4"/>
+      <c r="N80" s="3"/>
+      <c r="O80" s="4"/>
+      <c r="P80" s="10"/>
+      <c r="Q80" s="3" t="s">
+        <v>574</v>
+      </c>
+      <c r="R80" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S80" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T80" s="3">
+        <v>1</v>
+      </c>
+      <c r="U80" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V80" s="3" t="s">
+        <v>575</v>
+      </c>
+      <c r="W80" s="3" t="s">
+        <v>576</v>
+      </c>
+      <c r="X80" s="3" t="s">
+        <v>577</v>
+      </c>
+      <c r="Y80" s="3"/>
+      <c r="Z80" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA80" s="3"/>
+      <c r="AB80" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC80" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="AD80" s="3"/>
+      <c r="AE80" s="3"/>
+      <c r="AF80" s="3"/>
+      <c r="AG80" s="3"/>
+      <c r="AH80" s="3"/>
+      <c r="AI80" s="3"/>
+      <c r="AJ80" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK80" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="81" spans="1:37">
+      <c r="A81" s="7">
+        <v>79</v>
+      </c>
+      <c r="B81" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C81" s="7">
+        <v>2025062158</v>
+      </c>
+      <c r="D81" s="7"/>
+      <c r="E81" s="7"/>
+      <c r="F81" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="G81" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="H81" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="8"/>
+      <c r="N81" s="7"/>
+      <c r="O81" s="8"/>
+      <c r="P81" s="9"/>
+      <c r="Q81" s="7" t="s">
+        <v>580</v>
+      </c>
+      <c r="R81" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S81" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T81" s="7">
+        <v>1</v>
+      </c>
+      <c r="U81" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V81" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="W81" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="X81" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="Y81" s="7"/>
+      <c r="Z81" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="AA81" s="7"/>
+      <c r="AB81" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC81" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD81" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE81" s="7"/>
+      <c r="AF81" s="7"/>
+      <c r="AG81" s="7"/>
+      <c r="AH81" s="7"/>
+      <c r="AI81" s="7"/>
+      <c r="AJ81" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK81" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="82" spans="1:37">
+      <c r="A82" s="3">
+        <v>80</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C82" s="3">
+        <v>2025062181</v>
+      </c>
+      <c r="D82" s="3"/>
+      <c r="E82" s="3"/>
+      <c r="F82" s="3">
+        <v>3772</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>584</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I82" s="3"/>
+      <c r="J82" s="3"/>
+      <c r="K82" s="3"/>
+      <c r="L82" s="3"/>
+      <c r="M82" s="4"/>
+      <c r="N82" s="3"/>
+      <c r="O82" s="4"/>
+      <c r="P82" s="10"/>
+      <c r="Q82" s="3" t="s">
+        <v>585</v>
+      </c>
+      <c r="R82" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S82" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T82" s="3">
+        <v>1</v>
+      </c>
+      <c r="U82" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V82" s="3" t="s">
+        <v>586</v>
+      </c>
+      <c r="W82" s="3" t="s">
+        <v>587</v>
+      </c>
+      <c r="X82" s="3" t="s">
+        <v>588</v>
+      </c>
+      <c r="Y82" s="3"/>
+      <c r="Z82" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA82" s="3"/>
+      <c r="AB82" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC82" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD82" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE82" s="3"/>
+      <c r="AF82" s="3"/>
+      <c r="AG82" s="3"/>
+      <c r="AH82" s="3"/>
+      <c r="AI82" s="3"/>
+      <c r="AJ82" s="3"/>
+      <c r="AK82" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="83" spans="1:37">
+      <c r="A83" s="7">
+        <v>81</v>
+      </c>
+      <c r="B83" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C83" s="7">
+        <v>2025062183</v>
+      </c>
+      <c r="D83" s="7"/>
+      <c r="E83" s="7"/>
+      <c r="F83" s="7">
+        <v>4680</v>
+      </c>
+      <c r="G83" s="7" t="s">
+        <v>553</v>
+      </c>
+      <c r="H83" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I83" s="7"/>
+      <c r="J83" s="7"/>
+      <c r="K83" s="7"/>
+      <c r="L83" s="7"/>
+      <c r="M83" s="8"/>
+      <c r="N83" s="7"/>
+      <c r="O83" s="8"/>
+      <c r="P83" s="9"/>
+      <c r="Q83" s="7" t="s">
+        <v>556</v>
+      </c>
+      <c r="R83" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S83" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T83" s="7">
+        <v>1</v>
+      </c>
+      <c r="U83" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V83" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="W83" s="7" t="s">
+        <v>558</v>
+      </c>
+      <c r="X83" s="7" t="s">
+        <v>559</v>
+      </c>
+      <c r="Y83" s="7"/>
+      <c r="Z83" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA83" s="7"/>
+      <c r="AB83" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC83" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD83" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE83" s="7"/>
+      <c r="AF83" s="7"/>
+      <c r="AG83" s="7"/>
+      <c r="AH83" s="7"/>
+      <c r="AI83" s="7"/>
+      <c r="AJ83" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK83" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="84" spans="1:37">
+      <c r="A84" s="3">
+        <v>82</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C84" s="3">
+        <v>2025062190</v>
+      </c>
+      <c r="D84" s="3"/>
+      <c r="E84" s="3"/>
+      <c r="F84" s="3">
+        <v>2746</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>590</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I84" s="3"/>
+      <c r="J84" s="3"/>
+      <c r="K84" s="3"/>
+      <c r="L84" s="3"/>
+      <c r="M84" s="4"/>
+      <c r="N84" s="3"/>
+      <c r="O84" s="4"/>
+      <c r="P84" s="10"/>
+      <c r="Q84" s="3" t="s">
+        <v>591</v>
+      </c>
+      <c r="R84" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S84" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T84" s="3">
+        <v>1</v>
+      </c>
+      <c r="U84" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V84" s="3" t="s">
+        <v>592</v>
+      </c>
+      <c r="W84" s="3" t="s">
+        <v>593</v>
+      </c>
+      <c r="X84" s="3" t="s">
+        <v>594</v>
+      </c>
+      <c r="Y84" s="3"/>
+      <c r="Z84" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA84" s="3"/>
+      <c r="AB84" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC84" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD84" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE84" s="3"/>
+      <c r="AF84" s="3"/>
+      <c r="AG84" s="3"/>
+      <c r="AH84" s="3"/>
+      <c r="AI84" s="3"/>
+      <c r="AJ84" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK84" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="85" spans="1:37">
+      <c r="A85" s="7">
+        <v>83</v>
+      </c>
+      <c r="B85" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C85" s="7">
+        <v>2025062191</v>
+      </c>
+      <c r="D85" s="7"/>
+      <c r="E85" s="7"/>
+      <c r="F85" s="7">
+        <v>3957</v>
+      </c>
+      <c r="G85" s="7" t="s">
+        <v>595</v>
+      </c>
+      <c r="H85" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I85" s="7"/>
+      <c r="J85" s="7"/>
+      <c r="K85" s="7"/>
+      <c r="L85" s="7"/>
+      <c r="M85" s="8"/>
+      <c r="N85" s="7"/>
+      <c r="O85" s="8"/>
+      <c r="P85" s="8"/>
+      <c r="Q85" s="7" t="s">
+        <v>596</v>
+      </c>
+      <c r="R85" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S85" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T85" s="7">
+        <v>1</v>
+      </c>
+      <c r="U85" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V85" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="W85" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="X85" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="Y85" s="7"/>
+      <c r="Z85" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA85" s="7"/>
+      <c r="AB85" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC85" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD85" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE85" s="7"/>
+      <c r="AF85" s="7"/>
+      <c r="AG85" s="7"/>
+      <c r="AH85" s="7"/>
+      <c r="AI85" s="7"/>
+      <c r="AJ85" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK85" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 18-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$88</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$91</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="626">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-17  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="653">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-18  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -1863,6 +1863,41 @@
     <t>2025-06-16 16:38:00</t>
   </si>
   <si>
+    <t>E4316114061701</t>
+  </si>
+  <si>
+    <t>2025-06-17 06:49:48</t>
+  </si>
+  <si>
+    <t>HL28</t>
+  </si>
+  <si>
+    <t>HL-立式掃描器</t>
+  </si>
+  <si>
+    <t>掃瞄無反應或感應不良</t>
+  </si>
+  <si>
+    <t>門市tm2太空寶寶(MS-7580)刷讀所有條碼無反應有亮燈有逼聲，門市已有操作過掃描器校正仍異常....須請台芝到店協助(壞?)</t>
+  </si>
+  <si>
+    <t>2025-06-17 09:18:24</t>
+  </si>
+  <si>
+    <t>2025-06-18 09:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-18 10:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-18 13:18:00</t>
+  </si>
+  <si>
+    <t>更換立式掃描器
+換上8118001686
+換下8118001303</t>
+  </si>
+  <si>
     <t>E2759114061701</t>
   </si>
   <si>
@@ -1893,6 +1928,39 @@
     <t>重新啟動網路連線及設定皆為正常</t>
   </si>
   <si>
+    <t>1D767114061701</t>
+  </si>
+  <si>
+    <t>D767</t>
+  </si>
+  <si>
+    <t>板橋寶翠店</t>
+  </si>
+  <si>
+    <t>2025-06-17 10:18:19</t>
+  </si>
+  <si>
+    <t>門市反應MMK4代機無網路顯示尚未偵測到網路，門市已重開機多次且確認畫面未跳出設定介面視窗，PING60不通....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF0D767</t>
+  </si>
+  <si>
+    <t>2025-06-17 10:20:53</t>
+  </si>
+  <si>
+    <t>2025-06-18 11:15:00</t>
+  </si>
+  <si>
+    <t>2025-06-18 11:39:00</t>
+  </si>
+  <si>
+    <t>2025-06-18 14:20:00</t>
+  </si>
+  <si>
+    <t>MMK網路設定介面重設後正常</t>
+  </si>
+  <si>
     <t>12399114061701</t>
   </si>
   <si>
@@ -1942,6 +2010,21 @@
   </si>
   <si>
     <t>Switch7號孔8號孔接反</t>
+  </si>
+  <si>
+    <t>五股福鑫店</t>
+  </si>
+  <si>
+    <t>THILF03921</t>
+  </si>
+  <si>
+    <t>2025-06-18 11:18:15</t>
+  </si>
+  <si>
+    <t>2025-06-18 10:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-18 11:20:00</t>
   </si>
 </sst>
 </file>
@@ -2355,10 +2438,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK88"/>
+  <dimension ref="A1:AK91"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC85" sqref="AC85"/>
+      <selection activeCell="A91" sqref="A91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -9543,7 +9626,7 @@
         <v>38</v>
       </c>
       <c r="C86" s="3">
-        <v>2025062222</v>
+        <v>2025062220</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>599</v>
@@ -9552,46 +9635,46 @@
         <v>40</v>
       </c>
       <c r="F86" s="3">
-        <v>2759</v>
+        <v>4316</v>
       </c>
       <c r="G86" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I86" s="3" t="s">
         <v>600</v>
-      </c>
-      <c r="H86" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I86" s="3" t="s">
-        <v>601</v>
       </c>
       <c r="J86" s="3" t="s">
         <v>171</v>
       </c>
       <c r="K86" s="3" t="s">
-        <v>66</v>
+        <v>326</v>
       </c>
       <c r="L86" s="3" t="s">
-        <v>313</v>
+        <v>601</v>
       </c>
       <c r="M86" s="4" t="s">
-        <v>314</v>
+        <v>602</v>
       </c>
       <c r="N86" s="3">
-        <v>5804</v>
+        <v>2803</v>
       </c>
       <c r="O86" s="4" t="s">
-        <v>175</v>
+        <v>603</v>
       </c>
       <c r="P86" s="10" t="s">
-        <v>602</v>
+        <v>604</v>
       </c>
       <c r="Q86" s="3" t="s">
-        <v>603</v>
+        <v>257</v>
       </c>
       <c r="R86" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S86" s="3" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="T86" s="3">
         <v>1</v>
@@ -9600,26 +9683,26 @@
         <v>53</v>
       </c>
       <c r="V86" s="3" t="s">
-        <v>604</v>
+        <v>605</v>
       </c>
       <c r="W86" s="3" t="s">
-        <v>605</v>
+        <v>606</v>
       </c>
       <c r="X86" s="3" t="s">
-        <v>606</v>
+        <v>607</v>
       </c>
       <c r="Y86" s="3" t="s">
-        <v>607</v>
+        <v>608</v>
       </c>
       <c r="Z86" s="3">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="AA86" s="3"/>
       <c r="AB86" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC86" s="10" t="s">
-        <v>608</v>
+        <v>609</v>
       </c>
       <c r="AD86" s="3"/>
       <c r="AE86" s="3"/>
@@ -9640,25 +9723,25 @@
         <v>38</v>
       </c>
       <c r="C87" s="7">
-        <v>2025062232</v>
+        <v>2025062222</v>
       </c>
       <c r="D87" s="7" t="s">
-        <v>609</v>
+        <v>610</v>
       </c>
       <c r="E87" s="7" t="s">
         <v>40</v>
       </c>
       <c r="F87" s="7">
-        <v>2399</v>
+        <v>2759</v>
       </c>
       <c r="G87" s="7" t="s">
-        <v>610</v>
+        <v>611</v>
       </c>
       <c r="H87" s="7" t="s">
         <v>42</v>
       </c>
       <c r="I87" s="7" t="s">
-        <v>611</v>
+        <v>612</v>
       </c>
       <c r="J87" s="7" t="s">
         <v>171</v>
@@ -9679,10 +9762,10 @@
         <v>175</v>
       </c>
       <c r="P87" s="9" t="s">
-        <v>612</v>
+        <v>613</v>
       </c>
       <c r="Q87" s="7" t="s">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="R87" s="7" t="s">
         <v>51</v>
@@ -9697,16 +9780,16 @@
         <v>53</v>
       </c>
       <c r="V87" s="7" t="s">
-        <v>614</v>
+        <v>615</v>
       </c>
       <c r="W87" s="7" t="s">
-        <v>615</v>
+        <v>616</v>
       </c>
       <c r="X87" s="7" t="s">
-        <v>616</v>
+        <v>617</v>
       </c>
       <c r="Y87" s="7" t="s">
-        <v>617</v>
+        <v>618</v>
       </c>
       <c r="Z87" s="7">
         <v>0.5</v>
@@ -9716,7 +9799,7 @@
         <v>58</v>
       </c>
       <c r="AC87" s="9" t="s">
-        <v>608</v>
+        <v>619</v>
       </c>
       <c r="AD87" s="7"/>
       <c r="AE87" s="7"/>
@@ -9737,25 +9820,25 @@
         <v>38</v>
       </c>
       <c r="C88" s="3">
-        <v>2025062243</v>
+        <v>2025062231</v>
       </c>
       <c r="D88" s="3" t="s">
-        <v>618</v>
+        <v>620</v>
       </c>
       <c r="E88" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="F88" s="3">
-        <v>3601</v>
+      <c r="F88" s="3" t="s">
+        <v>621</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>442</v>
+        <v>622</v>
       </c>
       <c r="H88" s="3" t="s">
-        <v>42</v>
+        <v>123</v>
       </c>
       <c r="I88" s="3" t="s">
-        <v>619</v>
+        <v>623</v>
       </c>
       <c r="J88" s="3" t="s">
         <v>171</v>
@@ -9775,17 +9858,17 @@
       <c r="O88" s="4" t="s">
         <v>175</v>
       </c>
-      <c r="P88" s="4" t="s">
-        <v>620</v>
+      <c r="P88" s="10" t="s">
+        <v>624</v>
       </c>
       <c r="Q88" s="3" t="s">
-        <v>443</v>
+        <v>625</v>
       </c>
       <c r="R88" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S88" s="3" t="s">
-        <v>52</v>
+        <v>125</v>
       </c>
       <c r="T88" s="3">
         <v>1</v>
@@ -9794,26 +9877,26 @@
         <v>53</v>
       </c>
       <c r="V88" s="3" t="s">
-        <v>621</v>
+        <v>626</v>
       </c>
       <c r="W88" s="3" t="s">
-        <v>622</v>
+        <v>627</v>
       </c>
       <c r="X88" s="3" t="s">
-        <v>623</v>
+        <v>628</v>
       </c>
       <c r="Y88" s="3" t="s">
-        <v>624</v>
+        <v>629</v>
       </c>
       <c r="Z88" s="3">
-        <v>0.5</v>
+        <v>0.4</v>
       </c>
       <c r="AA88" s="3"/>
       <c r="AB88" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC88" s="4" t="s">
-        <v>625</v>
+      <c r="AC88" s="10" t="s">
+        <v>630</v>
       </c>
       <c r="AD88" s="3"/>
       <c r="AE88" s="3"/>
@@ -9823,6 +9906,277 @@
       <c r="AI88" s="3"/>
       <c r="AJ88" s="3"/>
       <c r="AK88" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="89" spans="1:37">
+      <c r="A89" s="7">
+        <v>87</v>
+      </c>
+      <c r="B89" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C89" s="7">
+        <v>2025062232</v>
+      </c>
+      <c r="D89" s="7" t="s">
+        <v>631</v>
+      </c>
+      <c r="E89" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F89" s="7">
+        <v>2399</v>
+      </c>
+      <c r="G89" s="7" t="s">
+        <v>632</v>
+      </c>
+      <c r="H89" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I89" s="7" t="s">
+        <v>633</v>
+      </c>
+      <c r="J89" s="7" t="s">
+        <v>171</v>
+      </c>
+      <c r="K89" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L89" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="M89" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="N89" s="7">
+        <v>5804</v>
+      </c>
+      <c r="O89" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="P89" s="9" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q89" s="7" t="s">
+        <v>635</v>
+      </c>
+      <c r="R89" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S89" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T89" s="7">
+        <v>1</v>
+      </c>
+      <c r="U89" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V89" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="W89" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="X89" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="Y89" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="Z89" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA89" s="7"/>
+      <c r="AB89" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC89" s="9" t="s">
+        <v>619</v>
+      </c>
+      <c r="AD89" s="7"/>
+      <c r="AE89" s="7"/>
+      <c r="AF89" s="7"/>
+      <c r="AG89" s="7"/>
+      <c r="AH89" s="7"/>
+      <c r="AI89" s="7"/>
+      <c r="AJ89" s="7"/>
+      <c r="AK89" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="90" spans="1:37">
+      <c r="A90" s="3">
+        <v>88</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C90" s="3">
+        <v>2025062243</v>
+      </c>
+      <c r="D90" s="3" t="s">
+        <v>640</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F90" s="3">
+        <v>3601</v>
+      </c>
+      <c r="G90" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="H90" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I90" s="3" t="s">
+        <v>641</v>
+      </c>
+      <c r="J90" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K90" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L90" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="M90" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="N90" s="3">
+        <v>5804</v>
+      </c>
+      <c r="O90" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P90" s="10" t="s">
+        <v>642</v>
+      </c>
+      <c r="Q90" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="R90" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S90" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T90" s="3">
+        <v>1</v>
+      </c>
+      <c r="U90" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V90" s="3" t="s">
+        <v>643</v>
+      </c>
+      <c r="W90" s="3" t="s">
+        <v>644</v>
+      </c>
+      <c r="X90" s="3" t="s">
+        <v>645</v>
+      </c>
+      <c r="Y90" s="3" t="s">
+        <v>646</v>
+      </c>
+      <c r="Z90" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA90" s="3"/>
+      <c r="AB90" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC90" s="10" t="s">
+        <v>647</v>
+      </c>
+      <c r="AD90" s="3"/>
+      <c r="AE90" s="3"/>
+      <c r="AF90" s="3"/>
+      <c r="AG90" s="3"/>
+      <c r="AH90" s="3"/>
+      <c r="AI90" s="3"/>
+      <c r="AJ90" s="3"/>
+      <c r="AK90" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="91" spans="1:37">
+      <c r="A91" s="7">
+        <v>89</v>
+      </c>
+      <c r="B91" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C91" s="7">
+        <v>2025062379</v>
+      </c>
+      <c r="D91" s="7"/>
+      <c r="E91" s="7"/>
+      <c r="F91" s="7">
+        <v>3921</v>
+      </c>
+      <c r="G91" s="7" t="s">
+        <v>648</v>
+      </c>
+      <c r="H91" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I91" s="7"/>
+      <c r="J91" s="7"/>
+      <c r="K91" s="7"/>
+      <c r="L91" s="7"/>
+      <c r="M91" s="8"/>
+      <c r="N91" s="7"/>
+      <c r="O91" s="8"/>
+      <c r="P91" s="8"/>
+      <c r="Q91" s="7" t="s">
+        <v>649</v>
+      </c>
+      <c r="R91" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S91" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T91" s="7">
+        <v>1</v>
+      </c>
+      <c r="U91" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V91" s="7" t="s">
+        <v>650</v>
+      </c>
+      <c r="W91" s="7" t="s">
+        <v>651</v>
+      </c>
+      <c r="X91" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="Y91" s="7"/>
+      <c r="Z91" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA91" s="7"/>
+      <c r="AB91" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC91" s="8" t="s">
+        <v>421</v>
+      </c>
+      <c r="AD91" s="7"/>
+      <c r="AE91" s="7"/>
+      <c r="AF91" s="7"/>
+      <c r="AG91" s="7"/>
+      <c r="AH91" s="7"/>
+      <c r="AI91" s="7"/>
+      <c r="AJ91" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK91" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 20-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$96</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$104</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="698">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-18  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="745">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-20  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2166,6 +2166,150 @@
     <t>更換掃描槍
 換下8119006304
 換上8119012065</t>
+  </si>
+  <si>
+    <t>12306114061901</t>
+  </si>
+  <si>
+    <t>八里凱旋門</t>
+  </si>
+  <si>
+    <t>2025-06-19 09:34:44</t>
+  </si>
+  <si>
+    <t>D302</t>
+  </si>
+  <si>
+    <t>發票印字不清</t>
+  </si>
+  <si>
+    <t>門市反應tm2熱感發票機(BSC10II)印出一條白線，已有關機紙捲重裝仍異常...請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF02306</t>
+  </si>
+  <si>
+    <t>2025-06-19 09:36:26</t>
+  </si>
+  <si>
+    <t>2025-06-20 09:39:00</t>
+  </si>
+  <si>
+    <t>2025-06-20 10:09:00</t>
+  </si>
+  <si>
+    <t>2025-06-20 13:36:00</t>
+  </si>
+  <si>
+    <t>熱感頭清潔異物後列印正常(發票黑色袋)</t>
+  </si>
+  <si>
+    <t>E5352114061801</t>
+  </si>
+  <si>
+    <t>三重重陽店</t>
+  </si>
+  <si>
+    <t>2025-06-18 23:30:06</t>
+  </si>
+  <si>
+    <t xml:space="preserve">6/19 09:40啟動緊急叫修：SC(SHUTTLE6S)開啟程式緩慢，門市TM主檔在6/18，請通訊功評確認：SC主機第二顆硬碟異常WDC WD10SPZX-22Z10T1  \\\\.\\PHYSICALDRIVE1  1000202273280 已重試磁碟 1 (PDO 名稱: \\Device\\00000035) 邏輯區塊位址 0x15035f 上的 IO 操作。請派工到店更換SC第二顆硬碟不備份還原。攜帶第一顆硬碟備用...請台芝到店協助PS.若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 與門市確認最後一天帳關到6/18，與通訊嘉芳確認銷售有收到，無TM1.2電子存根聯(後場電腦當機沒反應 倒致TM無法使用 麻煩來檢查)
+</t>
+  </si>
+  <si>
+    <t>THILF05352</t>
+  </si>
+  <si>
+    <t>2025-06-19 09:44:42</t>
+  </si>
+  <si>
+    <t>2025-06-19 12:47:00</t>
+  </si>
+  <si>
+    <t>2025-06-19 13:17:00</t>
+  </si>
+  <si>
+    <t>2025-06-19 15:44:00</t>
+  </si>
+  <si>
+    <t>13890114061901</t>
+  </si>
+  <si>
+    <t>2025-06-19 11:21:50</t>
+  </si>
+  <si>
+    <t>無電源反應、無法開機</t>
+  </si>
+  <si>
+    <t>門市反應今日一到門市查看TM2(TCX800)就無電源反應無法開機，重新拔插線路仍異常，已確認粉色插座及白色插座皆有過電，ping81不通無法vnc....請台芝到店協助
+已與門市確認6/19尚未清帳 PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對) 
+※非24H營業門市，周一公休，營業時間:周二至周日0700~1500</t>
+  </si>
+  <si>
+    <t>2025-06-19 11:25:28</t>
+  </si>
+  <si>
+    <t>2025-06-19 13:43:00</t>
+  </si>
+  <si>
+    <t>2025-06-19 14:13:00</t>
+  </si>
+  <si>
+    <t>2025-06-20 15:25:00</t>
+  </si>
+  <si>
+    <t>取消叫修</t>
+  </si>
+  <si>
+    <t>可正常使用已取消報修</t>
+  </si>
+  <si>
+    <t>新莊昌平店</t>
+  </si>
+  <si>
+    <t>THILF04701</t>
+  </si>
+  <si>
+    <t>2025-06-19 13:38:58</t>
+  </si>
+  <si>
+    <t>2025-06-19 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-19 13:40:00</t>
+  </si>
+  <si>
+    <t>新莊幸運店</t>
+  </si>
+  <si>
+    <t>THILF04679</t>
+  </si>
+  <si>
+    <t>2025-06-19 14:04:52</t>
+  </si>
+  <si>
+    <t>2025-06-19 13:45:00</t>
+  </si>
+  <si>
+    <t>2025-06-19 14:10:00</t>
+  </si>
+  <si>
+    <t>2025-06-20 09:48:47</t>
+  </si>
+  <si>
+    <t>2025-06-20 08:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-20 08:45:00</t>
+  </si>
+  <si>
+    <t>2025-06-20 09:50:13</t>
+  </si>
+  <si>
+    <t>2025-06-20 09:51:10</t>
+  </si>
+  <si>
+    <t>2025-06-20 09:00:00</t>
   </si>
 </sst>
 </file>
@@ -2579,10 +2723,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK96"/>
+  <dimension ref="A1:AK104"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC93" sqref="AC93"/>
+      <selection activeCell="AC101" sqref="AC101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -10755,7 +10899,7 @@
       <c r="O96" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="P96" s="4" t="s">
+      <c r="P96" s="10" t="s">
         <v>693</v>
       </c>
       <c r="Q96" s="3" t="s">
@@ -10792,7 +10936,7 @@
       <c r="AB96" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC96" s="4" t="s">
+      <c r="AC96" s="10" t="s">
         <v>697</v>
       </c>
       <c r="AD96" s="3"/>
@@ -10803,6 +10947,680 @@
       <c r="AI96" s="3"/>
       <c r="AJ96" s="3"/>
       <c r="AK96" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="97" spans="1:37">
+      <c r="A97" s="7">
+        <v>95</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C97" s="7">
+        <v>2025062506</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>698</v>
+      </c>
+      <c r="E97" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F97" s="7">
+        <v>2306</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>699</v>
+      </c>
+      <c r="H97" s="7" t="s">
+        <v>237</v>
+      </c>
+      <c r="I97" s="7" t="s">
+        <v>700</v>
+      </c>
+      <c r="J97" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K97" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L97" s="7" t="s">
+        <v>146</v>
+      </c>
+      <c r="M97" s="8" t="s">
+        <v>147</v>
+      </c>
+      <c r="N97" s="7" t="s">
+        <v>701</v>
+      </c>
+      <c r="O97" s="8" t="s">
+        <v>702</v>
+      </c>
+      <c r="P97" s="9" t="s">
+        <v>703</v>
+      </c>
+      <c r="Q97" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="R97" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S97" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T97" s="7">
+        <v>1</v>
+      </c>
+      <c r="U97" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V97" s="7" t="s">
+        <v>705</v>
+      </c>
+      <c r="W97" s="7" t="s">
+        <v>706</v>
+      </c>
+      <c r="X97" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="Y97" s="7" t="s">
+        <v>708</v>
+      </c>
+      <c r="Z97" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA97" s="7"/>
+      <c r="AB97" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC97" s="9" t="s">
+        <v>709</v>
+      </c>
+      <c r="AD97" s="7"/>
+      <c r="AE97" s="7"/>
+      <c r="AF97" s="7"/>
+      <c r="AG97" s="7"/>
+      <c r="AH97" s="7"/>
+      <c r="AI97" s="7"/>
+      <c r="AJ97" s="7"/>
+      <c r="AK97" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="98" spans="1:37">
+      <c r="A98" s="3">
+        <v>96</v>
+      </c>
+      <c r="B98" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C98" s="3">
+        <v>2025062512</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>710</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F98" s="3">
+        <v>5352</v>
+      </c>
+      <c r="G98" s="3" t="s">
+        <v>711</v>
+      </c>
+      <c r="H98" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I98" s="3" t="s">
+        <v>712</v>
+      </c>
+      <c r="J98" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="K98" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L98" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="M98" s="4" t="s">
+        <v>225</v>
+      </c>
+      <c r="N98" s="3">
+        <v>2405</v>
+      </c>
+      <c r="O98" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="P98" s="10" t="s">
+        <v>713</v>
+      </c>
+      <c r="Q98" s="3" t="s">
+        <v>714</v>
+      </c>
+      <c r="R98" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S98" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T98" s="3">
+        <v>1</v>
+      </c>
+      <c r="U98" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V98" s="3" t="s">
+        <v>715</v>
+      </c>
+      <c r="W98" s="3" t="s">
+        <v>716</v>
+      </c>
+      <c r="X98" s="3" t="s">
+        <v>717</v>
+      </c>
+      <c r="Y98" s="3" t="s">
+        <v>718</v>
+      </c>
+      <c r="Z98" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA98" s="3"/>
+      <c r="AB98" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC98" s="10" t="s">
+        <v>245</v>
+      </c>
+      <c r="AD98" s="3"/>
+      <c r="AE98" s="3"/>
+      <c r="AF98" s="3"/>
+      <c r="AG98" s="3"/>
+      <c r="AH98" s="3"/>
+      <c r="AI98" s="3"/>
+      <c r="AJ98" s="3"/>
+      <c r="AK98" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="99" spans="1:37">
+      <c r="A99" s="7">
+        <v>97</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C99" s="7">
+        <v>2025062555</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>719</v>
+      </c>
+      <c r="E99" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F99" s="7">
+        <v>3890</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>344</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I99" s="7" t="s">
+        <v>720</v>
+      </c>
+      <c r="J99" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K99" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L99" s="7" t="s">
+        <v>112</v>
+      </c>
+      <c r="M99" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="N99" s="7">
+        <v>2306</v>
+      </c>
+      <c r="O99" s="8" t="s">
+        <v>721</v>
+      </c>
+      <c r="P99" s="9" t="s">
+        <v>722</v>
+      </c>
+      <c r="Q99" s="7" t="s">
+        <v>347</v>
+      </c>
+      <c r="R99" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S99" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T99" s="7">
+        <v>1</v>
+      </c>
+      <c r="U99" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V99" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="W99" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="X99" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="Y99" s="7" t="s">
+        <v>726</v>
+      </c>
+      <c r="Z99" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA99" s="7"/>
+      <c r="AB99" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="AC99" s="9" t="s">
+        <v>728</v>
+      </c>
+      <c r="AD99" s="7"/>
+      <c r="AE99" s="7"/>
+      <c r="AF99" s="7"/>
+      <c r="AG99" s="7"/>
+      <c r="AH99" s="7"/>
+      <c r="AI99" s="7"/>
+      <c r="AJ99" s="7"/>
+      <c r="AK99" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="100" spans="1:37">
+      <c r="A100" s="3">
+        <v>98</v>
+      </c>
+      <c r="B100" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C100" s="3">
+        <v>2025062562</v>
+      </c>
+      <c r="D100" s="3"/>
+      <c r="E100" s="3"/>
+      <c r="F100" s="3">
+        <v>4701</v>
+      </c>
+      <c r="G100" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="H100" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I100" s="3"/>
+      <c r="J100" s="3"/>
+      <c r="K100" s="3"/>
+      <c r="L100" s="3"/>
+      <c r="M100" s="4"/>
+      <c r="N100" s="3"/>
+      <c r="O100" s="4"/>
+      <c r="P100" s="10"/>
+      <c r="Q100" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="R100" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S100" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T100" s="3">
+        <v>1</v>
+      </c>
+      <c r="U100" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V100" s="3" t="s">
+        <v>731</v>
+      </c>
+      <c r="W100" s="3" t="s">
+        <v>732</v>
+      </c>
+      <c r="X100" s="3" t="s">
+        <v>733</v>
+      </c>
+      <c r="Y100" s="3"/>
+      <c r="Z100" s="3">
+        <v>0.7</v>
+      </c>
+      <c r="AA100" s="3"/>
+      <c r="AB100" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC100" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD100" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE100" s="3"/>
+      <c r="AF100" s="3"/>
+      <c r="AG100" s="3"/>
+      <c r="AH100" s="3"/>
+      <c r="AI100" s="3"/>
+      <c r="AJ100" s="3"/>
+      <c r="AK100" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="101" spans="1:37">
+      <c r="A101" s="7">
+        <v>99</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C101" s="7">
+        <v>2025062570</v>
+      </c>
+      <c r="D101" s="7"/>
+      <c r="E101" s="7"/>
+      <c r="F101" s="7">
+        <v>4679</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>734</v>
+      </c>
+      <c r="H101" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I101" s="7"/>
+      <c r="J101" s="7"/>
+      <c r="K101" s="7"/>
+      <c r="L101" s="7"/>
+      <c r="M101" s="8"/>
+      <c r="N101" s="7"/>
+      <c r="O101" s="8"/>
+      <c r="P101" s="9"/>
+      <c r="Q101" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="R101" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S101" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T101" s="7">
+        <v>1</v>
+      </c>
+      <c r="U101" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V101" s="7" t="s">
+        <v>736</v>
+      </c>
+      <c r="W101" s="7" t="s">
+        <v>737</v>
+      </c>
+      <c r="X101" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="Y101" s="7"/>
+      <c r="Z101" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA101" s="7"/>
+      <c r="AB101" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC101" s="9" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD101" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE101" s="7"/>
+      <c r="AF101" s="7"/>
+      <c r="AG101" s="7"/>
+      <c r="AH101" s="7"/>
+      <c r="AI101" s="7"/>
+      <c r="AJ101" s="7"/>
+      <c r="AK101" s="7"/>
+    </row>
+    <row r="102" spans="1:37">
+      <c r="A102" s="3">
+        <v>100</v>
+      </c>
+      <c r="B102" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C102" s="3">
+        <v>2025062645</v>
+      </c>
+      <c r="D102" s="3"/>
+      <c r="E102" s="3"/>
+      <c r="F102" s="3">
+        <v>4701</v>
+      </c>
+      <c r="G102" s="3" t="s">
+        <v>729</v>
+      </c>
+      <c r="H102" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I102" s="3"/>
+      <c r="J102" s="3"/>
+      <c r="K102" s="3"/>
+      <c r="L102" s="3"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="3"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="10"/>
+      <c r="Q102" s="3" t="s">
+        <v>730</v>
+      </c>
+      <c r="R102" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S102" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T102" s="3">
+        <v>1</v>
+      </c>
+      <c r="U102" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V102" s="3" t="s">
+        <v>739</v>
+      </c>
+      <c r="W102" s="3" t="s">
+        <v>740</v>
+      </c>
+      <c r="X102" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="Y102" s="3"/>
+      <c r="Z102" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA102" s="3"/>
+      <c r="AB102" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC102" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD102" s="3"/>
+      <c r="AE102" s="3"/>
+      <c r="AF102" s="3"/>
+      <c r="AG102" s="3"/>
+      <c r="AH102" s="3"/>
+      <c r="AI102" s="3"/>
+      <c r="AJ102" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK102" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="103" spans="1:37">
+      <c r="A103" s="7">
+        <v>101</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C103" s="7">
+        <v>2025062646</v>
+      </c>
+      <c r="D103" s="7"/>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7">
+        <v>4701</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>729</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I103" s="7"/>
+      <c r="J103" s="7"/>
+      <c r="K103" s="7"/>
+      <c r="L103" s="7"/>
+      <c r="M103" s="8"/>
+      <c r="N103" s="7"/>
+      <c r="O103" s="8"/>
+      <c r="P103" s="9"/>
+      <c r="Q103" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="R103" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S103" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T103" s="7">
+        <v>1</v>
+      </c>
+      <c r="U103" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V103" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="W103" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="X103" s="7" t="s">
+        <v>741</v>
+      </c>
+      <c r="Y103" s="7"/>
+      <c r="Z103" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA103" s="7"/>
+      <c r="AB103" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC103" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD103" s="7"/>
+      <c r="AE103" s="7"/>
+      <c r="AF103" s="7"/>
+      <c r="AG103" s="7"/>
+      <c r="AH103" s="7"/>
+      <c r="AI103" s="7"/>
+      <c r="AJ103" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK103" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="104" spans="1:37">
+      <c r="A104" s="3">
+        <v>102</v>
+      </c>
+      <c r="B104" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C104" s="3">
+        <v>2025062647</v>
+      </c>
+      <c r="D104" s="3"/>
+      <c r="E104" s="3"/>
+      <c r="F104" s="3">
+        <v>4679</v>
+      </c>
+      <c r="G104" s="3" t="s">
+        <v>734</v>
+      </c>
+      <c r="H104" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I104" s="3"/>
+      <c r="J104" s="3"/>
+      <c r="K104" s="3"/>
+      <c r="L104" s="3"/>
+      <c r="M104" s="4"/>
+      <c r="N104" s="3"/>
+      <c r="O104" s="4"/>
+      <c r="P104" s="4"/>
+      <c r="Q104" s="3" t="s">
+        <v>735</v>
+      </c>
+      <c r="R104" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S104" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T104" s="3">
+        <v>1</v>
+      </c>
+      <c r="U104" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V104" s="3" t="s">
+        <v>743</v>
+      </c>
+      <c r="W104" s="3" t="s">
+        <v>741</v>
+      </c>
+      <c r="X104" s="3" t="s">
+        <v>744</v>
+      </c>
+      <c r="Y104" s="3"/>
+      <c r="Z104" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA104" s="3"/>
+      <c r="AB104" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC104" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD104" s="3"/>
+      <c r="AE104" s="3"/>
+      <c r="AF104" s="3"/>
+      <c r="AG104" s="3"/>
+      <c r="AH104" s="3"/>
+      <c r="AI104" s="3"/>
+      <c r="AJ104" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK104" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 23-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$109</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$110</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="777">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-20  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="789">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-23  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2409,6 +2409,44 @@
   </si>
   <si>
     <t>2025-06-20 14:40:00</t>
+  </si>
+  <si>
+    <t>E4739114062101</t>
+  </si>
+  <si>
+    <t>淡水櫻花店</t>
+  </si>
+  <si>
+    <t>2025-06-21 06:16:38</t>
+  </si>
+  <si>
+    <t>D308</t>
+  </si>
+  <si>
+    <t>上蓋打不開</t>
+  </si>
+  <si>
+    <t>2025/06/21  09:03 萊爾富百大門市啟動緊急叫修: 門市反應tm1熱感發票機(BSC10)上一筆明細未列印完成，上蓋打開後無法合起來，門市告知無法自行排除...台芝到店協助(印明細出來卡住沒印出來就故障，上蓋打開就無法蓋回去)</t>
+  </si>
+  <si>
+    <t>THILF04739</t>
+  </si>
+  <si>
+    <t>2025-06-21 09:17:59</t>
+  </si>
+  <si>
+    <t>2025-06-21 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-21 13:57:00</t>
+  </si>
+  <si>
+    <t>2025-06-21 15:17:00</t>
+  </si>
+  <si>
+    <t>更換發票機
+換下8155003726
+換上8155006260</t>
   </si>
 </sst>
 </file>
@@ -2822,10 +2860,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK109"/>
+  <dimension ref="A1:AK110"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A109" sqref="A109"/>
+      <selection activeCell="AC107" sqref="AC107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12101,7 +12139,7 @@
       <c r="M109" s="8"/>
       <c r="N109" s="7"/>
       <c r="O109" s="8"/>
-      <c r="P109" s="8"/>
+      <c r="P109" s="9"/>
       <c r="Q109" s="7" t="s">
         <v>773</v>
       </c>
@@ -12134,7 +12172,7 @@
       <c r="AB109" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC109" s="8" t="s">
+      <c r="AC109" s="9" t="s">
         <v>421</v>
       </c>
       <c r="AD109" s="7"/>
@@ -12147,6 +12185,103 @@
         <v>60</v>
       </c>
       <c r="AK109" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="110" spans="1:37">
+      <c r="A110" s="3">
+        <v>108</v>
+      </c>
+      <c r="B110" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C110" s="3">
+        <v>2025062775</v>
+      </c>
+      <c r="D110" s="3" t="s">
+        <v>777</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="F110" s="3">
+        <v>4739</v>
+      </c>
+      <c r="G110" s="3" t="s">
+        <v>778</v>
+      </c>
+      <c r="H110" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I110" s="3" t="s">
+        <v>779</v>
+      </c>
+      <c r="J110" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K110" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="L110" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M110" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N110" s="3" t="s">
+        <v>780</v>
+      </c>
+      <c r="O110" s="4" t="s">
+        <v>781</v>
+      </c>
+      <c r="P110" s="4" t="s">
+        <v>782</v>
+      </c>
+      <c r="Q110" s="3" t="s">
+        <v>783</v>
+      </c>
+      <c r="R110" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S110" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T110" s="3">
+        <v>1</v>
+      </c>
+      <c r="U110" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V110" s="3" t="s">
+        <v>784</v>
+      </c>
+      <c r="W110" s="3" t="s">
+        <v>785</v>
+      </c>
+      <c r="X110" s="3" t="s">
+        <v>786</v>
+      </c>
+      <c r="Y110" s="3" t="s">
+        <v>787</v>
+      </c>
+      <c r="Z110" s="3">
+        <v>1</v>
+      </c>
+      <c r="AA110" s="3"/>
+      <c r="AB110" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC110" s="4" t="s">
+        <v>788</v>
+      </c>
+      <c r="AD110" s="3"/>
+      <c r="AE110" s="3"/>
+      <c r="AF110" s="3"/>
+      <c r="AG110" s="3"/>
+      <c r="AH110" s="3"/>
+      <c r="AI110" s="3"/>
+      <c r="AJ110" s="3"/>
+      <c r="AK110" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 24-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$114</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$120</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="821">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-23  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="853">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-24  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2514,6 +2514,38 @@
 換下81Z1001088</t>
   </si>
   <si>
+    <t>13840114062301</t>
+  </si>
+  <si>
+    <t>2025-06-23 14:07:53</t>
+  </si>
+  <si>
+    <t>門市反應TM2-CCD掃描器(HC76-TR)刷讀所有條碼都感應不良，有亮燈無嗶聲，嘗試執行掃描器校正，但刷讀第六段條碼都無反應..請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-06-23 14:09:42</t>
+  </si>
+  <si>
+    <t>2025-06-24 10:52:00</t>
+  </si>
+  <si>
+    <t>2025-06-24 11:22:00</t>
+  </si>
+  <si>
+    <t>2025-06-24 18:09:00</t>
+  </si>
+  <si>
+    <t>更換掃描槍
+換下8119011671
+換上8119012858</t>
+  </si>
+  <si>
+    <t>2025-06-24 10:54:00</t>
+  </si>
+  <si>
+    <t>2025-06-24 11:24:00</t>
+  </si>
+  <si>
     <t>三重高中店</t>
   </si>
   <si>
@@ -2545,6 +2577,72 @@
   </si>
   <si>
     <t>2025-06-23 15:35:00</t>
+  </si>
+  <si>
+    <t>D346</t>
+  </si>
+  <si>
+    <t>三重維德店</t>
+  </si>
+  <si>
+    <t>THILF0D346</t>
+  </si>
+  <si>
+    <t>2025-06-24 13:28:43</t>
+  </si>
+  <si>
+    <t>2025-06-24 12:50:00</t>
+  </si>
+  <si>
+    <t>2025-06-24 13:27:00</t>
+  </si>
+  <si>
+    <t>蘆洲希望店</t>
+  </si>
+  <si>
+    <t>THILF05354</t>
+  </si>
+  <si>
+    <t>2025-06-24 14:10:49</t>
+  </si>
+  <si>
+    <t>2025-06-24 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-24 14:00:00</t>
+  </si>
+  <si>
+    <t>D195</t>
+  </si>
+  <si>
+    <t>三重車路頭</t>
+  </si>
+  <si>
+    <t>THILF0D195</t>
+  </si>
+  <si>
+    <t>2025-06-24 14:19:55</t>
+  </si>
+  <si>
+    <t>2025-06-24 13:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-24 14:19:00</t>
+  </si>
+  <si>
+    <t>三重太璞宮</t>
+  </si>
+  <si>
+    <t>THILF04968</t>
+  </si>
+  <si>
+    <t>2025-06-24 15:16:29</t>
+  </si>
+  <si>
+    <t>2025-06-24 14:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-24 15:15:00</t>
   </si>
 </sst>
 </file>
@@ -2958,10 +3056,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK114"/>
+  <dimension ref="A1:AK120"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC111" sqref="AC111"/>
+      <selection activeCell="AC117" sqref="AC117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -12582,32 +12680,52 @@
         <v>111</v>
       </c>
       <c r="B113" s="7" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C113" s="7">
-        <v>2025062881</v>
-      </c>
-      <c r="D113" s="7"/>
-      <c r="E113" s="7"/>
+        <v>2025062880</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>810</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>40</v>
+      </c>
       <c r="F113" s="7">
-        <v>4260</v>
+        <v>3840</v>
       </c>
       <c r="G113" s="7" t="s">
-        <v>810</v>
+        <v>301</v>
       </c>
       <c r="H113" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="I113" s="7"/>
-      <c r="J113" s="7"/>
-      <c r="K113" s="7"/>
-      <c r="L113" s="7"/>
-      <c r="M113" s="8"/>
-      <c r="N113" s="7"/>
-      <c r="O113" s="8"/>
-      <c r="P113" s="9"/>
+      <c r="I113" s="7" t="s">
+        <v>811</v>
+      </c>
+      <c r="J113" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="K113" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L113" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="M113" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="N113" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="O113" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="P113" s="9" t="s">
+        <v>812</v>
+      </c>
       <c r="Q113" s="7" t="s">
-        <v>811</v>
+        <v>304</v>
       </c>
       <c r="R113" s="7" t="s">
         <v>51</v>
@@ -12622,29 +12740,29 @@
         <v>53</v>
       </c>
       <c r="V113" s="7" t="s">
-        <v>812</v>
+        <v>813</v>
       </c>
       <c r="W113" s="7" t="s">
-        <v>813</v>
+        <v>814</v>
       </c>
       <c r="X113" s="7" t="s">
-        <v>814</v>
-      </c>
-      <c r="Y113" s="7"/>
+        <v>815</v>
+      </c>
+      <c r="Y113" s="7" t="s">
+        <v>816</v>
+      </c>
       <c r="Z113" s="7">
-        <v>3</v>
+        <v>0.5</v>
       </c>
       <c r="AA113" s="7"/>
       <c r="AB113" s="7" t="s">
         <v>58</v>
       </c>
       <c r="AC113" s="9" t="s">
-        <v>815</v>
+        <v>817</v>
       </c>
       <c r="AD113" s="7"/>
-      <c r="AE113" s="7" t="s">
-        <v>60</v>
-      </c>
+      <c r="AE113" s="7"/>
       <c r="AF113" s="7"/>
       <c r="AG113" s="7"/>
       <c r="AH113" s="7"/>
@@ -12659,77 +12777,565 @@
         <v>112</v>
       </c>
       <c r="B114" s="3" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C114" s="3">
-        <v>2025062901</v>
-      </c>
-      <c r="D114" s="3"/>
-      <c r="E114" s="3"/>
+        <v>2025062880</v>
+      </c>
+      <c r="D114" s="3" t="s">
+        <v>810</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F114" s="3">
-        <v>2224</v>
+        <v>3840</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>816</v>
+        <v>301</v>
       </c>
       <c r="H114" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="I114" s="3"/>
-      <c r="J114" s="3"/>
-      <c r="K114" s="3"/>
-      <c r="L114" s="3"/>
-      <c r="M114" s="4"/>
-      <c r="N114" s="3"/>
-      <c r="O114" s="4"/>
-      <c r="P114" s="4"/>
+        <v>42</v>
+      </c>
+      <c r="I114" s="3" t="s">
+        <v>811</v>
+      </c>
+      <c r="J114" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="K114" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L114" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="M114" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="N114" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="O114" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="P114" s="10" t="s">
+        <v>812</v>
+      </c>
       <c r="Q114" s="3" t="s">
-        <v>817</v>
+        <v>304</v>
       </c>
       <c r="R114" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S114" s="3" t="s">
-        <v>125</v>
+        <v>52</v>
       </c>
       <c r="T114" s="3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U114" s="3" t="s">
         <v>53</v>
       </c>
       <c r="V114" s="3" t="s">
+        <v>813</v>
+      </c>
+      <c r="W114" s="3" t="s">
         <v>818</v>
       </c>
-      <c r="W114" s="3" t="s">
+      <c r="X114" s="3" t="s">
         <v>819</v>
       </c>
-      <c r="X114" s="3" t="s">
-        <v>820</v>
-      </c>
-      <c r="Y114" s="3"/>
+      <c r="Y114" s="3" t="s">
+        <v>816</v>
+      </c>
       <c r="Z114" s="3">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="AA114" s="3"/>
       <c r="AB114" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC114" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="AD114" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AC114" s="10" t="s">
+        <v>817</v>
+      </c>
+      <c r="AD114" s="3"/>
       <c r="AE114" s="3"/>
       <c r="AF114" s="3"/>
       <c r="AG114" s="3"/>
       <c r="AH114" s="3"/>
       <c r="AI114" s="3"/>
-      <c r="AJ114" s="3" t="s">
-        <v>60</v>
-      </c>
+      <c r="AJ114" s="3"/>
       <c r="AK114" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="115" spans="1:37">
+      <c r="A115" s="7">
+        <v>113</v>
+      </c>
+      <c r="B115" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C115" s="7">
+        <v>2025062881</v>
+      </c>
+      <c r="D115" s="7"/>
+      <c r="E115" s="7"/>
+      <c r="F115" s="7">
+        <v>4260</v>
+      </c>
+      <c r="G115" s="7" t="s">
+        <v>820</v>
+      </c>
+      <c r="H115" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I115" s="7"/>
+      <c r="J115" s="7"/>
+      <c r="K115" s="7"/>
+      <c r="L115" s="7"/>
+      <c r="M115" s="8"/>
+      <c r="N115" s="7"/>
+      <c r="O115" s="8"/>
+      <c r="P115" s="9"/>
+      <c r="Q115" s="7" t="s">
+        <v>821</v>
+      </c>
+      <c r="R115" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S115" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T115" s="7">
+        <v>1</v>
+      </c>
+      <c r="U115" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V115" s="7" t="s">
+        <v>822</v>
+      </c>
+      <c r="W115" s="7" t="s">
+        <v>823</v>
+      </c>
+      <c r="X115" s="7" t="s">
+        <v>824</v>
+      </c>
+      <c r="Y115" s="7"/>
+      <c r="Z115" s="7">
+        <v>3</v>
+      </c>
+      <c r="AA115" s="7"/>
+      <c r="AB115" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC115" s="9" t="s">
+        <v>825</v>
+      </c>
+      <c r="AD115" s="7"/>
+      <c r="AE115" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF115" s="7"/>
+      <c r="AG115" s="7"/>
+      <c r="AH115" s="7"/>
+      <c r="AI115" s="7"/>
+      <c r="AJ115" s="7"/>
+      <c r="AK115" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="116" spans="1:37">
+      <c r="A116" s="3">
+        <v>114</v>
+      </c>
+      <c r="B116" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C116" s="3">
+        <v>2025062901</v>
+      </c>
+      <c r="D116" s="3"/>
+      <c r="E116" s="3"/>
+      <c r="F116" s="3">
+        <v>2224</v>
+      </c>
+      <c r="G116" s="3" t="s">
+        <v>826</v>
+      </c>
+      <c r="H116" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I116" s="3"/>
+      <c r="J116" s="3"/>
+      <c r="K116" s="3"/>
+      <c r="L116" s="3"/>
+      <c r="M116" s="4"/>
+      <c r="N116" s="3"/>
+      <c r="O116" s="4"/>
+      <c r="P116" s="10"/>
+      <c r="Q116" s="3" t="s">
+        <v>827</v>
+      </c>
+      <c r="R116" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S116" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T116" s="3">
+        <v>1</v>
+      </c>
+      <c r="U116" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V116" s="3" t="s">
+        <v>828</v>
+      </c>
+      <c r="W116" s="3" t="s">
+        <v>829</v>
+      </c>
+      <c r="X116" s="3" t="s">
+        <v>830</v>
+      </c>
+      <c r="Y116" s="3"/>
+      <c r="Z116" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA116" s="3"/>
+      <c r="AB116" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC116" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD116" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE116" s="3"/>
+      <c r="AF116" s="3"/>
+      <c r="AG116" s="3"/>
+      <c r="AH116" s="3"/>
+      <c r="AI116" s="3"/>
+      <c r="AJ116" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK116" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="117" spans="1:37">
+      <c r="A117" s="7">
+        <v>115</v>
+      </c>
+      <c r="B117" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C117" s="7">
+        <v>2025063127</v>
+      </c>
+      <c r="D117" s="7"/>
+      <c r="E117" s="7"/>
+      <c r="F117" s="7" t="s">
+        <v>831</v>
+      </c>
+      <c r="G117" s="7" t="s">
+        <v>832</v>
+      </c>
+      <c r="H117" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I117" s="7"/>
+      <c r="J117" s="7"/>
+      <c r="K117" s="7"/>
+      <c r="L117" s="7"/>
+      <c r="M117" s="8"/>
+      <c r="N117" s="7"/>
+      <c r="O117" s="8"/>
+      <c r="P117" s="9"/>
+      <c r="Q117" s="7" t="s">
+        <v>833</v>
+      </c>
+      <c r="R117" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S117" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T117" s="7">
+        <v>1</v>
+      </c>
+      <c r="U117" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V117" s="7" t="s">
+        <v>834</v>
+      </c>
+      <c r="W117" s="7" t="s">
+        <v>835</v>
+      </c>
+      <c r="X117" s="7" t="s">
+        <v>836</v>
+      </c>
+      <c r="Y117" s="7"/>
+      <c r="Z117" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA117" s="7"/>
+      <c r="AB117" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC117" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD117" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE117" s="7"/>
+      <c r="AF117" s="7"/>
+      <c r="AG117" s="7"/>
+      <c r="AH117" s="7"/>
+      <c r="AI117" s="7"/>
+      <c r="AJ117" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK117" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="118" spans="1:37">
+      <c r="A118" s="3">
+        <v>116</v>
+      </c>
+      <c r="B118" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C118" s="3">
+        <v>2025063138</v>
+      </c>
+      <c r="D118" s="3"/>
+      <c r="E118" s="3"/>
+      <c r="F118" s="3">
+        <v>5354</v>
+      </c>
+      <c r="G118" s="3" t="s">
+        <v>837</v>
+      </c>
+      <c r="H118" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="I118" s="3"/>
+      <c r="J118" s="3"/>
+      <c r="K118" s="3"/>
+      <c r="L118" s="3"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="3"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="10"/>
+      <c r="Q118" s="3" t="s">
+        <v>838</v>
+      </c>
+      <c r="R118" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S118" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T118" s="3">
+        <v>1</v>
+      </c>
+      <c r="U118" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V118" s="3" t="s">
+        <v>839</v>
+      </c>
+      <c r="W118" s="3" t="s">
+        <v>840</v>
+      </c>
+      <c r="X118" s="3" t="s">
+        <v>841</v>
+      </c>
+      <c r="Y118" s="3"/>
+      <c r="Z118" s="3">
+        <v>3</v>
+      </c>
+      <c r="AA118" s="3"/>
+      <c r="AB118" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC118" s="10" t="s">
+        <v>410</v>
+      </c>
+      <c r="AD118" s="3"/>
+      <c r="AE118" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AF118" s="3"/>
+      <c r="AG118" s="3"/>
+      <c r="AH118" s="3"/>
+      <c r="AI118" s="3"/>
+      <c r="AJ118" s="3"/>
+      <c r="AK118" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="119" spans="1:37">
+      <c r="A119" s="7">
+        <v>117</v>
+      </c>
+      <c r="B119" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C119" s="7">
+        <v>2025063141</v>
+      </c>
+      <c r="D119" s="7"/>
+      <c r="E119" s="7"/>
+      <c r="F119" s="7" t="s">
+        <v>842</v>
+      </c>
+      <c r="G119" s="7" t="s">
+        <v>843</v>
+      </c>
+      <c r="H119" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="I119" s="7"/>
+      <c r="J119" s="7"/>
+      <c r="K119" s="7"/>
+      <c r="L119" s="7"/>
+      <c r="M119" s="8"/>
+      <c r="N119" s="7"/>
+      <c r="O119" s="8"/>
+      <c r="P119" s="9"/>
+      <c r="Q119" s="7" t="s">
+        <v>844</v>
+      </c>
+      <c r="R119" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S119" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T119" s="7">
+        <v>1</v>
+      </c>
+      <c r="U119" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V119" s="7" t="s">
+        <v>845</v>
+      </c>
+      <c r="W119" s="7" t="s">
+        <v>846</v>
+      </c>
+      <c r="X119" s="7" t="s">
+        <v>847</v>
+      </c>
+      <c r="Y119" s="7"/>
+      <c r="Z119" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA119" s="7"/>
+      <c r="AB119" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC119" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD119" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE119" s="7"/>
+      <c r="AF119" s="7"/>
+      <c r="AG119" s="7"/>
+      <c r="AH119" s="7"/>
+      <c r="AI119" s="7"/>
+      <c r="AJ119" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK119" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="120" spans="1:37">
+      <c r="A120" s="3">
+        <v>118</v>
+      </c>
+      <c r="B120" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C120" s="3">
+        <v>2025063146</v>
+      </c>
+      <c r="D120" s="3"/>
+      <c r="E120" s="3"/>
+      <c r="F120" s="3">
+        <v>4968</v>
+      </c>
+      <c r="G120" s="3" t="s">
+        <v>848</v>
+      </c>
+      <c r="H120" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I120" s="3"/>
+      <c r="J120" s="3"/>
+      <c r="K120" s="3"/>
+      <c r="L120" s="3"/>
+      <c r="M120" s="4"/>
+      <c r="N120" s="3"/>
+      <c r="O120" s="4"/>
+      <c r="P120" s="4"/>
+      <c r="Q120" s="3" t="s">
+        <v>849</v>
+      </c>
+      <c r="R120" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S120" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T120" s="3">
+        <v>1</v>
+      </c>
+      <c r="U120" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V120" s="3" t="s">
+        <v>850</v>
+      </c>
+      <c r="W120" s="3" t="s">
+        <v>851</v>
+      </c>
+      <c r="X120" s="3" t="s">
+        <v>852</v>
+      </c>
+      <c r="Y120" s="3"/>
+      <c r="Z120" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA120" s="3"/>
+      <c r="AB120" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC120" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD120" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE120" s="3"/>
+      <c r="AF120" s="3"/>
+      <c r="AG120" s="3"/>
+      <c r="AH120" s="3"/>
+      <c r="AI120" s="3"/>
+      <c r="AJ120" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK120" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 25-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$121</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$125</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="865">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-24  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="894">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-25  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2679,6 +2679,93 @@
   </si>
   <si>
     <t>2025-06-24 15:15:00</t>
+  </si>
+  <si>
+    <t>12069114062401</t>
+  </si>
+  <si>
+    <t>板橋江子翠站</t>
+  </si>
+  <si>
+    <t>2025-06-24 21:47:28</t>
+  </si>
+  <si>
+    <t>TM2熱感發票機(BSC-10)沒有電源反應，確認線路無脫落，重新開關機也無反應.........還請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF02069</t>
+  </si>
+  <si>
+    <t>2025-06-24 21:53:30</t>
+  </si>
+  <si>
+    <t>2025-06-25 14:28:00</t>
+  </si>
+  <si>
+    <t>2025-06-25 14:58:00</t>
+  </si>
+  <si>
+    <t>2025-06-26 01:53:00</t>
+  </si>
+  <si>
+    <t>取消報修</t>
+  </si>
+  <si>
+    <t>TT01</t>
+  </si>
+  <si>
+    <t>五股訓練教室</t>
+  </si>
+  <si>
+    <t>THILF0TT01</t>
+  </si>
+  <si>
+    <t>2025-06-25 08:46:53</t>
+  </si>
+  <si>
+    <t>2025-06-25 08:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-25 08:50:00</t>
+  </si>
+  <si>
+    <t>PMQ2+STAR</t>
+  </si>
+  <si>
+    <t>L516</t>
+  </si>
+  <si>
+    <t>車麗屋新莊店</t>
+  </si>
+  <si>
+    <t>THILF0L516</t>
+  </si>
+  <si>
+    <t>2025-06-25 13:34:33</t>
+  </si>
+  <si>
+    <t>2025-06-25 13:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-25 13:20:00</t>
+  </si>
+  <si>
+    <t>金山銀山店</t>
+  </si>
+  <si>
+    <t>新北市金山區</t>
+  </si>
+  <si>
+    <t>THILF04906</t>
+  </si>
+  <si>
+    <t>2025-06-25 14:33:42</t>
+  </si>
+  <si>
+    <t>2025-06-25 14:18:00</t>
+  </si>
+  <si>
+    <t>2025-06-25 14:40:00</t>
   </si>
 </sst>
 </file>
@@ -3092,10 +3179,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK121"/>
+  <dimension ref="A1:AK125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A121" sqref="A121"/>
+      <selection activeCell="A125" sqref="A125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13421,7 +13508,7 @@
       <c r="M121" s="8"/>
       <c r="N121" s="7"/>
       <c r="O121" s="8"/>
-      <c r="P121" s="8"/>
+      <c r="P121" s="9"/>
       <c r="Q121" s="7" t="s">
         <v>861</v>
       </c>
@@ -13454,7 +13541,7 @@
       <c r="AB121" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC121" s="8" t="s">
+      <c r="AC121" s="9" t="s">
         <v>98</v>
       </c>
       <c r="AD121" s="7" t="s">
@@ -13469,6 +13556,334 @@
         <v>60</v>
       </c>
       <c r="AK121" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="122" spans="1:37">
+      <c r="A122" s="3">
+        <v>120</v>
+      </c>
+      <c r="B122" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C122" s="3">
+        <v>2025063174</v>
+      </c>
+      <c r="D122" s="3" t="s">
+        <v>865</v>
+      </c>
+      <c r="E122" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F122" s="3">
+        <v>2069</v>
+      </c>
+      <c r="G122" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="H122" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I122" s="3" t="s">
+        <v>867</v>
+      </c>
+      <c r="J122" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="K122" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L122" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="M122" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="N122" s="3" t="s">
+        <v>534</v>
+      </c>
+      <c r="O122" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="P122" s="10" t="s">
+        <v>868</v>
+      </c>
+      <c r="Q122" s="3" t="s">
+        <v>869</v>
+      </c>
+      <c r="R122" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S122" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T122" s="3">
+        <v>1</v>
+      </c>
+      <c r="U122" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V122" s="3" t="s">
+        <v>870</v>
+      </c>
+      <c r="W122" s="3" t="s">
+        <v>871</v>
+      </c>
+      <c r="X122" s="3" t="s">
+        <v>872</v>
+      </c>
+      <c r="Y122" s="3" t="s">
+        <v>873</v>
+      </c>
+      <c r="Z122" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA122" s="3"/>
+      <c r="AB122" s="3" t="s">
+        <v>737</v>
+      </c>
+      <c r="AC122" s="10" t="s">
+        <v>874</v>
+      </c>
+      <c r="AD122" s="3"/>
+      <c r="AE122" s="3"/>
+      <c r="AF122" s="3"/>
+      <c r="AG122" s="3"/>
+      <c r="AH122" s="3"/>
+      <c r="AI122" s="3"/>
+      <c r="AJ122" s="3"/>
+      <c r="AK122" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="123" spans="1:37">
+      <c r="A123" s="7">
+        <v>121</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C123" s="7">
+        <v>2025063175</v>
+      </c>
+      <c r="D123" s="7"/>
+      <c r="E123" s="7"/>
+      <c r="F123" s="7" t="s">
+        <v>875</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>876</v>
+      </c>
+      <c r="H123" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I123" s="7"/>
+      <c r="J123" s="7"/>
+      <c r="K123" s="7"/>
+      <c r="L123" s="7"/>
+      <c r="M123" s="8"/>
+      <c r="N123" s="7"/>
+      <c r="O123" s="8"/>
+      <c r="P123" s="9"/>
+      <c r="Q123" s="7" t="s">
+        <v>877</v>
+      </c>
+      <c r="R123" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S123" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T123" s="7">
+        <v>1</v>
+      </c>
+      <c r="U123" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V123" s="7" t="s">
+        <v>878</v>
+      </c>
+      <c r="W123" s="7" t="s">
+        <v>879</v>
+      </c>
+      <c r="X123" s="7" t="s">
+        <v>880</v>
+      </c>
+      <c r="Y123" s="7"/>
+      <c r="Z123" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA123" s="7"/>
+      <c r="AB123" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC123" s="9" t="s">
+        <v>881</v>
+      </c>
+      <c r="AD123" s="7"/>
+      <c r="AE123" s="7"/>
+      <c r="AF123" s="7"/>
+      <c r="AG123" s="7"/>
+      <c r="AH123" s="7"/>
+      <c r="AI123" s="7"/>
+      <c r="AJ123" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK123" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="124" spans="1:37">
+      <c r="A124" s="3">
+        <v>122</v>
+      </c>
+      <c r="B124" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C124" s="3">
+        <v>2025063231</v>
+      </c>
+      <c r="D124" s="3"/>
+      <c r="E124" s="3"/>
+      <c r="F124" s="3" t="s">
+        <v>882</v>
+      </c>
+      <c r="G124" s="3" t="s">
+        <v>883</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I124" s="3"/>
+      <c r="J124" s="3"/>
+      <c r="K124" s="3"/>
+      <c r="L124" s="3"/>
+      <c r="M124" s="4"/>
+      <c r="N124" s="3"/>
+      <c r="O124" s="4"/>
+      <c r="P124" s="10"/>
+      <c r="Q124" s="3" t="s">
+        <v>884</v>
+      </c>
+      <c r="R124" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S124" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T124" s="3">
+        <v>1</v>
+      </c>
+      <c r="U124" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V124" s="3" t="s">
+        <v>885</v>
+      </c>
+      <c r="W124" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="X124" s="3" t="s">
+        <v>887</v>
+      </c>
+      <c r="Y124" s="3"/>
+      <c r="Z124" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA124" s="3"/>
+      <c r="AB124" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC124" s="10" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD124" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE124" s="3"/>
+      <c r="AF124" s="3"/>
+      <c r="AG124" s="3"/>
+      <c r="AH124" s="3"/>
+      <c r="AI124" s="3"/>
+      <c r="AJ124" s="3"/>
+      <c r="AK124" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="125" spans="1:37">
+      <c r="A125" s="7">
+        <v>123</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C125" s="7">
+        <v>2025063250</v>
+      </c>
+      <c r="D125" s="7"/>
+      <c r="E125" s="7"/>
+      <c r="F125" s="7">
+        <v>4906</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>888</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>889</v>
+      </c>
+      <c r="I125" s="7"/>
+      <c r="J125" s="7"/>
+      <c r="K125" s="7"/>
+      <c r="L125" s="7"/>
+      <c r="M125" s="8"/>
+      <c r="N125" s="7"/>
+      <c r="O125" s="8"/>
+      <c r="P125" s="8"/>
+      <c r="Q125" s="7" t="s">
+        <v>890</v>
+      </c>
+      <c r="R125" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S125" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T125" s="7">
+        <v>1</v>
+      </c>
+      <c r="U125" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V125" s="7" t="s">
+        <v>891</v>
+      </c>
+      <c r="W125" s="7" t="s">
+        <v>892</v>
+      </c>
+      <c r="X125" s="7" t="s">
+        <v>893</v>
+      </c>
+      <c r="Y125" s="7"/>
+      <c r="Z125" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA125" s="7"/>
+      <c r="AB125" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC125" s="8" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD125" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE125" s="7"/>
+      <c r="AF125" s="7"/>
+      <c r="AG125" s="7"/>
+      <c r="AH125" s="7"/>
+      <c r="AI125" s="7"/>
+      <c r="AJ125" s="7"/>
+      <c r="AK125" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 26-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$125</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$128</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="894">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-25  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="908">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-26  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2732,6 +2732,31 @@
     <t>PMQ2+STAR</t>
   </si>
   <si>
+    <t>12069114062501</t>
+  </si>
+  <si>
+    <t>2025-06-25 09:25:31</t>
+  </si>
+  <si>
+    <t>門市反應TM1(TCX800)無法開機，重新拔插線路仍異常，已確認粉色插座及白色插座皆有過電開機仍異常黑屏，確認TM右下角未亮電源燈，PING.80不通無法VNC...請台芝到店協助確認 已與門市確認入帳日6/25不清楚是否有交易資料，PS若因更換HD.請跟店長宣達:1.請門市先回報代收會計 2.請確認SC的代收資料是否正確 (須與代收單據逐一核對)</t>
+  </si>
+  <si>
+    <t>2025-06-25 09:31:57</t>
+  </si>
+  <si>
+    <t>2025-06-25 15:45:00</t>
+  </si>
+  <si>
+    <t>2025-06-25 16:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-26 13:31:00</t>
+  </si>
+  <si>
+    <t>更換TCx800變壓器
+測試功能正常</t>
+  </si>
+  <si>
     <t>L516</t>
   </si>
   <si>
@@ -2766,6 +2791,24 @@
   </si>
   <si>
     <t>2025-06-25 14:40:00</t>
+  </si>
+  <si>
+    <t>淡水小坪頂</t>
+  </si>
+  <si>
+    <t>THILF05101</t>
+  </si>
+  <si>
+    <t>2025-06-25 16:17:46</t>
+  </si>
+  <si>
+    <t>2025-06-25 15:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-25 16:16:00</t>
+  </si>
+  <si>
+    <t>2025-06-25 16:40:51</t>
   </si>
 </sst>
 </file>
@@ -3179,10 +3222,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK125"/>
+  <dimension ref="A1:AK128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A125" sqref="A125"/>
+      <selection activeCell="AC125" sqref="AC125"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -13738,38 +13781,58 @@
         <v>122</v>
       </c>
       <c r="B124" s="3" t="s">
-        <v>94</v>
+        <v>38</v>
       </c>
       <c r="C124" s="3">
-        <v>2025063231</v>
-      </c>
-      <c r="D124" s="3"/>
-      <c r="E124" s="3"/>
-      <c r="F124" s="3" t="s">
+        <v>2025063183</v>
+      </c>
+      <c r="D124" s="3" t="s">
         <v>882</v>
       </c>
+      <c r="E124" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F124" s="3">
+        <v>2069</v>
+      </c>
       <c r="G124" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="H124" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I124" s="3" t="s">
         <v>883</v>
       </c>
-      <c r="H124" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="I124" s="3"/>
-      <c r="J124" s="3"/>
-      <c r="K124" s="3"/>
-      <c r="L124" s="3"/>
-      <c r="M124" s="4"/>
-      <c r="N124" s="3"/>
-      <c r="O124" s="4"/>
-      <c r="P124" s="10"/>
+      <c r="J124" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="K124" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L124" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="M124" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="N124" s="3">
+        <v>2306</v>
+      </c>
+      <c r="O124" s="4" t="s">
+        <v>731</v>
+      </c>
+      <c r="P124" s="10" t="s">
+        <v>884</v>
+      </c>
       <c r="Q124" s="3" t="s">
-        <v>884</v>
+        <v>869</v>
       </c>
       <c r="R124" s="3" t="s">
         <v>51</v>
       </c>
       <c r="S124" s="3" t="s">
-        <v>73</v>
+        <v>125</v>
       </c>
       <c r="T124" s="3">
         <v>1</v>
@@ -13786,20 +13849,20 @@
       <c r="X124" s="3" t="s">
         <v>887</v>
       </c>
-      <c r="Y124" s="3"/>
+      <c r="Y124" s="3" t="s">
+        <v>888</v>
+      </c>
       <c r="Z124" s="3">
-        <v>0.3</v>
+        <v>0.9</v>
       </c>
       <c r="AA124" s="3"/>
       <c r="AB124" s="3" t="s">
         <v>58</v>
       </c>
       <c r="AC124" s="10" t="s">
-        <v>214</v>
-      </c>
-      <c r="AD124" s="3" t="s">
-        <v>60</v>
-      </c>
+        <v>889</v>
+      </c>
+      <c r="AD124" s="3"/>
       <c r="AE124" s="3"/>
       <c r="AF124" s="3"/>
       <c r="AG124" s="3"/>
@@ -13818,18 +13881,18 @@
         <v>94</v>
       </c>
       <c r="C125" s="7">
-        <v>2025063250</v>
+        <v>2025063231</v>
       </c>
       <c r="D125" s="7"/>
       <c r="E125" s="7"/>
-      <c r="F125" s="7">
-        <v>4906</v>
+      <c r="F125" s="7" t="s">
+        <v>890</v>
       </c>
       <c r="G125" s="7" t="s">
-        <v>888</v>
+        <v>891</v>
       </c>
       <c r="H125" s="7" t="s">
-        <v>889</v>
+        <v>63</v>
       </c>
       <c r="I125" s="7"/>
       <c r="J125" s="7"/>
@@ -13838,15 +13901,15 @@
       <c r="M125" s="8"/>
       <c r="N125" s="7"/>
       <c r="O125" s="8"/>
-      <c r="P125" s="8"/>
+      <c r="P125" s="9"/>
       <c r="Q125" s="7" t="s">
-        <v>890</v>
+        <v>892</v>
       </c>
       <c r="R125" s="7" t="s">
         <v>51</v>
       </c>
       <c r="S125" s="7" t="s">
-        <v>52</v>
+        <v>73</v>
       </c>
       <c r="T125" s="7">
         <v>1</v>
@@ -13855,24 +13918,24 @@
         <v>53</v>
       </c>
       <c r="V125" s="7" t="s">
-        <v>891</v>
+        <v>893</v>
       </c>
       <c r="W125" s="7" t="s">
-        <v>892</v>
+        <v>894</v>
       </c>
       <c r="X125" s="7" t="s">
-        <v>893</v>
+        <v>895</v>
       </c>
       <c r="Y125" s="7"/>
       <c r="Z125" s="7">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="AA125" s="7"/>
       <c r="AB125" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC125" s="8" t="s">
-        <v>129</v>
+      <c r="AC125" s="9" t="s">
+        <v>214</v>
       </c>
       <c r="AD125" s="7" t="s">
         <v>60</v>
@@ -13884,6 +13947,239 @@
       <c r="AI125" s="7"/>
       <c r="AJ125" s="7"/>
       <c r="AK125" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="126" spans="1:37">
+      <c r="A126" s="3">
+        <v>124</v>
+      </c>
+      <c r="B126" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C126" s="3">
+        <v>2025063250</v>
+      </c>
+      <c r="D126" s="3"/>
+      <c r="E126" s="3"/>
+      <c r="F126" s="3">
+        <v>4906</v>
+      </c>
+      <c r="G126" s="3" t="s">
+        <v>896</v>
+      </c>
+      <c r="H126" s="3" t="s">
+        <v>897</v>
+      </c>
+      <c r="I126" s="3"/>
+      <c r="J126" s="3"/>
+      <c r="K126" s="3"/>
+      <c r="L126" s="3"/>
+      <c r="M126" s="4"/>
+      <c r="N126" s="3"/>
+      <c r="O126" s="4"/>
+      <c r="P126" s="10"/>
+      <c r="Q126" s="3" t="s">
+        <v>898</v>
+      </c>
+      <c r="R126" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S126" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T126" s="3">
+        <v>1</v>
+      </c>
+      <c r="U126" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V126" s="3" t="s">
+        <v>899</v>
+      </c>
+      <c r="W126" s="3" t="s">
+        <v>900</v>
+      </c>
+      <c r="X126" s="3" t="s">
+        <v>901</v>
+      </c>
+      <c r="Y126" s="3"/>
+      <c r="Z126" s="3">
+        <v>0.4</v>
+      </c>
+      <c r="AA126" s="3"/>
+      <c r="AB126" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC126" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD126" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE126" s="3"/>
+      <c r="AF126" s="3"/>
+      <c r="AG126" s="3"/>
+      <c r="AH126" s="3"/>
+      <c r="AI126" s="3"/>
+      <c r="AJ126" s="3"/>
+      <c r="AK126" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="127" spans="1:37">
+      <c r="A127" s="7">
+        <v>125</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C127" s="7">
+        <v>2025063278</v>
+      </c>
+      <c r="D127" s="7"/>
+      <c r="E127" s="7"/>
+      <c r="F127" s="7">
+        <v>5101</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>902</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I127" s="7"/>
+      <c r="J127" s="7"/>
+      <c r="K127" s="7"/>
+      <c r="L127" s="7"/>
+      <c r="M127" s="8"/>
+      <c r="N127" s="7"/>
+      <c r="O127" s="8"/>
+      <c r="P127" s="9"/>
+      <c r="Q127" s="7" t="s">
+        <v>903</v>
+      </c>
+      <c r="R127" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S127" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T127" s="7">
+        <v>1</v>
+      </c>
+      <c r="U127" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V127" s="7" t="s">
+        <v>904</v>
+      </c>
+      <c r="W127" s="7" t="s">
+        <v>905</v>
+      </c>
+      <c r="X127" s="7" t="s">
+        <v>906</v>
+      </c>
+      <c r="Y127" s="7"/>
+      <c r="Z127" s="7">
+        <v>0.6</v>
+      </c>
+      <c r="AA127" s="7"/>
+      <c r="AB127" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC127" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="AD127" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE127" s="7"/>
+      <c r="AF127" s="7"/>
+      <c r="AG127" s="7"/>
+      <c r="AH127" s="7"/>
+      <c r="AI127" s="7"/>
+      <c r="AJ127" s="7"/>
+      <c r="AK127" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="128" spans="1:37">
+      <c r="A128" s="3">
+        <v>126</v>
+      </c>
+      <c r="B128" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C128" s="3">
+        <v>2025063285</v>
+      </c>
+      <c r="D128" s="3"/>
+      <c r="E128" s="3"/>
+      <c r="F128" s="3">
+        <v>2069</v>
+      </c>
+      <c r="G128" s="3" t="s">
+        <v>866</v>
+      </c>
+      <c r="H128" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I128" s="3"/>
+      <c r="J128" s="3"/>
+      <c r="K128" s="3"/>
+      <c r="L128" s="3"/>
+      <c r="M128" s="4"/>
+      <c r="N128" s="3"/>
+      <c r="O128" s="4"/>
+      <c r="P128" s="4"/>
+      <c r="Q128" s="3" t="s">
+        <v>869</v>
+      </c>
+      <c r="R128" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S128" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T128" s="3">
+        <v>1</v>
+      </c>
+      <c r="U128" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V128" s="3" t="s">
+        <v>907</v>
+      </c>
+      <c r="W128" s="3" t="s">
+        <v>886</v>
+      </c>
+      <c r="X128" s="3" t="s">
+        <v>887</v>
+      </c>
+      <c r="Y128" s="3"/>
+      <c r="Z128" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA128" s="3"/>
+      <c r="AB128" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC128" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD128" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE128" s="3"/>
+      <c r="AF128" s="3"/>
+      <c r="AG128" s="3"/>
+      <c r="AH128" s="3"/>
+      <c r="AI128" s="3"/>
+      <c r="AJ128" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK128" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 27-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$128</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$135</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="908">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-26  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="964">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-27  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2809,6 +2809,178 @@
   </si>
   <si>
     <t>2025-06-25 16:40:51</t>
+  </si>
+  <si>
+    <t>15354114062601</t>
+  </si>
+  <si>
+    <t>2025-06-26 09:26:13</t>
+  </si>
+  <si>
+    <t>HL35</t>
+  </si>
+  <si>
+    <t>HL-4G分享器</t>
+  </si>
+  <si>
+    <t>網路障礙借用</t>
+  </si>
+  <si>
+    <t>06/26 09:26 總公司玫君來電啟動緊急叫修:門市目前店內網路不通，ping全店僅90通重啟hub、adsl仍異常，門市今日開幕，須請台芝到店借用4G</t>
+  </si>
+  <si>
+    <t>2025-06-26 09:28:22</t>
+  </si>
+  <si>
+    <t>2025-06-26 11:03:00</t>
+  </si>
+  <si>
+    <t>2025-06-26 11:33:00</t>
+  </si>
+  <si>
+    <t>2025-06-26 15:28:00</t>
+  </si>
+  <si>
+    <t>至店上檢查網路皆為正常</t>
+  </si>
+  <si>
+    <t>12691114062601</t>
+  </si>
+  <si>
+    <t>2025-06-26 10:42:07</t>
+  </si>
+  <si>
+    <t>門市反應tm1多卡機(QP3000E)無法使用悠遊卡交易，已協助版本更新後悠遊卡機開機顯示:代碼0 comport成功開啟或成功關閉....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-06-26 10:44:11</t>
+  </si>
+  <si>
+    <t>2025-06-26 11:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-26 11:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-27 14:44:00</t>
+  </si>
+  <si>
+    <t>更換多卡機
+換上8183001602
+換下8183001984</t>
+  </si>
+  <si>
+    <t>E3785114062601</t>
+  </si>
+  <si>
+    <t>2025-06-26 14:56:44</t>
+  </si>
+  <si>
+    <t>門市反應tm1太空寶寶(MS-7580)有時刷讀條碼無反應有亮燈有逼聲，門市反應後方接頭接觸不良，重插後又可以刷但沒多久又不行....須請台芝到店協助(無反應)</t>
+  </si>
+  <si>
+    <t>2025-06-26 15:06:38</t>
+  </si>
+  <si>
+    <t>2025-06-27 08:45:00</t>
+  </si>
+  <si>
+    <t>2025-06-27 09:15:00</t>
+  </si>
+  <si>
+    <t>2025-06-27 19:06:00</t>
+  </si>
+  <si>
+    <t>更換PS2轉接頭</t>
+  </si>
+  <si>
+    <t>板橋仁化店</t>
+  </si>
+  <si>
+    <t>THILF03962</t>
+  </si>
+  <si>
+    <t>2025-06-26 15:10:44</t>
+  </si>
+  <si>
+    <t>2025-06-26 14:25:00</t>
+  </si>
+  <si>
+    <t>2025-06-26 15:10:00</t>
+  </si>
+  <si>
+    <t>板橋藝文中心</t>
+  </si>
+  <si>
+    <t>THILF03399</t>
+  </si>
+  <si>
+    <t>2025-06-26 15:57:32</t>
+  </si>
+  <si>
+    <t>2025-06-26 15:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-26 15:55:00</t>
+  </si>
+  <si>
+    <t>14153114062701</t>
+  </si>
+  <si>
+    <t>淡水莊園店</t>
+  </si>
+  <si>
+    <t>2025-06-27 09:16:28</t>
+  </si>
+  <si>
+    <t>THILF04153</t>
+  </si>
+  <si>
+    <t>2025-06-27 09:17:40</t>
+  </si>
+  <si>
+    <t>2025-06-27 12:05:00</t>
+  </si>
+  <si>
+    <t>2025-06-27 12:35:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 13:17:00</t>
+  </si>
+  <si>
+    <t>現場多卡機當機狀態，將電源重新插上重啟可正常使用，先請店員觀察狀況</t>
+  </si>
+  <si>
+    <t>12691114062701</t>
+  </si>
+  <si>
+    <t>2025-06-27 09:20:53</t>
+  </si>
+  <si>
+    <t>F602</t>
+  </si>
+  <si>
+    <t>無法讀卡</t>
+  </si>
+  <si>
+    <t>門市反應tm1多卡機(QP3000E)無法使用悠遊卡/一卡通/愛金卡交易，已協助版本更新後悠遊卡機開機顯示通訊逾時，一卡通重開也顯示0801一卡通機異常，門市6/26有報修更換過設備....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-06-27 09:23:31</t>
+  </si>
+  <si>
+    <t>2025-06-27 10:20:00</t>
+  </si>
+  <si>
+    <t>2025-06-27 10:50:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 13:23:00</t>
+  </si>
+  <si>
+    <t>更換多卡機及變壓器
+換上8183002072
+換下8183001602</t>
   </si>
 </sst>
 </file>
@@ -3222,10 +3394,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK128"/>
+  <dimension ref="A1:AK135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="AC125" sqref="AC125"/>
+      <selection activeCell="A135" sqref="A135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14132,7 +14304,7 @@
       <c r="M128" s="4"/>
       <c r="N128" s="3"/>
       <c r="O128" s="4"/>
-      <c r="P128" s="4"/>
+      <c r="P128" s="10"/>
       <c r="Q128" s="3" t="s">
         <v>869</v>
       </c>
@@ -14165,7 +14337,7 @@
       <c r="AB128" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AC128" s="4" t="s">
+      <c r="AC128" s="10" t="s">
         <v>98</v>
       </c>
       <c r="AD128" s="3" t="s">
@@ -14180,6 +14352,649 @@
         <v>60</v>
       </c>
       <c r="AK128" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="129" spans="1:37">
+      <c r="A129" s="7">
+        <v>127</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C129" s="7">
+        <v>2025063311</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>908</v>
+      </c>
+      <c r="E129" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F129" s="7">
+        <v>5354</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>849</v>
+      </c>
+      <c r="H129" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="I129" s="7" t="s">
+        <v>909</v>
+      </c>
+      <c r="J129" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K129" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L129" s="7" t="s">
+        <v>910</v>
+      </c>
+      <c r="M129" s="8" t="s">
+        <v>911</v>
+      </c>
+      <c r="N129" s="7">
+        <v>3502</v>
+      </c>
+      <c r="O129" s="8" t="s">
+        <v>912</v>
+      </c>
+      <c r="P129" s="9" t="s">
+        <v>913</v>
+      </c>
+      <c r="Q129" s="7" t="s">
+        <v>850</v>
+      </c>
+      <c r="R129" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S129" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T129" s="7">
+        <v>1</v>
+      </c>
+      <c r="U129" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V129" s="7" t="s">
+        <v>914</v>
+      </c>
+      <c r="W129" s="7" t="s">
+        <v>915</v>
+      </c>
+      <c r="X129" s="7" t="s">
+        <v>916</v>
+      </c>
+      <c r="Y129" s="7" t="s">
+        <v>917</v>
+      </c>
+      <c r="Z129" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA129" s="7"/>
+      <c r="AB129" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC129" s="9" t="s">
+        <v>918</v>
+      </c>
+      <c r="AD129" s="7"/>
+      <c r="AE129" s="7"/>
+      <c r="AF129" s="7"/>
+      <c r="AG129" s="7"/>
+      <c r="AH129" s="7"/>
+      <c r="AI129" s="7"/>
+      <c r="AJ129" s="7"/>
+      <c r="AK129" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="130" spans="1:37">
+      <c r="A130" s="3">
+        <v>128</v>
+      </c>
+      <c r="B130" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C130" s="3">
+        <v>2025063337</v>
+      </c>
+      <c r="D130" s="3" t="s">
+        <v>919</v>
+      </c>
+      <c r="E130" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F130" s="3">
+        <v>2691</v>
+      </c>
+      <c r="G130" s="3" t="s">
+        <v>486</v>
+      </c>
+      <c r="H130" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="I130" s="3" t="s">
+        <v>920</v>
+      </c>
+      <c r="J130" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="K130" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L130" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M130" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="N130" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="O130" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P130" s="10" t="s">
+        <v>921</v>
+      </c>
+      <c r="Q130" s="3" t="s">
+        <v>487</v>
+      </c>
+      <c r="R130" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S130" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="T130" s="3">
+        <v>1</v>
+      </c>
+      <c r="U130" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V130" s="3" t="s">
+        <v>922</v>
+      </c>
+      <c r="W130" s="3" t="s">
+        <v>923</v>
+      </c>
+      <c r="X130" s="3" t="s">
+        <v>924</v>
+      </c>
+      <c r="Y130" s="3" t="s">
+        <v>925</v>
+      </c>
+      <c r="Z130" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA130" s="3"/>
+      <c r="AB130" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC130" s="10" t="s">
+        <v>926</v>
+      </c>
+      <c r="AD130" s="3"/>
+      <c r="AE130" s="3"/>
+      <c r="AF130" s="3"/>
+      <c r="AG130" s="3"/>
+      <c r="AH130" s="3"/>
+      <c r="AI130" s="3"/>
+      <c r="AJ130" s="3"/>
+      <c r="AK130" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="131" spans="1:37">
+      <c r="A131" s="7">
+        <v>129</v>
+      </c>
+      <c r="B131" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C131" s="7">
+        <v>2025063401</v>
+      </c>
+      <c r="D131" s="7" t="s">
+        <v>927</v>
+      </c>
+      <c r="E131" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F131" s="7">
+        <v>3785</v>
+      </c>
+      <c r="G131" s="7" t="s">
+        <v>311</v>
+      </c>
+      <c r="H131" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I131" s="7" t="s">
+        <v>928</v>
+      </c>
+      <c r="J131" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="K131" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="L131" s="7" t="s">
+        <v>601</v>
+      </c>
+      <c r="M131" s="8" t="s">
+        <v>602</v>
+      </c>
+      <c r="N131" s="7">
+        <v>2803</v>
+      </c>
+      <c r="O131" s="8" t="s">
+        <v>603</v>
+      </c>
+      <c r="P131" s="9" t="s">
+        <v>929</v>
+      </c>
+      <c r="Q131" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="R131" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S131" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T131" s="7">
+        <v>1</v>
+      </c>
+      <c r="U131" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V131" s="7" t="s">
+        <v>930</v>
+      </c>
+      <c r="W131" s="7" t="s">
+        <v>931</v>
+      </c>
+      <c r="X131" s="7" t="s">
+        <v>932</v>
+      </c>
+      <c r="Y131" s="7" t="s">
+        <v>933</v>
+      </c>
+      <c r="Z131" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA131" s="7"/>
+      <c r="AB131" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC131" s="9" t="s">
+        <v>934</v>
+      </c>
+      <c r="AD131" s="7"/>
+      <c r="AE131" s="7"/>
+      <c r="AF131" s="7"/>
+      <c r="AG131" s="7"/>
+      <c r="AH131" s="7"/>
+      <c r="AI131" s="7"/>
+      <c r="AJ131" s="7"/>
+      <c r="AK131" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="132" spans="1:37">
+      <c r="A132" s="3">
+        <v>130</v>
+      </c>
+      <c r="B132" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C132" s="3">
+        <v>2025063403</v>
+      </c>
+      <c r="D132" s="3"/>
+      <c r="E132" s="3"/>
+      <c r="F132" s="3">
+        <v>3962</v>
+      </c>
+      <c r="G132" s="3" t="s">
+        <v>935</v>
+      </c>
+      <c r="H132" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I132" s="3"/>
+      <c r="J132" s="3"/>
+      <c r="K132" s="3"/>
+      <c r="L132" s="3"/>
+      <c r="M132" s="4"/>
+      <c r="N132" s="3"/>
+      <c r="O132" s="4"/>
+      <c r="P132" s="10"/>
+      <c r="Q132" s="3" t="s">
+        <v>936</v>
+      </c>
+      <c r="R132" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S132" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T132" s="3">
+        <v>1</v>
+      </c>
+      <c r="U132" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V132" s="3" t="s">
+        <v>937</v>
+      </c>
+      <c r="W132" s="3" t="s">
+        <v>938</v>
+      </c>
+      <c r="X132" s="3" t="s">
+        <v>939</v>
+      </c>
+      <c r="Y132" s="3"/>
+      <c r="Z132" s="3">
+        <v>0.8</v>
+      </c>
+      <c r="AA132" s="3"/>
+      <c r="AB132" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC132" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD132" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE132" s="3"/>
+      <c r="AF132" s="3"/>
+      <c r="AG132" s="3"/>
+      <c r="AH132" s="3"/>
+      <c r="AI132" s="3"/>
+      <c r="AJ132" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK132" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="133" spans="1:37">
+      <c r="A133" s="7">
+        <v>131</v>
+      </c>
+      <c r="B133" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C133" s="7">
+        <v>2025063425</v>
+      </c>
+      <c r="D133" s="7"/>
+      <c r="E133" s="7"/>
+      <c r="F133" s="7">
+        <v>3399</v>
+      </c>
+      <c r="G133" s="7" t="s">
+        <v>940</v>
+      </c>
+      <c r="H133" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I133" s="7"/>
+      <c r="J133" s="7"/>
+      <c r="K133" s="7"/>
+      <c r="L133" s="7"/>
+      <c r="M133" s="8"/>
+      <c r="N133" s="7"/>
+      <c r="O133" s="8"/>
+      <c r="P133" s="9"/>
+      <c r="Q133" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="R133" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S133" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T133" s="7">
+        <v>1</v>
+      </c>
+      <c r="U133" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V133" s="7" t="s">
+        <v>942</v>
+      </c>
+      <c r="W133" s="7" t="s">
+        <v>943</v>
+      </c>
+      <c r="X133" s="7" t="s">
+        <v>944</v>
+      </c>
+      <c r="Y133" s="7"/>
+      <c r="Z133" s="7">
+        <v>0.3</v>
+      </c>
+      <c r="AA133" s="7"/>
+      <c r="AB133" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC133" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD133" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE133" s="7"/>
+      <c r="AF133" s="7"/>
+      <c r="AG133" s="7"/>
+      <c r="AH133" s="7"/>
+      <c r="AI133" s="7"/>
+      <c r="AJ133" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK133" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="134" spans="1:37">
+      <c r="A134" s="3">
+        <v>132</v>
+      </c>
+      <c r="B134" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C134" s="3">
+        <v>2025063451</v>
+      </c>
+      <c r="D134" s="3" t="s">
+        <v>945</v>
+      </c>
+      <c r="E134" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F134" s="3">
+        <v>4153</v>
+      </c>
+      <c r="G134" s="3" t="s">
+        <v>946</v>
+      </c>
+      <c r="H134" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I134" s="3" t="s">
+        <v>947</v>
+      </c>
+      <c r="J134" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K134" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="L134" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="M134" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="N134" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="O134" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P134" s="10" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q134" s="3" t="s">
+        <v>948</v>
+      </c>
+      <c r="R134" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S134" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T134" s="3">
+        <v>1</v>
+      </c>
+      <c r="U134" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V134" s="3" t="s">
+        <v>949</v>
+      </c>
+      <c r="W134" s="3" t="s">
+        <v>950</v>
+      </c>
+      <c r="X134" s="3" t="s">
+        <v>951</v>
+      </c>
+      <c r="Y134" s="3" t="s">
+        <v>952</v>
+      </c>
+      <c r="Z134" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA134" s="3"/>
+      <c r="AB134" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC134" s="10" t="s">
+        <v>953</v>
+      </c>
+      <c r="AD134" s="3"/>
+      <c r="AE134" s="3"/>
+      <c r="AF134" s="3"/>
+      <c r="AG134" s="3"/>
+      <c r="AH134" s="3"/>
+      <c r="AI134" s="3"/>
+      <c r="AJ134" s="3"/>
+      <c r="AK134" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="135" spans="1:37">
+      <c r="A135" s="7">
+        <v>133</v>
+      </c>
+      <c r="B135" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C135" s="7">
+        <v>2025063452</v>
+      </c>
+      <c r="D135" s="7" t="s">
+        <v>954</v>
+      </c>
+      <c r="E135" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F135" s="7">
+        <v>2691</v>
+      </c>
+      <c r="G135" s="7" t="s">
+        <v>486</v>
+      </c>
+      <c r="H135" s="7" t="s">
+        <v>184</v>
+      </c>
+      <c r="I135" s="7" t="s">
+        <v>955</v>
+      </c>
+      <c r="J135" s="7" t="s">
+        <v>65</v>
+      </c>
+      <c r="K135" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L135" s="7" t="s">
+        <v>172</v>
+      </c>
+      <c r="M135" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="N135" s="7" t="s">
+        <v>956</v>
+      </c>
+      <c r="O135" s="8" t="s">
+        <v>957</v>
+      </c>
+      <c r="P135" s="8" t="s">
+        <v>958</v>
+      </c>
+      <c r="Q135" s="7" t="s">
+        <v>487</v>
+      </c>
+      <c r="R135" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S135" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="T135" s="7">
+        <v>1</v>
+      </c>
+      <c r="U135" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V135" s="7" t="s">
+        <v>959</v>
+      </c>
+      <c r="W135" s="7" t="s">
+        <v>960</v>
+      </c>
+      <c r="X135" s="7" t="s">
+        <v>961</v>
+      </c>
+      <c r="Y135" s="7" t="s">
+        <v>962</v>
+      </c>
+      <c r="Z135" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA135" s="7"/>
+      <c r="AB135" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC135" s="8" t="s">
+        <v>963</v>
+      </c>
+      <c r="AD135" s="7"/>
+      <c r="AE135" s="7"/>
+      <c r="AF135" s="7"/>
+      <c r="AG135" s="7"/>
+      <c r="AH135" s="7"/>
+      <c r="AI135" s="7"/>
+      <c r="AJ135" s="7"/>
+      <c r="AK135" s="7" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Auto commit on 30-2025-time
</commit_message>
<xml_diff>
--- a/IM/202506_HL_Maintain_Report.xlsx
+++ b/IM/202506_HL_Maintain_Report.xlsx
@@ -11,16 +11,16 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Report'!$1:$2</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$135</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Report'!$A$1:$AK$144</definedName>
   </definedNames>
   <calcPr calcId="999999" calcMode="auto" calcCompleted="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="964">
-  <si>
-    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-27  )</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="1030">
+  <si>
+    <t>萊爾富 工作統計表  篩選月份：202506   (  製表日期:2025-06-30  )</t>
   </si>
   <si>
     <t>項次</t>
@@ -2981,6 +2981,208 @@
     <t>更換多卡機及變壓器
 換上8183002072
 換下8183001602</t>
+  </si>
+  <si>
+    <t>14406114062701</t>
+  </si>
+  <si>
+    <t>板橋稚暉店</t>
+  </si>
+  <si>
+    <t>2025-06-27 20:11:45</t>
+  </si>
+  <si>
+    <t>HL59</t>
+  </si>
+  <si>
+    <t>HL-LIFE-ET熱感機T70II</t>
+  </si>
+  <si>
+    <t>門市反應MMK四代機熱感機(T70II)無法列印小白單並顯示紅燈，確認紙卷厚度超過5公分，已嘗試重啟熱感機、重新安裝紙卷，客服協助遠端重啟MMK仍異常...需請台芝到店協助。</t>
+  </si>
+  <si>
+    <t>THILF04406</t>
+  </si>
+  <si>
+    <t>2025-06-27 20:14:27</t>
+  </si>
+  <si>
+    <t>2025-06-30 14:30:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 15:07:00</t>
+  </si>
+  <si>
+    <t>2025-07-01 00:14:00</t>
+  </si>
+  <si>
+    <t>更換T70
+換上：8138001696
+換下：8138002690</t>
+  </si>
+  <si>
+    <t>E2749114062901</t>
+  </si>
+  <si>
+    <t>淡水灰瑤子</t>
+  </si>
+  <si>
+    <t>2025-06-29 06:05:03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">門市反應mmk4代機跳電後無法連線，畫面出現網路設定介面視窗但重新設定後仍異常重開機也異常，ping60不通....須請台芝到店協助(跳電，無法連線)
+</t>
+  </si>
+  <si>
+    <t>THILF02749</t>
+  </si>
+  <si>
+    <t>2025-06-29 09:25:42</t>
+  </si>
+  <si>
+    <t>2025-06-30 13:09:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 13:39:00</t>
+  </si>
+  <si>
+    <t>2025-07-01 13:00:00</t>
+  </si>
+  <si>
+    <t>現場重新啟動後連線及設定皆正常</t>
+  </si>
+  <si>
+    <t>14539114062901</t>
+  </si>
+  <si>
+    <t>三重自信店</t>
+  </si>
+  <si>
+    <t>2025-06-29 12:25:34</t>
+  </si>
+  <si>
+    <t>門市反應MMK四代機無法連線畫面顯示乙太網路沒有有效的ip，PING60不通，門市嘗試重啟MMK後無跳出網路偵測介面.....請台芝到店協助</t>
+  </si>
+  <si>
+    <t>THILF04539</t>
+  </si>
+  <si>
+    <t>2025-06-29 12:26:32</t>
+  </si>
+  <si>
+    <t>2025-06-30 10:35:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 11:05:00</t>
+  </si>
+  <si>
+    <t>現場已可以正常使用,測試連線皆為正常</t>
+  </si>
+  <si>
+    <t>13399114063001</t>
+  </si>
+  <si>
+    <t>2025-06-30 10:15:41</t>
+  </si>
+  <si>
+    <t>當機/自動開關機</t>
+  </si>
+  <si>
+    <t>06/30 10:21 啟動緊急叫修:(SHUTTLE7S)-門市反應稍早主任告知要重啟數據機，門市重啟後sc離線，與門市確認sc有正常開機但連不上e網，ping1不通無法vnc，已請門市將1port重新拔插更換孔位至2、3port仍異常且與門市確認未亮燈....須請台芝到店協助</t>
+  </si>
+  <si>
+    <t>2025-06-30 10:22:07</t>
+  </si>
+  <si>
+    <t>2025-06-30 12:23:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 12:48:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 16:22:00</t>
+  </si>
+  <si>
+    <t>更換網路線
+測試功能正常</t>
+  </si>
+  <si>
+    <t>2025-06-30 13:56:58</t>
+  </si>
+  <si>
+    <t>2025-06-30 12:40:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 13:35:00</t>
+  </si>
+  <si>
+    <t>D161</t>
+  </si>
+  <si>
+    <t>北縣僑中三店</t>
+  </si>
+  <si>
+    <t>THILF0D161</t>
+  </si>
+  <si>
+    <t>2025-06-30 13:57:01</t>
+  </si>
+  <si>
+    <t>2025-06-30 13:15:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 13:55:00</t>
+  </si>
+  <si>
+    <t>北縣板龍店</t>
+  </si>
+  <si>
+    <t>THILF02403</t>
+  </si>
+  <si>
+    <t>2025-06-30 14:46:33</t>
+  </si>
+  <si>
+    <t>2025-06-30 14:15:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 14:45:00</t>
+  </si>
+  <si>
+    <t>北縣芝蘭店</t>
+  </si>
+  <si>
+    <t>新北市三芝區</t>
+  </si>
+  <si>
+    <t>THILF02237</t>
+  </si>
+  <si>
+    <t>2025-06-30 14:53:49</t>
+  </si>
+  <si>
+    <t>2025-06-30 14:00:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 14:53:00</t>
+  </si>
+  <si>
+    <t>L501</t>
+  </si>
+  <si>
+    <t>車麗屋板橋店</t>
+  </si>
+  <si>
+    <t>THILF0L501</t>
+  </si>
+  <si>
+    <t>2025-06-30 15:29:10</t>
+  </si>
+  <si>
+    <t>2025-06-30 15:12:00</t>
+  </si>
+  <si>
+    <t>2025-06-30 15:27:00</t>
   </si>
 </sst>
 </file>
@@ -3394,10 +3596,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AK135"/>
+  <dimension ref="A1:AK144"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0" showGridLines="true" showRowColHeaders="1">
-      <selection activeCell="A135" sqref="A135"/>
+      <selection activeCell="AC141" sqref="AC141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -14947,7 +15149,7 @@
       <c r="O135" s="8" t="s">
         <v>957</v>
       </c>
-      <c r="P135" s="8" t="s">
+      <c r="P135" s="9" t="s">
         <v>958</v>
       </c>
       <c r="Q135" s="7" t="s">
@@ -14984,7 +15186,7 @@
       <c r="AB135" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="AC135" s="8" t="s">
+      <c r="AC135" s="9" t="s">
         <v>963</v>
       </c>
       <c r="AD135" s="7"/>
@@ -14995,6 +15197,781 @@
       <c r="AI135" s="7"/>
       <c r="AJ135" s="7"/>
       <c r="AK135" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="136" spans="1:37">
+      <c r="A136" s="3">
+        <v>134</v>
+      </c>
+      <c r="B136" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C136" s="3">
+        <v>2025063571</v>
+      </c>
+      <c r="D136" s="3" t="s">
+        <v>964</v>
+      </c>
+      <c r="E136" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F136" s="3">
+        <v>4406</v>
+      </c>
+      <c r="G136" s="3" t="s">
+        <v>965</v>
+      </c>
+      <c r="H136" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I136" s="3" t="s">
+        <v>966</v>
+      </c>
+      <c r="J136" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="K136" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="L136" s="3" t="s">
+        <v>967</v>
+      </c>
+      <c r="M136" s="4" t="s">
+        <v>968</v>
+      </c>
+      <c r="N136" s="3">
+        <v>5903</v>
+      </c>
+      <c r="O136" s="4" t="s">
+        <v>535</v>
+      </c>
+      <c r="P136" s="10" t="s">
+        <v>969</v>
+      </c>
+      <c r="Q136" s="3" t="s">
+        <v>970</v>
+      </c>
+      <c r="R136" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S136" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T136" s="3">
+        <v>1</v>
+      </c>
+      <c r="U136" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V136" s="3" t="s">
+        <v>971</v>
+      </c>
+      <c r="W136" s="3" t="s">
+        <v>972</v>
+      </c>
+      <c r="X136" s="3" t="s">
+        <v>973</v>
+      </c>
+      <c r="Y136" s="3" t="s">
+        <v>974</v>
+      </c>
+      <c r="Z136" s="3">
+        <v>0.6</v>
+      </c>
+      <c r="AA136" s="3"/>
+      <c r="AB136" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC136" s="10" t="s">
+        <v>975</v>
+      </c>
+      <c r="AD136" s="3"/>
+      <c r="AE136" s="3"/>
+      <c r="AF136" s="3"/>
+      <c r="AG136" s="3"/>
+      <c r="AH136" s="3"/>
+      <c r="AI136" s="3"/>
+      <c r="AJ136" s="3"/>
+      <c r="AK136" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="137" spans="1:37">
+      <c r="A137" s="7">
+        <v>135</v>
+      </c>
+      <c r="B137" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C137" s="7">
+        <v>2025063586</v>
+      </c>
+      <c r="D137" s="7" t="s">
+        <v>976</v>
+      </c>
+      <c r="E137" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="F137" s="7">
+        <v>2749</v>
+      </c>
+      <c r="G137" s="7" t="s">
+        <v>977</v>
+      </c>
+      <c r="H137" s="7" t="s">
+        <v>163</v>
+      </c>
+      <c r="I137" s="7" t="s">
+        <v>978</v>
+      </c>
+      <c r="J137" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="K137" s="7" t="s">
+        <v>326</v>
+      </c>
+      <c r="L137" s="7" t="s">
+        <v>313</v>
+      </c>
+      <c r="M137" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="N137" s="7">
+        <v>5804</v>
+      </c>
+      <c r="O137" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="P137" s="9" t="s">
+        <v>979</v>
+      </c>
+      <c r="Q137" s="7" t="s">
+        <v>980</v>
+      </c>
+      <c r="R137" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S137" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T137" s="7">
+        <v>1</v>
+      </c>
+      <c r="U137" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V137" s="7" t="s">
+        <v>981</v>
+      </c>
+      <c r="W137" s="7" t="s">
+        <v>982</v>
+      </c>
+      <c r="X137" s="7" t="s">
+        <v>983</v>
+      </c>
+      <c r="Y137" s="7" t="s">
+        <v>984</v>
+      </c>
+      <c r="Z137" s="7">
+        <v>0.5</v>
+      </c>
+      <c r="AA137" s="7"/>
+      <c r="AB137" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC137" s="9" t="s">
+        <v>985</v>
+      </c>
+      <c r="AD137" s="7"/>
+      <c r="AE137" s="7"/>
+      <c r="AF137" s="7"/>
+      <c r="AG137" s="7"/>
+      <c r="AH137" s="7"/>
+      <c r="AI137" s="7"/>
+      <c r="AJ137" s="7"/>
+      <c r="AK137" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="138" spans="1:37">
+      <c r="A138" s="3">
+        <v>136</v>
+      </c>
+      <c r="B138" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C138" s="3">
+        <v>2025063589</v>
+      </c>
+      <c r="D138" s="3" t="s">
+        <v>986</v>
+      </c>
+      <c r="E138" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="F138" s="3">
+        <v>4539</v>
+      </c>
+      <c r="G138" s="3" t="s">
+        <v>987</v>
+      </c>
+      <c r="H138" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="I138" s="3" t="s">
+        <v>988</v>
+      </c>
+      <c r="J138" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="K138" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="L138" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="M138" s="4" t="s">
+        <v>314</v>
+      </c>
+      <c r="N138" s="3">
+        <v>5804</v>
+      </c>
+      <c r="O138" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="P138" s="10" t="s">
+        <v>989</v>
+      </c>
+      <c r="Q138" s="3" t="s">
+        <v>990</v>
+      </c>
+      <c r="R138" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S138" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T138" s="3">
+        <v>1</v>
+      </c>
+      <c r="U138" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V138" s="3" t="s">
+        <v>991</v>
+      </c>
+      <c r="W138" s="3" t="s">
+        <v>992</v>
+      </c>
+      <c r="X138" s="3" t="s">
+        <v>993</v>
+      </c>
+      <c r="Y138" s="3" t="s">
+        <v>984</v>
+      </c>
+      <c r="Z138" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA138" s="3"/>
+      <c r="AB138" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC138" s="10" t="s">
+        <v>994</v>
+      </c>
+      <c r="AD138" s="3"/>
+      <c r="AE138" s="3"/>
+      <c r="AF138" s="3"/>
+      <c r="AG138" s="3"/>
+      <c r="AH138" s="3"/>
+      <c r="AI138" s="3"/>
+      <c r="AJ138" s="3"/>
+      <c r="AK138" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="139" spans="1:37">
+      <c r="A139" s="7">
+        <v>137</v>
+      </c>
+      <c r="B139" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="C139" s="7">
+        <v>2025063598</v>
+      </c>
+      <c r="D139" s="7" t="s">
+        <v>995</v>
+      </c>
+      <c r="E139" s="7" t="s">
+        <v>221</v>
+      </c>
+      <c r="F139" s="7">
+        <v>3399</v>
+      </c>
+      <c r="G139" s="7" t="s">
+        <v>940</v>
+      </c>
+      <c r="H139" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I139" s="7" t="s">
+        <v>996</v>
+      </c>
+      <c r="J139" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="K139" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="L139" s="7" t="s">
+        <v>224</v>
+      </c>
+      <c r="M139" s="8" t="s">
+        <v>225</v>
+      </c>
+      <c r="N139" s="7">
+        <v>2401</v>
+      </c>
+      <c r="O139" s="8" t="s">
+        <v>997</v>
+      </c>
+      <c r="P139" s="9" t="s">
+        <v>998</v>
+      </c>
+      <c r="Q139" s="7" t="s">
+        <v>941</v>
+      </c>
+      <c r="R139" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S139" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T139" s="7">
+        <v>1</v>
+      </c>
+      <c r="U139" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V139" s="7" t="s">
+        <v>999</v>
+      </c>
+      <c r="W139" s="7" t="s">
+        <v>1000</v>
+      </c>
+      <c r="X139" s="7" t="s">
+        <v>1001</v>
+      </c>
+      <c r="Y139" s="7" t="s">
+        <v>1002</v>
+      </c>
+      <c r="Z139" s="7">
+        <v>0.4</v>
+      </c>
+      <c r="AA139" s="7"/>
+      <c r="AB139" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC139" s="9" t="s">
+        <v>1003</v>
+      </c>
+      <c r="AD139" s="7"/>
+      <c r="AE139" s="7"/>
+      <c r="AF139" s="7"/>
+      <c r="AG139" s="7"/>
+      <c r="AH139" s="7"/>
+      <c r="AI139" s="7"/>
+      <c r="AJ139" s="7"/>
+      <c r="AK139" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="140" spans="1:37">
+      <c r="A140" s="3">
+        <v>138</v>
+      </c>
+      <c r="B140" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C140" s="3">
+        <v>2025063630</v>
+      </c>
+      <c r="D140" s="3"/>
+      <c r="E140" s="3"/>
+      <c r="F140" s="3">
+        <v>2749</v>
+      </c>
+      <c r="G140" s="3" t="s">
+        <v>977</v>
+      </c>
+      <c r="H140" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="I140" s="3"/>
+      <c r="J140" s="3"/>
+      <c r="K140" s="3"/>
+      <c r="L140" s="3"/>
+      <c r="M140" s="4"/>
+      <c r="N140" s="3"/>
+      <c r="O140" s="4"/>
+      <c r="P140" s="10"/>
+      <c r="Q140" s="3" t="s">
+        <v>980</v>
+      </c>
+      <c r="R140" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S140" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="T140" s="3">
+        <v>1</v>
+      </c>
+      <c r="U140" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V140" s="3" t="s">
+        <v>1004</v>
+      </c>
+      <c r="W140" s="3" t="s">
+        <v>1005</v>
+      </c>
+      <c r="X140" s="3" t="s">
+        <v>1006</v>
+      </c>
+      <c r="Y140" s="3"/>
+      <c r="Z140" s="3">
+        <v>0.9</v>
+      </c>
+      <c r="AA140" s="3"/>
+      <c r="AB140" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC140" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="AD140" s="3"/>
+      <c r="AE140" s="3"/>
+      <c r="AF140" s="3"/>
+      <c r="AG140" s="3"/>
+      <c r="AH140" s="3"/>
+      <c r="AI140" s="3"/>
+      <c r="AJ140" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK140" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="141" spans="1:37">
+      <c r="A141" s="7">
+        <v>139</v>
+      </c>
+      <c r="B141" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C141" s="7">
+        <v>2025063631</v>
+      </c>
+      <c r="D141" s="7"/>
+      <c r="E141" s="7"/>
+      <c r="F141" s="7" t="s">
+        <v>1007</v>
+      </c>
+      <c r="G141" s="7" t="s">
+        <v>1008</v>
+      </c>
+      <c r="H141" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="I141" s="7"/>
+      <c r="J141" s="7"/>
+      <c r="K141" s="7"/>
+      <c r="L141" s="7"/>
+      <c r="M141" s="8"/>
+      <c r="N141" s="7"/>
+      <c r="O141" s="8"/>
+      <c r="P141" s="9"/>
+      <c r="Q141" s="7" t="s">
+        <v>1009</v>
+      </c>
+      <c r="R141" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S141" s="7" t="s">
+        <v>125</v>
+      </c>
+      <c r="T141" s="7">
+        <v>1</v>
+      </c>
+      <c r="U141" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V141" s="7" t="s">
+        <v>1010</v>
+      </c>
+      <c r="W141" s="7" t="s">
+        <v>1011</v>
+      </c>
+      <c r="X141" s="7" t="s">
+        <v>1012</v>
+      </c>
+      <c r="Y141" s="7"/>
+      <c r="Z141" s="7">
+        <v>0.7</v>
+      </c>
+      <c r="AA141" s="7"/>
+      <c r="AB141" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC141" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="AD141" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE141" s="7"/>
+      <c r="AF141" s="7"/>
+      <c r="AG141" s="7"/>
+      <c r="AH141" s="7"/>
+      <c r="AI141" s="7"/>
+      <c r="AJ141" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK141" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="142" spans="1:37">
+      <c r="A142" s="3">
+        <v>140</v>
+      </c>
+      <c r="B142" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C142" s="3">
+        <v>2025063693</v>
+      </c>
+      <c r="D142" s="3"/>
+      <c r="E142" s="3"/>
+      <c r="F142" s="3">
+        <v>2403</v>
+      </c>
+      <c r="G142" s="3" t="s">
+        <v>1013</v>
+      </c>
+      <c r="H142" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I142" s="3"/>
+      <c r="J142" s="3"/>
+      <c r="K142" s="3"/>
+      <c r="L142" s="3"/>
+      <c r="M142" s="4"/>
+      <c r="N142" s="3"/>
+      <c r="O142" s="4"/>
+      <c r="P142" s="10"/>
+      <c r="Q142" s="3" t="s">
+        <v>1014</v>
+      </c>
+      <c r="R142" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S142" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T142" s="3">
+        <v>1</v>
+      </c>
+      <c r="U142" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V142" s="3" t="s">
+        <v>1015</v>
+      </c>
+      <c r="W142" s="3" t="s">
+        <v>1016</v>
+      </c>
+      <c r="X142" s="3" t="s">
+        <v>1017</v>
+      </c>
+      <c r="Y142" s="3"/>
+      <c r="Z142" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="AA142" s="3"/>
+      <c r="AB142" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC142" s="10" t="s">
+        <v>421</v>
+      </c>
+      <c r="AD142" s="3"/>
+      <c r="AE142" s="3"/>
+      <c r="AF142" s="3"/>
+      <c r="AG142" s="3"/>
+      <c r="AH142" s="3"/>
+      <c r="AI142" s="3"/>
+      <c r="AJ142" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK142" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="143" spans="1:37">
+      <c r="A143" s="7">
+        <v>141</v>
+      </c>
+      <c r="B143" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="C143" s="7">
+        <v>2025063697</v>
+      </c>
+      <c r="D143" s="7"/>
+      <c r="E143" s="7"/>
+      <c r="F143" s="7">
+        <v>2237</v>
+      </c>
+      <c r="G143" s="7" t="s">
+        <v>1018</v>
+      </c>
+      <c r="H143" s="7" t="s">
+        <v>1019</v>
+      </c>
+      <c r="I143" s="7"/>
+      <c r="J143" s="7"/>
+      <c r="K143" s="7"/>
+      <c r="L143" s="7"/>
+      <c r="M143" s="8"/>
+      <c r="N143" s="7"/>
+      <c r="O143" s="8"/>
+      <c r="P143" s="9"/>
+      <c r="Q143" s="7" t="s">
+        <v>1020</v>
+      </c>
+      <c r="R143" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="S143" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="T143" s="7">
+        <v>1</v>
+      </c>
+      <c r="U143" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="V143" s="7" t="s">
+        <v>1021</v>
+      </c>
+      <c r="W143" s="7" t="s">
+        <v>1022</v>
+      </c>
+      <c r="X143" s="7" t="s">
+        <v>1023</v>
+      </c>
+      <c r="Y143" s="7"/>
+      <c r="Z143" s="7">
+        <v>0.9</v>
+      </c>
+      <c r="AA143" s="7"/>
+      <c r="AB143" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC143" s="9" t="s">
+        <v>366</v>
+      </c>
+      <c r="AD143" s="7"/>
+      <c r="AE143" s="7"/>
+      <c r="AF143" s="7"/>
+      <c r="AG143" s="7"/>
+      <c r="AH143" s="7"/>
+      <c r="AI143" s="7"/>
+      <c r="AJ143" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="AK143" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="144" spans="1:37">
+      <c r="A144" s="3">
+        <v>142</v>
+      </c>
+      <c r="B144" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C144" s="3">
+        <v>2025063701</v>
+      </c>
+      <c r="D144" s="3"/>
+      <c r="E144" s="3"/>
+      <c r="F144" s="3" t="s">
+        <v>1024</v>
+      </c>
+      <c r="G144" s="3" t="s">
+        <v>1025</v>
+      </c>
+      <c r="H144" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I144" s="3"/>
+      <c r="J144" s="3"/>
+      <c r="K144" s="3"/>
+      <c r="L144" s="3"/>
+      <c r="M144" s="4"/>
+      <c r="N144" s="3"/>
+      <c r="O144" s="4"/>
+      <c r="P144" s="4"/>
+      <c r="Q144" s="3" t="s">
+        <v>1026</v>
+      </c>
+      <c r="R144" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="S144" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="T144" s="3">
+        <v>1</v>
+      </c>
+      <c r="U144" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="V144" s="3" t="s">
+        <v>1027</v>
+      </c>
+      <c r="W144" s="3" t="s">
+        <v>1028</v>
+      </c>
+      <c r="X144" s="3" t="s">
+        <v>1029</v>
+      </c>
+      <c r="Y144" s="3"/>
+      <c r="Z144" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="AA144" s="3"/>
+      <c r="AB144" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AC144" s="4" t="s">
+        <v>214</v>
+      </c>
+      <c r="AD144" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AE144" s="3"/>
+      <c r="AF144" s="3"/>
+      <c r="AG144" s="3"/>
+      <c r="AH144" s="3"/>
+      <c r="AI144" s="3"/>
+      <c r="AJ144" s="3"/>
+      <c r="AK144" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>